<commit_message>
add .gitignore for csv and remove old files
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Backtesting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Trade History" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
   <si>
     <t>Position</t>
   </si>
@@ -102,13 +97,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +113,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -170,11 +158,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -182,28 +169,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -250,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,10 +254,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,7 +288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,31 +463,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="7" customWidth="1"/>
-    <col min="6" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="10" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="11" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,7 +488,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -539,13 +500,13 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -564,7 +525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -572,34 +533,34 @@
         <v>15</v>
       </c>
       <c r="C2" s="4">
-        <v>45666.635416666657</v>
+        <v>45666.63541666666</v>
       </c>
       <c r="D2" s="4">
-        <v>45666.645833333343</v>
-      </c>
-      <c r="E2" s="7">
+        <v>45666.64583333334</v>
+      </c>
+      <c r="E2">
         <v>93188.2</v>
       </c>
       <c r="F2" s="1">
-        <v>93801.349971594973</v>
+        <v>93801.34997159497</v>
       </c>
       <c r="G2" s="1">
-        <v>91348.750085215084</v>
+        <v>91348.75008521508</v>
       </c>
       <c r="H2" s="1">
         <v>93452</v>
       </c>
-      <c r="I2" s="9">
-        <v>0.16309223621077859</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="11">
-        <v>-43.023731912403868</v>
+      <c r="I2" s="1">
+        <v>0.1630922362107786</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <v>-43.02373191240387</v>
       </c>
       <c r="L2" s="1">
-        <v>9956.9762680875956</v>
+        <v>9956.976268087596</v>
       </c>
       <c r="M2" s="1">
         <v>100</v>
@@ -611,10 +572,10 @@
         <v>613.1499715949758</v>
       </c>
       <c r="P2">
-        <v>1839.4499147849131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1839.449914784913</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -622,49 +583,49 @@
         <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>45666.649305555547</v>
+        <v>45666.64930555555</v>
       </c>
       <c r="D3" s="4">
-        <v>45666.659722222219</v>
-      </c>
-      <c r="E3" s="7">
+        <v>45666.65972222222</v>
+      </c>
+      <c r="E3">
         <v>93739.87</v>
       </c>
       <c r="F3" s="1">
         <v>94376.30887387348</v>
       </c>
       <c r="G3" s="1">
-        <v>91830.553378379525</v>
+        <v>91830.55337837953</v>
       </c>
       <c r="H3" s="1">
-        <v>94100.49</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.15644827298947961</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="11">
-        <v>-56.418376205467673</v>
+        <v>94100.49000000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.1564482729894796</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>-56.41837620546767</v>
       </c>
       <c r="L3" s="1">
-        <v>9900.5578918821284</v>
+        <v>9900.557891882128</v>
       </c>
       <c r="M3" s="1">
-        <v>99.569762680875954</v>
+        <v>99.56976268087595</v>
       </c>
       <c r="N3" t="s">
         <v>19</v>
       </c>
       <c r="O3">
-        <v>636.43887387348514</v>
+        <v>636.4388738734851</v>
       </c>
       <c r="P3">
         <v>1909.31662162047</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -672,49 +633,49 @@
         <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>45666.663194444453</v>
+        <v>45666.66319444445</v>
       </c>
       <c r="D4" s="4">
-        <v>45666.822916666657</v>
-      </c>
-      <c r="E4" s="7">
+        <v>45666.82291666666</v>
+      </c>
+      <c r="E4">
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
-        <v>94919.843700976169</v>
+        <v>94919.84370097617</v>
       </c>
       <c r="G4" s="1">
-        <v>92216.548897071494</v>
+        <v>92216.54889707149</v>
       </c>
       <c r="H4" s="1">
-        <v>92106.85</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0.14649616279484851</v>
-      </c>
-      <c r="J4" s="10" t="s">
+        <v>92106.85000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.1464961627948485</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="11">
-        <v>313.08720424026609</v>
+      <c r="K4">
+        <v>313.0872042402661</v>
       </c>
       <c r="L4" s="1">
-        <v>10213.645096122391</v>
+        <v>10213.64509612239</v>
       </c>
       <c r="M4" s="1">
-        <v>99.005578918821286</v>
+        <v>99.00557891882129</v>
       </c>
       <c r="N4" t="s">
         <v>19</v>
       </c>
       <c r="O4">
-        <v>675.82370097616513</v>
+        <v>675.8237009761651</v>
       </c>
       <c r="P4">
-        <v>2027.4711029285099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2027.47110292851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -725,31 +686,31 @@
         <v>45667.75</v>
       </c>
       <c r="D5" s="4">
-        <v>45670.541666666657</v>
-      </c>
-      <c r="E5" s="7">
+        <v>45670.54166666666</v>
+      </c>
+      <c r="E5">
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
-        <v>96318.698924743541</v>
+        <v>96318.69892474354</v>
       </c>
       <c r="G5" s="1">
         <v>92990.82322576936</v>
       </c>
       <c r="H5" s="1">
-        <v>90583.24</v>
-      </c>
-      <c r="I5" s="9">
+        <v>90583.24000000001</v>
+      </c>
+      <c r="I5" s="1">
         <v>0.1227647426767863</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="11">
-        <v>601.97568806819379</v>
+      <c r="K5">
+        <v>601.9756880681938</v>
       </c>
       <c r="L5" s="1">
-        <v>10815.620784190591</v>
+        <v>10815.62078419059</v>
       </c>
       <c r="M5" s="1">
         <v>102.1364509612239</v>
@@ -758,13 +719,13 @@
         <v>19</v>
       </c>
       <c r="O5">
-        <v>831.96892474354536</v>
+        <v>831.9689247435454</v>
       </c>
       <c r="P5">
-        <v>2495.9067742306361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2495.906774230636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -772,31 +733,31 @@
         <v>15</v>
       </c>
       <c r="C6" s="4">
-        <v>45670.635416666657</v>
+        <v>45670.63541666666</v>
       </c>
       <c r="D6" s="4">
-        <v>45670.868055555547</v>
-      </c>
-      <c r="E6" s="7">
-        <v>92680.01</v>
+        <v>45670.86805555555</v>
+      </c>
+      <c r="E6">
+        <v>92680.00999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>93739.195790475918</v>
+        <v>93739.19579047592</v>
       </c>
       <c r="G6" s="1">
-        <v>89502.452628572224</v>
+        <v>89502.45262857222</v>
       </c>
       <c r="H6" s="1">
-        <v>93228.99</v>
-      </c>
-      <c r="I6" s="9">
-        <v>0.10211259329046329</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="11">
-        <v>-56.057771464599632</v>
+        <v>93228.99000000001</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.1021125932904633</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>-56.05777146459963</v>
       </c>
       <c r="L6" s="1">
         <v>10759.56301272599</v>
@@ -811,10 +772,10 @@
         <v>1059.185790475924</v>
       </c>
       <c r="P6">
-        <v>3177.5573714277712</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3177.557371427771</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -825,46 +786,46 @@
         <v>45673.625</v>
       </c>
       <c r="D7" s="4">
-        <v>45673.670138888891</v>
-      </c>
-      <c r="E7" s="7">
+        <v>45673.67013888889</v>
+      </c>
+      <c r="E7">
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
-        <v>96887.646241804439</v>
+        <v>96887.64624180444</v>
       </c>
       <c r="G7" s="1">
-        <v>99621.981274586666</v>
+        <v>99621.98127458667</v>
       </c>
       <c r="H7" s="1">
         <v>99815.27</v>
       </c>
-      <c r="I7" s="9">
-        <v>0.15739933671226791</v>
-      </c>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="1">
+        <v>0.1573993367122679</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="11">
-        <v>353.21040755579878</v>
+      <c r="K7">
+        <v>353.2104075557988</v>
       </c>
       <c r="L7" s="1">
         <v>11112.77342028179</v>
       </c>
       <c r="M7" s="1">
-        <v>107.59563012725989</v>
+        <v>107.5956301272599</v>
       </c>
       <c r="N7" t="s">
         <v>19</v>
       </c>
       <c r="O7">
-        <v>683.58375819555658</v>
+        <v>683.5837581955566</v>
       </c>
       <c r="P7">
-        <v>2050.7512745866702</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2050.75127458667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -872,31 +833,31 @@
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>45674.871527777781</v>
+        <v>45674.87152777778</v>
       </c>
       <c r="D8" s="4">
-        <v>45675.541666666657</v>
-      </c>
-      <c r="E8" s="7">
+        <v>45675.54166666666</v>
+      </c>
+      <c r="E8">
         <v>104692.7</v>
       </c>
       <c r="F8" s="1">
         <v>104197.1529992671</v>
       </c>
       <c r="G8" s="1">
-        <v>106179.34100219861</v>
+        <v>106179.3410021986</v>
       </c>
       <c r="H8" s="1">
         <v>103424.59</v>
       </c>
-      <c r="I8" s="9">
-        <v>0.22425266228726379</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="11">
-        <v>-284.37704357310218</v>
+      <c r="I8" s="1">
+        <v>0.2242526622872638</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8">
+        <v>-284.3770435731022</v>
       </c>
       <c r="L8" s="1">
         <v>10828.39637670869</v>
@@ -908,13 +869,13 @@
         <v>19</v>
       </c>
       <c r="O8">
-        <v>495.54700073288399</v>
+        <v>495.547000732884</v>
       </c>
       <c r="P8">
         <v>1486.641002198638</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -922,34 +883,34 @@
         <v>16</v>
       </c>
       <c r="C9" s="4">
-        <v>45675.701388888891</v>
+        <v>45675.70138888889</v>
       </c>
       <c r="D9" s="4">
-        <v>45676.541666666657</v>
-      </c>
-      <c r="E9" s="7">
+        <v>45676.54166666666</v>
+      </c>
+      <c r="E9">
         <v>103240.85</v>
       </c>
       <c r="F9" s="1">
         <v>102688.8552242209</v>
       </c>
       <c r="G9" s="1">
-        <v>104896.83432733751</v>
+        <v>104896.8343273375</v>
       </c>
       <c r="H9" s="1">
         <v>105157.8</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="1">
         <v>0.1961684575986099</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="11">
-        <v>376.04512479365468</v>
+      <c r="K9">
+        <v>376.0451247936547</v>
       </c>
       <c r="L9" s="1">
-        <v>11204.441501502341</v>
+        <v>11204.44150150234</v>
       </c>
       <c r="M9" s="1">
         <v>108.2839637670869</v>
@@ -958,13 +919,13 @@
         <v>19</v>
       </c>
       <c r="O9">
-        <v>551.99477577915241</v>
+        <v>551.9947757791524</v>
       </c>
       <c r="P9">
         <v>1655.984327337472</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -972,30 +933,30 @@
         <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>45677.659722222219</v>
+        <v>45677.65972222222</v>
       </c>
       <c r="D10" s="4">
-        <v>45677.673611111109</v>
-      </c>
-      <c r="E10" s="7">
+        <v>45677.67361111111</v>
+      </c>
+      <c r="E10">
         <v>105535.7</v>
       </c>
       <c r="F10" s="1">
         <v>104427.1512541753</v>
       </c>
       <c r="G10" s="1">
-        <v>108861.34623747411</v>
+        <v>108861.3462374741</v>
       </c>
       <c r="H10" s="1">
         <v>103708</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="1">
         <v>0.1010730610061438</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10">
         <v>-184.7312336009287</v>
       </c>
       <c r="L10" s="1">
@@ -1014,7 +975,7 @@
         <v>3325.64623747408</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1022,12 +983,12 @@
         <v>16</v>
       </c>
       <c r="C11" s="4">
-        <v>45678.628472222219</v>
+        <v>45678.62847222222</v>
       </c>
       <c r="D11" s="4">
-        <v>45678.673611111109</v>
-      </c>
-      <c r="E11" s="7">
+        <v>45678.67361111111</v>
+      </c>
+      <c r="E11">
         <v>103281.22</v>
       </c>
       <c r="F11" s="1">
@@ -1039,32 +1000,32 @@
       <c r="H11" s="1">
         <v>106300</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="1">
         <v>0.1152930814464031</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="11">
-        <v>348.04444840877261</v>
+      <c r="K11">
+        <v>348.0444484087726</v>
       </c>
       <c r="L11" s="1">
-        <v>11367.754716310181</v>
+        <v>11367.75471631018</v>
       </c>
       <c r="M11" s="1">
-        <v>110.19710267901409</v>
+        <v>110.1971026790141</v>
       </c>
       <c r="N11" t="s">
         <v>19</v>
       </c>
       <c r="O11">
-        <v>955.79978691299038</v>
+        <v>955.7997869129904</v>
       </c>
       <c r="P11">
-        <v>2867.3993607389862</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2867.399360738986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1072,16 +1033,16 @@
         <v>16</v>
       </c>
       <c r="C12" s="4">
-        <v>45678.861111111109</v>
+        <v>45678.86111111111</v>
       </c>
       <c r="D12" s="4">
-        <v>45679.541666666657</v>
-      </c>
-      <c r="E12" s="7">
+        <v>45679.54166666666</v>
+      </c>
+      <c r="E12">
         <v>106072</v>
       </c>
       <c r="F12" s="1">
-        <v>105391.07836610261</v>
+        <v>105391.0783661026</v>
       </c>
       <c r="G12" s="1">
         <v>108114.7649016923</v>
@@ -1089,20 +1050,20 @@
       <c r="H12" s="1">
         <v>105039.74</v>
       </c>
-      <c r="I12" s="9">
-        <v>0.16694659341698481</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="11">
+      <c r="I12" s="1">
+        <v>0.1669465934169848</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12">
         <v>-172.3322905206158</v>
       </c>
       <c r="L12" s="1">
-        <v>11195.422425789569</v>
+        <v>11195.42242578957</v>
       </c>
       <c r="M12" s="1">
-        <v>113.67754716310181</v>
+        <v>113.6775471631018</v>
       </c>
       <c r="N12" t="s">
         <v>19</v>
@@ -1114,7 +1075,7 @@
         <v>2042.764901692251</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1122,16 +1083,16 @@
         <v>16</v>
       </c>
       <c r="C13" s="4">
-        <v>45679.548611111109</v>
+        <v>45679.54861111111</v>
       </c>
       <c r="D13" s="4">
-        <v>45679.565972222219</v>
-      </c>
-      <c r="E13" s="7">
+        <v>45679.56597222222</v>
+      </c>
+      <c r="E13">
         <v>104947.17</v>
       </c>
       <c r="F13" s="1">
-        <v>104638.47922487849</v>
+        <v>104638.4792248785</v>
       </c>
       <c r="G13" s="1">
         <v>105873.2423253646</v>
@@ -1139,17 +1100,17 @@
       <c r="H13" s="1">
         <v>104283.67</v>
       </c>
-      <c r="I13" s="9">
-        <v>0.36267434364960688</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="11">
-        <v>-240.63442701151419</v>
+      <c r="I13" s="1">
+        <v>0.3626743436496069</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13">
+        <v>-240.6344270115142</v>
       </c>
       <c r="L13" s="1">
-        <v>10954.787998778051</v>
+        <v>10954.78799877805</v>
       </c>
       <c r="M13" s="1">
         <v>111.9542242578957</v>
@@ -1158,13 +1119,13 @@
         <v>19</v>
       </c>
       <c r="O13">
-        <v>308.69077512154757</v>
+        <v>308.6907751215476</v>
       </c>
       <c r="P13">
-        <v>926.07232536464289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>926.0723253646429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1172,16 +1133,16 @@
         <v>16</v>
       </c>
       <c r="C14" s="4">
-        <v>45679.579861111109</v>
+        <v>45679.57986111111</v>
       </c>
       <c r="D14" s="4">
-        <v>45679.694444444453</v>
-      </c>
-      <c r="E14" s="7">
+        <v>45679.69444444445</v>
+      </c>
+      <c r="E14">
         <v>104073.94</v>
       </c>
       <c r="F14" s="1">
-        <v>103607.83220123249</v>
+        <v>103607.8322012325</v>
       </c>
       <c r="G14" s="1">
         <v>105472.2633963026</v>
@@ -1189,17 +1150,17 @@
       <c r="H14" s="1">
         <v>103339.12</v>
       </c>
-      <c r="I14" s="9">
-        <v>0.23502691926082819</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="11">
-        <v>-172.70248081124339</v>
+      <c r="I14" s="1">
+        <v>0.2350269192608282</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14">
+        <v>-172.7024808112434</v>
       </c>
       <c r="L14" s="1">
-        <v>10782.085517966811</v>
+        <v>10782.08551796681</v>
       </c>
       <c r="M14" s="1">
         <v>109.5478799877805</v>
@@ -1208,13 +1169,13 @@
         <v>19</v>
       </c>
       <c r="O14">
-        <v>466.10779876753799</v>
+        <v>466.107798767538</v>
       </c>
       <c r="P14">
-        <v>1398.3233963026139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1398.323396302614</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1222,12 +1183,12 @@
         <v>16</v>
       </c>
       <c r="C15" s="4">
-        <v>45679.881944444453</v>
+        <v>45679.88194444445</v>
       </c>
       <c r="D15" s="4">
-        <v>45680.541666666657</v>
-      </c>
-      <c r="E15" s="7">
+        <v>45680.54166666666</v>
+      </c>
+      <c r="E15">
         <v>103891.76</v>
       </c>
       <c r="F15" s="1">
@@ -1239,14 +1200,14 @@
       <c r="H15" s="1">
         <v>101592.48</v>
       </c>
-      <c r="I15" s="9">
-        <v>0.21213591568689311</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="11">
-        <v>-487.75986822055938</v>
+      <c r="I15" s="1">
+        <v>0.2121359156868931</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>-487.7598682205594</v>
       </c>
       <c r="L15" s="1">
         <v>10294.32564974625</v>
@@ -1258,13 +1219,13 @@
         <v>19</v>
       </c>
       <c r="O15">
-        <v>508.26308609999251</v>
+        <v>508.2630860999925</v>
       </c>
       <c r="P15">
         <v>1524.789258299978</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1272,12 +1233,12 @@
         <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>45680.829861111109</v>
+        <v>45680.82986111111</v>
       </c>
       <c r="D16" s="4">
-        <v>45680.850694444453</v>
-      </c>
-      <c r="E16" s="7">
+        <v>45680.85069444445</v>
+      </c>
+      <c r="E16">
         <v>103770.04</v>
       </c>
       <c r="F16" s="1">
@@ -1289,17 +1250,17 @@
       <c r="H16" s="1">
         <v>106421.03</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="1">
         <v>0.1191027928070732</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16">
         <v>315.7403127036236</v>
       </c>
       <c r="L16" s="1">
-        <v>10610.065962449869</v>
+        <v>10610.06596244987</v>
       </c>
       <c r="M16" s="1">
         <v>102.9432564974625</v>
@@ -1308,13 +1269,13 @@
         <v>19</v>
       </c>
       <c r="O16">
-        <v>864.32277590848389</v>
+        <v>864.3227759084839</v>
       </c>
       <c r="P16">
-        <v>2592.9683277254521</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2592.968327725452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1322,12 +1283,12 @@
         <v>16</v>
       </c>
       <c r="C17" s="4">
-        <v>45681.829861111109</v>
+        <v>45681.82986111111</v>
       </c>
       <c r="D17" s="4">
-        <v>45681.847222222219</v>
-      </c>
-      <c r="E17" s="7">
+        <v>45681.84722222222</v>
+      </c>
+      <c r="E17">
         <v>105760.94</v>
       </c>
       <c r="F17" s="1">
@@ -1339,17 +1300,17 @@
       <c r="H17" s="1">
         <v>105291.54</v>
       </c>
-      <c r="I17" s="9">
-        <v>0.22742242852035471</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="11">
+      <c r="I17" s="1">
+        <v>0.2274224285203547</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17">
         <v>-106.7520879474565</v>
       </c>
       <c r="L17" s="1">
-        <v>10503.313874502421</v>
+        <v>10503.31387450242</v>
       </c>
       <c r="M17" s="1">
         <v>106.1006596244987</v>
@@ -1358,13 +1319,13 @@
         <v>19</v>
       </c>
       <c r="O17">
-        <v>466.53560211631702</v>
+        <v>466.535602116317</v>
       </c>
       <c r="P17">
-        <v>1399.6068063489511</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1399.606806348951</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1372,34 +1333,34 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <v>45681.857638888891</v>
+        <v>45681.85763888889</v>
       </c>
       <c r="D18" s="4">
-        <v>45682.586805555547</v>
-      </c>
-      <c r="E18" s="7">
+        <v>45682.58680555555</v>
+      </c>
+      <c r="E18">
         <v>105052.52</v>
       </c>
       <c r="F18" s="1">
         <v>104590.815085935</v>
       </c>
       <c r="G18" s="1">
-        <v>106437.63474219519</v>
+        <v>106437.6347421952</v>
       </c>
       <c r="H18" s="1">
         <v>104541.68</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="1">
         <v>0.2274897570837339</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="11">
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18">
         <v>-116.2108675086571</v>
       </c>
       <c r="L18" s="1">
-        <v>10387.103006993761</v>
+        <v>10387.10300699376</v>
       </c>
       <c r="M18" s="1">
         <v>105.0331387450242</v>
@@ -1411,10 +1372,10 @@
         <v>461.7049140650488</v>
       </c>
       <c r="P18">
-        <v>1385.1147421951609</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1385.114742195161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1422,31 +1383,31 @@
         <v>16</v>
       </c>
       <c r="C19" s="4">
-        <v>45683.885416666657</v>
+        <v>45683.88541666666</v>
       </c>
       <c r="D19" s="4">
         <v>45683.90625</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19">
         <v>104795.54</v>
       </c>
       <c r="F19" s="1">
         <v>104635.5126717815</v>
       </c>
       <c r="G19" s="1">
-        <v>105275.62198465561</v>
+        <v>105275.6219846556</v>
       </c>
       <c r="H19" s="1">
         <v>104552.48</v>
       </c>
-      <c r="I19" s="9">
-        <v>0.64908307366157403</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="11">
-        <v>-157.76613188418071</v>
+      <c r="I19" s="1">
+        <v>0.649083073661574</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19">
+        <v>-157.7661318841807</v>
       </c>
       <c r="L19" s="1">
         <v>10229.33687510958</v>
@@ -1458,13 +1419,13 @@
         <v>19</v>
       </c>
       <c r="O19">
-        <v>160.02732821853709</v>
+        <v>160.0273282185371</v>
       </c>
       <c r="P19">
         <v>480.0819846555969</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1472,34 +1433,34 @@
         <v>15</v>
       </c>
       <c r="C20" s="4">
-        <v>45684.541666666657</v>
+        <v>45684.54166666666</v>
       </c>
       <c r="D20" s="4">
-        <v>45684.545138888891</v>
-      </c>
-      <c r="E20" s="7">
+        <v>45684.54513888889</v>
+      </c>
+      <c r="E20">
         <v>100632.01</v>
       </c>
       <c r="F20" s="1">
         <v>101286.0915115136</v>
       </c>
       <c r="G20" s="1">
-        <v>98669.765465459277</v>
+        <v>98669.76546545928</v>
       </c>
       <c r="H20" s="1">
         <v>100622.87</v>
       </c>
-      <c r="I20" s="9">
-        <v>0.15639238680571149</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="11">
-        <v>1.4294264154041121</v>
+      <c r="I20" s="1">
+        <v>0.1563923868057115</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20">
+        <v>1.429426415404112</v>
       </c>
       <c r="L20" s="1">
-        <v>10230.766301524989</v>
+        <v>10230.76630152499</v>
       </c>
       <c r="M20" s="1">
         <v>102.2933687510958</v>
@@ -1508,13 +1469,13 @@
         <v>19</v>
       </c>
       <c r="O20">
-        <v>654.08151151357742</v>
+        <v>654.0815115135774</v>
       </c>
       <c r="P20">
         <v>1962.244534540718</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1522,34 +1483,34 @@
         <v>15</v>
       </c>
       <c r="C21" s="4">
-        <v>45684.850694444453</v>
+        <v>45684.85069444445</v>
       </c>
       <c r="D21" s="4">
-        <v>45684.864583333343</v>
-      </c>
-      <c r="E21" s="7">
-        <v>100351.67999999999</v>
+        <v>45684.86458333334</v>
+      </c>
+      <c r="E21">
+        <v>100351.68</v>
       </c>
       <c r="F21" s="1">
         <v>100958.2739530618</v>
       </c>
       <c r="G21" s="1">
-        <v>98531.898140814548</v>
+        <v>98531.89814081455</v>
       </c>
       <c r="H21" s="1">
         <v>100932.23</v>
       </c>
-      <c r="I21" s="9">
-        <v>0.16865922005790809</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="11">
-        <v>-97.915110204619054</v>
+      <c r="I21" s="1">
+        <v>0.1686592200579081</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21">
+        <v>-97.91511020461905</v>
       </c>
       <c r="L21" s="1">
-        <v>10132.851191320369</v>
+        <v>10132.85119132037</v>
       </c>
       <c r="M21" s="1">
         <v>102.3076630152499</v>
@@ -1558,13 +1519,13 @@
         <v>19</v>
       </c>
       <c r="O21">
-        <v>606.59395306181978</v>
+        <v>606.5939530618198</v>
       </c>
       <c r="P21">
         <v>1819.781859185445</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1572,34 +1533,34 @@
         <v>15</v>
       </c>
       <c r="C22" s="4">
-        <v>45684.871527777781</v>
+        <v>45684.87152777778</v>
       </c>
       <c r="D22" s="4">
-        <v>45684.878472222219</v>
-      </c>
-      <c r="E22" s="7">
+        <v>45684.87847222222</v>
+      </c>
+      <c r="E22">
         <v>101386.5</v>
       </c>
       <c r="F22" s="1">
         <v>102047.4840323447</v>
       </c>
       <c r="G22" s="1">
-        <v>99403.547902965991</v>
+        <v>99403.54790296599</v>
       </c>
       <c r="H22" s="1">
         <v>101604</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="1">
         <v>0.1532994852443969</v>
       </c>
-      <c r="J22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="11">
-        <v>-33.342638040656333</v>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22">
+        <v>-33.34263804065633</v>
       </c>
       <c r="L22" s="1">
-        <v>10099.508553279709</v>
+        <v>10099.50855327971</v>
       </c>
       <c r="M22" s="1">
         <v>101.3285119132037</v>
@@ -1608,13 +1569,13 @@
         <v>19</v>
       </c>
       <c r="O22">
-        <v>660.98403234466969</v>
+        <v>660.9840323446697</v>
       </c>
       <c r="P22">
-        <v>1982.9520970340091</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1982.952097034009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1622,12 +1583,12 @@
         <v>15</v>
       </c>
       <c r="C23" s="4">
-        <v>45684.881944444453</v>
+        <v>45684.88194444445</v>
       </c>
       <c r="D23" s="4">
         <v>45685.625</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23">
         <v>102295.12</v>
       </c>
       <c r="F23" s="1">
@@ -1639,32 +1600,32 @@
       <c r="H23" s="1">
         <v>102625.01</v>
       </c>
-      <c r="I23" s="9">
-        <v>0.14147039296331701</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="11">
+      <c r="I23" s="1">
+        <v>0.141470392963317</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23">
         <v>-46.66966793466856</v>
       </c>
       <c r="L23" s="1">
         <v>10052.83888534504</v>
       </c>
       <c r="M23" s="1">
-        <v>100.99508553279711</v>
+        <v>100.9950855327971</v>
       </c>
       <c r="N23" t="s">
         <v>19</v>
       </c>
       <c r="O23">
-        <v>713.89556088237441</v>
+        <v>713.8955608823744</v>
       </c>
       <c r="P23">
-        <v>2141.6866826471228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2141.686682647123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1672,16 +1633,16 @@
         <v>16</v>
       </c>
       <c r="C24" s="4">
-        <v>45687.736111111109</v>
+        <v>45687.73611111111</v>
       </c>
       <c r="D24" s="4">
-        <v>45688.565972222219</v>
-      </c>
-      <c r="E24" s="7">
+        <v>45688.56597222222</v>
+      </c>
+      <c r="E24">
         <v>105018.14</v>
       </c>
       <c r="F24" s="1">
-        <v>104555.74558261409</v>
+        <v>104555.7455826141</v>
       </c>
       <c r="G24" s="1">
         <v>106405.3232521578</v>
@@ -1689,32 +1650,32 @@
       <c r="H24" s="1">
         <v>104551.09</v>
       </c>
-      <c r="I24" s="9">
-        <v>0.21740831003491171</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="11">
+      <c r="I24" s="1">
+        <v>0.2174083100349117</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24">
         <v>-101.5405512018061</v>
       </c>
       <c r="L24" s="1">
-        <v>9951.2983341432355</v>
+        <v>9951.298334143235</v>
       </c>
       <c r="M24" s="1">
-        <v>100.52838885345039</v>
+        <v>100.5283888534504</v>
       </c>
       <c r="N24" t="s">
         <v>19</v>
       </c>
       <c r="O24">
-        <v>462.39441738592001</v>
+        <v>462.39441738592</v>
       </c>
       <c r="P24">
-        <v>1387.1832521577739</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1387.183252157774</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1722,31 +1683,31 @@
         <v>15</v>
       </c>
       <c r="C25" s="4">
-        <v>45690.590277777781</v>
+        <v>45690.59027777778</v>
       </c>
       <c r="D25" s="4">
-        <v>45690.722222222219</v>
-      </c>
-      <c r="E25" s="7">
+        <v>45690.72222222222</v>
+      </c>
+      <c r="E25">
         <v>99272.12</v>
       </c>
       <c r="F25" s="1">
         <v>99715.13450807023</v>
       </c>
       <c r="G25" s="1">
-        <v>97943.076475789276</v>
+        <v>97943.07647578928</v>
       </c>
       <c r="H25" s="1">
         <v>97727</v>
       </c>
-      <c r="I25" s="9">
-        <v>0.22462691746802951</v>
-      </c>
-      <c r="J25" s="10" t="s">
+      <c r="I25" s="1">
+        <v>0.2246269174680295</v>
+      </c>
+      <c r="J25" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="11">
-        <v>347.07554271820072</v>
+      <c r="K25">
+        <v>347.0755427182007</v>
       </c>
       <c r="L25" s="1">
         <v>10298.37387686144</v>
@@ -1758,13 +1719,13 @@
         <v>19</v>
       </c>
       <c r="O25">
-        <v>443.01450807023502</v>
+        <v>443.014508070235</v>
       </c>
       <c r="P25">
-        <v>1329.0435242107201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1329.04352421072</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1772,31 +1733,31 @@
         <v>15</v>
       </c>
       <c r="C26" s="4">
-        <v>45690.822916666657</v>
+        <v>45690.82291666666</v>
       </c>
       <c r="D26" s="4">
-        <v>45691.541666666657</v>
-      </c>
-      <c r="E26" s="7">
+        <v>45691.54166666666</v>
+      </c>
+      <c r="E26">
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
-        <v>99337.822219288209</v>
+        <v>99337.82221928821</v>
       </c>
       <c r="G26" s="1">
-        <v>96036.733342135369</v>
+        <v>96036.73334213537</v>
       </c>
       <c r="H26" s="1">
-        <v>94564.71</v>
-      </c>
-      <c r="I26" s="9">
+        <v>94564.71000000001</v>
+      </c>
+      <c r="I26" s="1">
         <v>0.1247875990027113</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="11">
-        <v>492.64147484686339</v>
+      <c r="K26">
+        <v>492.6414748468634</v>
       </c>
       <c r="L26" s="1">
         <v>10791.0153517083</v>
@@ -1808,13 +1769,13 @@
         <v>19</v>
       </c>
       <c r="O26">
-        <v>825.27221928820654</v>
+        <v>825.2722192882065</v>
       </c>
       <c r="P26">
-        <v>2475.8166578646342</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2475.816657864634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1822,30 +1783,30 @@
         <v>15</v>
       </c>
       <c r="C27" s="4">
-        <v>45691.611111111109</v>
+        <v>45691.61111111111</v>
       </c>
       <c r="D27" s="4">
-        <v>45691.635416666657</v>
-      </c>
-      <c r="E27" s="7">
+        <v>45691.63541666666</v>
+      </c>
+      <c r="E27">
         <v>96150.84</v>
       </c>
       <c r="F27" s="1">
-        <v>97150.404590042002</v>
+        <v>97150.404590042</v>
       </c>
       <c r="G27" s="1">
-        <v>93152.146229873964</v>
+        <v>93152.14622987396</v>
       </c>
       <c r="H27" s="1">
         <v>96570</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="1">
         <v>0.107957159139209</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="11">
+      <c r="J27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27">
         <v>-45.25132282479121</v>
       </c>
       <c r="L27" s="1">
@@ -1858,13 +1819,13 @@
         <v>19</v>
       </c>
       <c r="O27">
-        <v>999.56459004200588</v>
+        <v>999.5645900420059</v>
       </c>
       <c r="P27">
-        <v>2998.6937701260322</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2998.693770126032</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1872,49 +1833,49 @@
         <v>15</v>
       </c>
       <c r="C28" s="4">
-        <v>45691.666666666657</v>
+        <v>45691.66666666666</v>
       </c>
       <c r="D28" s="4">
-        <v>45691.784722222219</v>
-      </c>
-      <c r="E28" s="7">
-        <v>98730.93</v>
+        <v>45691.78472222222</v>
+      </c>
+      <c r="E28">
+        <v>98730.92999999999</v>
       </c>
       <c r="F28" s="1">
-        <v>99908.622508374698</v>
+        <v>99908.6225083747</v>
       </c>
       <c r="G28" s="1">
-        <v>95197.852474875894</v>
+        <v>95197.85247487589</v>
       </c>
       <c r="H28" s="1">
         <v>99795.94</v>
       </c>
-      <c r="I28" s="9">
-        <v>9.1244225062732123E-2</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="11">
-        <v>-97.176012134061182</v>
+      <c r="I28" s="1">
+        <v>0.09124422506273212</v>
+      </c>
+      <c r="J28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28">
+        <v>-97.17601213406118</v>
       </c>
       <c r="L28" s="1">
-        <v>10648.588016749451</v>
+        <v>10648.58801674945</v>
       </c>
       <c r="M28" s="1">
-        <v>107.45764028883509</v>
+        <v>107.4576402888351</v>
       </c>
       <c r="N28" t="s">
         <v>19</v>
       </c>
       <c r="O28">
-        <v>1177.6925083747051</v>
+        <v>1177.692508374705</v>
       </c>
       <c r="P28">
-        <v>3533.0775251240989</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3533.077525124099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1922,31 +1883,31 @@
         <v>15</v>
       </c>
       <c r="C29" s="4">
-        <v>45693.576388888891</v>
+        <v>45693.57638888889</v>
       </c>
       <c r="D29" s="4">
-        <v>45693.611111111109</v>
-      </c>
-      <c r="E29" s="7">
-        <v>98581.99</v>
+        <v>45693.61111111111</v>
+      </c>
+      <c r="E29">
+        <v>98581.99000000001</v>
       </c>
       <c r="F29" s="1">
-        <v>98923.605897969013</v>
+        <v>98923.60589796901</v>
       </c>
       <c r="G29" s="1">
-        <v>97557.142306092981</v>
+        <v>97557.14230609298</v>
       </c>
       <c r="H29" s="1">
-        <v>98746.93</v>
-      </c>
-      <c r="I29" s="9">
-        <v>0.31171230847445819</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="11">
-        <v>-51.413828159773317</v>
+        <v>98746.92999999999</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.3117123084744582</v>
+      </c>
+      <c r="J29" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29">
+        <v>-51.41382815977332</v>
       </c>
       <c r="L29" s="1">
         <v>10597.17418858967</v>
@@ -1958,13 +1919,13 @@
         <v>19</v>
       </c>
       <c r="O29">
-        <v>341.61589796900807</v>
+        <v>341.6158979690081</v>
       </c>
       <c r="P29">
         <v>1024.847693907024</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1972,49 +1933,49 @@
         <v>15</v>
       </c>
       <c r="C30" s="4">
-        <v>45694.864583333343</v>
+        <v>45694.86458333334</v>
       </c>
       <c r="D30" s="4">
-        <v>45695.541666666657</v>
-      </c>
-      <c r="E30" s="7">
-        <v>96870.9</v>
+        <v>45695.54166666666</v>
+      </c>
+      <c r="E30">
+        <v>96870.89999999999</v>
       </c>
       <c r="F30" s="1">
-        <v>97360.841236914697</v>
+        <v>97360.8412369147</v>
       </c>
       <c r="G30" s="1">
-        <v>95401.076289255885</v>
+        <v>95401.07628925589</v>
       </c>
       <c r="H30" s="1">
         <v>97900</v>
       </c>
-      <c r="I30" s="9">
-        <v>0.21629480007282181</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="11">
-        <v>-222.58897875494219</v>
+      <c r="I30" s="1">
+        <v>0.2162948000728218</v>
+      </c>
+      <c r="J30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30">
+        <v>-222.5889787549422</v>
       </c>
       <c r="L30" s="1">
         <v>10374.58520983473</v>
       </c>
       <c r="M30" s="1">
-        <v>105.97174188589671</v>
+        <v>105.9717418858967</v>
       </c>
       <c r="N30" t="s">
         <v>19</v>
       </c>
       <c r="O30">
-        <v>489.94123691470298</v>
+        <v>489.941236914703</v>
       </c>
       <c r="P30">
-        <v>1469.8237107441089</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1469.823710744109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2022,31 +1983,31 @@
         <v>15</v>
       </c>
       <c r="C31" s="4">
-        <v>45696.569444444453</v>
+        <v>45696.56944444445</v>
       </c>
       <c r="D31" s="4">
-        <v>45696.645833333343</v>
-      </c>
-      <c r="E31" s="7">
+        <v>45696.64583333334</v>
+      </c>
+      <c r="E31">
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
-        <v>96632.080105326022</v>
+        <v>96632.08010532602</v>
       </c>
       <c r="G31" s="1">
-        <v>95777.079684021941</v>
+        <v>95777.07968402194</v>
       </c>
       <c r="H31" s="1">
         <v>95688</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="1">
         <v>0.4853604724082356</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="11">
-        <v>354.47331381390762</v>
+      <c r="K31">
+        <v>354.4733138139076</v>
       </c>
       <c r="L31" s="1">
         <v>10729.05852364864</v>
@@ -2061,10 +2022,10 @@
         <v>213.7501053260203</v>
       </c>
       <c r="P31">
-        <v>641.25031597806083</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>641.2503159780608</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2072,49 +2033,49 @@
         <v>15</v>
       </c>
       <c r="C32" s="4">
-        <v>45696.711805555547</v>
+        <v>45696.71180555555</v>
       </c>
       <c r="D32" s="4">
-        <v>45696.777777777781</v>
-      </c>
-      <c r="E32" s="7">
-        <v>96282.74</v>
+        <v>45696.77777777778</v>
+      </c>
+      <c r="E32">
+        <v>96282.74000000001</v>
       </c>
       <c r="F32" s="1">
-        <v>96504.355459768733</v>
+        <v>96504.35545976873</v>
       </c>
       <c r="G32" s="1">
-        <v>95617.893620693823</v>
+        <v>95617.89362069382</v>
       </c>
       <c r="H32" s="1">
         <v>96423.03</v>
       </c>
-      <c r="I32" s="9">
-        <v>0.48412951582192121</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="11">
-        <v>-67.918529774654218</v>
+      <c r="I32" s="1">
+        <v>0.4841295158219212</v>
+      </c>
+      <c r="J32" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32">
+        <v>-67.91852977465422</v>
       </c>
       <c r="L32" s="1">
-        <v>10661.139993873991</v>
+        <v>10661.13999387399</v>
       </c>
       <c r="M32" s="1">
-        <v>107.29058523648639</v>
+        <v>107.2905852364864</v>
       </c>
       <c r="N32" t="s">
         <v>19</v>
       </c>
       <c r="O32">
-        <v>221.61545976872731</v>
+        <v>221.6154597687273</v>
       </c>
       <c r="P32">
-        <v>664.84637930618192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>664.8463793061819</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2122,49 +2083,49 @@
         <v>15</v>
       </c>
       <c r="C33" s="4">
-        <v>45696.805555555547</v>
+        <v>45696.80555555555</v>
       </c>
       <c r="D33" s="4">
-        <v>45697.572916666657</v>
-      </c>
-      <c r="E33" s="7">
+        <v>45697.57291666666</v>
+      </c>
+      <c r="E33">
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
-        <v>96814.100350878842</v>
+        <v>96814.10035087884</v>
       </c>
       <c r="G33" s="1">
-        <v>96048.258947363458</v>
+        <v>96048.25894736346</v>
       </c>
       <c r="H33" s="1">
         <v>95915.44</v>
       </c>
-      <c r="I33" s="9">
-        <v>0.55683278260679903</v>
-      </c>
-      <c r="J33" s="10" t="s">
+      <c r="I33" s="1">
+        <v>0.556832782606799</v>
+      </c>
+      <c r="J33" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="11">
-        <v>393.79214385952667</v>
+      <c r="K33">
+        <v>393.7921438595267</v>
       </c>
       <c r="L33" s="1">
-        <v>11054.932137733511</v>
+        <v>11054.93213773351</v>
       </c>
       <c r="M33" s="1">
-        <v>106.61139993873989</v>
+        <v>106.6113999387399</v>
       </c>
       <c r="N33" t="s">
         <v>19</v>
       </c>
       <c r="O33">
-        <v>191.46035087884229</v>
+        <v>191.4603508788423</v>
       </c>
       <c r="P33">
-        <v>574.38105263654143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>574.3810526365414</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2172,31 +2133,31 @@
         <v>15</v>
       </c>
       <c r="C34" s="4">
-        <v>45697.652777777781</v>
+        <v>45697.65277777778</v>
       </c>
       <c r="D34" s="4">
-        <v>45697.899305555547</v>
-      </c>
-      <c r="E34" s="7">
+        <v>45697.89930555555</v>
+      </c>
+      <c r="E34">
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
-        <v>96880.507053391193</v>
+        <v>96880.50705339119</v>
       </c>
       <c r="G34" s="1">
-        <v>95806.678839826433</v>
+        <v>95806.67883982643</v>
       </c>
       <c r="H34" s="1">
-        <v>95376.65</v>
-      </c>
-      <c r="I34" s="9">
-        <v>0.41179518280804822</v>
-      </c>
-      <c r="J34" s="10" t="s">
+        <v>95376.64999999999</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.4117951828080482</v>
+      </c>
+      <c r="J34" t="s">
         <v>18</v>
       </c>
-      <c r="K34" s="11">
-        <v>508.73176884106641</v>
+      <c r="K34">
+        <v>508.7317688410664</v>
       </c>
       <c r="L34" s="1">
         <v>11563.66390657458</v>
@@ -2208,13 +2169,13 @@
         <v>19</v>
       </c>
       <c r="O34">
-        <v>268.45705339119007</v>
+        <v>268.4570533911901</v>
       </c>
       <c r="P34">
-        <v>805.37116017357039</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <v>805.3711601735704</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2222,16 +2183,16 @@
         <v>15</v>
       </c>
       <c r="C35" s="4">
-        <v>45699.888888888891</v>
+        <v>45699.88888888889</v>
       </c>
       <c r="D35" s="4">
-        <v>45699.899305555547</v>
-      </c>
-      <c r="E35" s="7">
+        <v>45699.89930555555</v>
+      </c>
+      <c r="E35">
         <v>95686.37</v>
       </c>
       <c r="F35" s="1">
-        <v>96056.143740286512</v>
+        <v>96056.14374028651</v>
       </c>
       <c r="G35" s="1">
         <v>94577.04877914043</v>
@@ -2239,14 +2200,14 @@
       <c r="H35" s="1">
         <v>95959.38</v>
       </c>
-      <c r="I35" s="9">
-        <v>0.31272269084371818</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="11">
-        <v>-85.376421827246432</v>
+      <c r="I35" s="1">
+        <v>0.3127226908437182</v>
+      </c>
+      <c r="J35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35">
+        <v>-85.37642182724643</v>
       </c>
       <c r="L35" s="1">
         <v>11478.28748474733</v>
@@ -2258,13 +2219,13 @@
         <v>19</v>
       </c>
       <c r="O35">
-        <v>369.77374028651678</v>
+        <v>369.7737402865168</v>
       </c>
       <c r="P35">
-        <v>1109.3212208595651</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1109.321220859565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2277,44 +2238,44 @@
       <c r="D36" s="4">
         <v>45700.5625</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36">
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
-        <v>96720.531834451787</v>
+        <v>96720.53183445179</v>
       </c>
       <c r="G36" s="1">
-        <v>95109.084496644617</v>
+        <v>95109.08449664462</v>
       </c>
       <c r="H36" s="1">
-        <v>94844.800000000003</v>
-      </c>
-      <c r="I36" s="9">
-        <v>0.28491871165624028</v>
-      </c>
-      <c r="J36" s="10" t="s">
+        <v>94844.8</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.2849187116562403</v>
+      </c>
+      <c r="J36" t="s">
         <v>18</v>
       </c>
-      <c r="K36" s="11">
-        <v>419.64822283712539</v>
+      <c r="K36">
+        <v>419.6482228371254</v>
       </c>
       <c r="L36" s="1">
         <v>11897.93570758446</v>
       </c>
       <c r="M36" s="1">
-        <v>114.78287484747329</v>
+        <v>114.7828748474733</v>
       </c>
       <c r="N36" t="s">
         <v>19</v>
       </c>
       <c r="O36">
-        <v>402.86183445178898</v>
+        <v>402.861834451789</v>
       </c>
       <c r="P36">
-        <v>1208.5855033553819</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1208.585503355382</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2322,31 +2283,31 @@
         <v>15</v>
       </c>
       <c r="C37" s="4">
-        <v>45701.798611111109</v>
+        <v>45701.79861111111</v>
       </c>
       <c r="D37" s="4">
-        <v>45701.895833333343</v>
-      </c>
-      <c r="E37" s="7">
+        <v>45701.89583333334</v>
+      </c>
+      <c r="E37">
         <v>96270.05</v>
       </c>
       <c r="F37" s="1">
-        <v>96701.702112878702</v>
+        <v>96701.70211287875</v>
       </c>
       <c r="G37" s="1">
-        <v>94975.093661363804</v>
+        <v>94975.09366136376</v>
       </c>
       <c r="H37" s="1">
-        <v>96412.79</v>
-      </c>
-      <c r="I37" s="9">
-        <v>0.27563714742957268</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="11">
-        <v>-39.344446424094649</v>
+        <v>96412.78999999999</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.2756371474295727</v>
+      </c>
+      <c r="J37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37">
+        <v>-39.34444642409465</v>
       </c>
       <c r="L37" s="1">
         <v>11858.59126116036</v>
@@ -2358,18 +2319,18 @@
         <v>19</v>
       </c>
       <c r="O37">
-        <v>431.65211287874263</v>
+        <v>431.6521128787426</v>
       </c>
       <c r="P37">
         <v>1294.956338636242</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2377,7 +2338,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2385,15 +2346,15 @@
         <v>11858.59126116036</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="5">
-        <v>0.18585912611603631</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.1858591261160363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -2401,7 +2362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
attempt to fix PnL - still not working
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Backtesting\strategy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Trade History" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
   <si>
     <t>Position</t>
   </si>
@@ -50,6 +55,9 @@
   </si>
   <si>
     <t>Risk Amount ($)</t>
+  </si>
+  <si>
+    <t>Actual Risk ($)</t>
   </si>
   <si>
     <t>Risk-Reward Ratio</t>
@@ -97,13 +105,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +121,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -158,10 +173,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -169,13 +185,24 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -222,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,9 +281,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,22 +492,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="15.7109375" customWidth="1"/>
+    <col min="6" max="8" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="7" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +544,7 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -524,69 +562,75 @@
       <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4">
-        <v>45666.63541666666</v>
+        <v>45666.635416666657</v>
       </c>
       <c r="D2" s="4">
-        <v>45666.64583333334</v>
+        <v>45666.645833333343</v>
       </c>
       <c r="E2">
         <v>93188.2</v>
       </c>
       <c r="F2" s="1">
-        <v>93801.34997159497</v>
+        <v>93801.349971594973</v>
       </c>
       <c r="G2" s="1">
-        <v>91348.75008521508</v>
+        <v>91348.750085215084</v>
       </c>
       <c r="H2" s="1">
         <v>93452</v>
       </c>
       <c r="I2" s="1">
-        <v>0.1630922362107786</v>
+        <v>0.16309223621077859</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <v>-43.02373191240387</v>
+        <v>18</v>
+      </c>
+      <c r="K2" s="7">
+        <v>-43.023731912403868</v>
       </c>
       <c r="L2" s="1">
-        <v>9956.976268087596</v>
+        <v>9956.9762680875956</v>
       </c>
       <c r="M2" s="1">
         <v>100</v>
       </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2">
+      <c r="N2">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2">
         <v>613.1499715949758</v>
       </c>
-      <c r="P2">
-        <v>1839.449914784913</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2">
+        <v>1839.4499147849131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4">
-        <v>45666.64930555555</v>
+        <v>45666.649305555547</v>
       </c>
       <c r="D3" s="4">
-        <v>45666.65972222222</v>
+        <v>45666.659722222219</v>
       </c>
       <c r="E3">
         <v>93739.87</v>
@@ -595,169 +639,178 @@
         <v>94376.30887387348</v>
       </c>
       <c r="G3" s="1">
-        <v>91830.55337837953</v>
+        <v>91830.553378379525</v>
       </c>
       <c r="H3" s="1">
-        <v>94100.49000000001</v>
+        <v>94100.49</v>
       </c>
       <c r="I3" s="1">
-        <v>0.1564482729894796</v>
+        <v>0.15644827298947961</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3">
-        <v>-56.41837620546767</v>
+        <v>18</v>
+      </c>
+      <c r="K3" s="7">
+        <v>-56.418376205467673</v>
       </c>
       <c r="L3" s="1">
-        <v>9900.557891882128</v>
+        <v>9900.5578918821284</v>
       </c>
       <c r="M3" s="1">
-        <v>99.56976268087595</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3">
-        <v>636.4388738734851</v>
+        <v>99.569762680875954</v>
+      </c>
+      <c r="N3">
+        <v>99.569762680875954</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
       </c>
       <c r="P3">
+        <v>636.43887387348514</v>
+      </c>
+      <c r="Q3">
         <v>1909.31662162047</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
-        <v>45666.66319444445</v>
+        <v>45666.663194444453</v>
       </c>
       <c r="D4" s="4">
-        <v>45666.82291666666</v>
+        <v>45666.822916666657</v>
       </c>
       <c r="E4">
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
-        <v>94919.84370097617</v>
+        <v>94919.843700976169</v>
       </c>
       <c r="G4" s="1">
-        <v>92216.54889707149</v>
+        <v>92216.548897071494</v>
       </c>
       <c r="H4" s="1">
-        <v>92106.85000000001</v>
+        <v>92106.85</v>
       </c>
       <c r="I4" s="1">
-        <v>0.1464961627948485</v>
+        <v>0.14649616279484851</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4">
-        <v>313.0872042402661</v>
+        <v>19</v>
+      </c>
+      <c r="K4" s="7">
+        <v>313.08720424026609</v>
       </c>
       <c r="L4" s="1">
-        <v>10213.64509612239</v>
+        <v>10213.645096122391</v>
       </c>
       <c r="M4" s="1">
-        <v>99.00557891882129</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4">
-        <v>675.8237009761651</v>
+        <v>99.005578918821286</v>
+      </c>
+      <c r="N4">
+        <v>99.005578918821286</v>
+      </c>
+      <c r="O4" t="s">
+        <v>20</v>
       </c>
       <c r="P4">
-        <v>2027.47110292851</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>675.82370097616513</v>
+      </c>
+      <c r="Q4">
+        <v>2027.4711029285099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4">
         <v>45667.75</v>
       </c>
       <c r="D5" s="4">
-        <v>45670.54166666666</v>
+        <v>45670.541666666657</v>
       </c>
       <c r="E5">
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
-        <v>96318.69892474354</v>
+        <v>96318.698924743541</v>
       </c>
       <c r="G5" s="1">
         <v>92990.82322576936</v>
       </c>
       <c r="H5" s="1">
-        <v>90583.24000000001</v>
+        <v>90583.24</v>
       </c>
       <c r="I5" s="1">
         <v>0.1227647426767863</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5">
-        <v>601.9756880681938</v>
+        <v>19</v>
+      </c>
+      <c r="K5" s="7">
+        <v>601.97568806819379</v>
       </c>
       <c r="L5" s="1">
-        <v>10815.62078419059</v>
+        <v>10815.620784190591</v>
       </c>
       <c r="M5" s="1">
         <v>102.1364509612239</v>
       </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5">
-        <v>831.9689247435454</v>
+      <c r="N5">
+        <v>102.1364509612239</v>
+      </c>
+      <c r="O5" t="s">
+        <v>20</v>
       </c>
       <c r="P5">
-        <v>2495.906774230636</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>831.96892474354536</v>
+      </c>
+      <c r="Q5">
+        <v>2495.9067742306361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4">
-        <v>45670.63541666666</v>
+        <v>45670.635416666657</v>
       </c>
       <c r="D6" s="4">
-        <v>45670.86805555555</v>
+        <v>45670.868055555547</v>
       </c>
       <c r="E6">
-        <v>92680.00999999999</v>
+        <v>92680.01</v>
       </c>
       <c r="F6" s="1">
-        <v>93739.19579047592</v>
+        <v>93739.195790475918</v>
       </c>
       <c r="G6" s="1">
-        <v>89502.45262857222</v>
+        <v>89502.452628572224</v>
       </c>
       <c r="H6" s="1">
-        <v>93228.99000000001</v>
+        <v>93228.99</v>
       </c>
       <c r="I6" s="1">
-        <v>0.1021125932904633</v>
+        <v>0.10211259329046329</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6">
-        <v>-56.05777146459963</v>
+        <v>18</v>
+      </c>
+      <c r="K6" s="7">
+        <v>-56.057771464599632</v>
       </c>
       <c r="L6" s="1">
         <v>10759.56301272599</v>
@@ -765,78 +818,84 @@
       <c r="M6" s="1">
         <v>108.1562078419059</v>
       </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6">
+      <c r="N6">
+        <v>108.1562078419059</v>
+      </c>
+      <c r="O6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6">
         <v>1059.185790475924</v>
       </c>
-      <c r="P6">
-        <v>3177.557371427771</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6">
+        <v>3177.5573714277712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4">
         <v>45673.625</v>
       </c>
       <c r="D7" s="4">
-        <v>45673.67013888889</v>
+        <v>45673.670138888891</v>
       </c>
       <c r="E7">
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
-        <v>96887.64624180444</v>
+        <v>96887.646241804439</v>
       </c>
       <c r="G7" s="1">
-        <v>99621.98127458667</v>
+        <v>99621.981274586666</v>
       </c>
       <c r="H7" s="1">
         <v>99815.27</v>
       </c>
       <c r="I7" s="1">
-        <v>0.1573993367122679</v>
+        <v>0.15739933671226791</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7">
-        <v>353.2104075557988</v>
+        <v>19</v>
+      </c>
+      <c r="K7" s="7">
+        <v>353.21040755579878</v>
       </c>
       <c r="L7" s="1">
         <v>11112.77342028179</v>
       </c>
       <c r="M7" s="1">
-        <v>107.5956301272599</v>
-      </c>
-      <c r="N7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7">
-        <v>683.5837581955566</v>
+        <v>107.59563012725989</v>
+      </c>
+      <c r="N7">
+        <v>107.59563012725989</v>
+      </c>
+      <c r="O7" t="s">
+        <v>20</v>
       </c>
       <c r="P7">
-        <v>2050.75127458667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>683.58375819555658</v>
+      </c>
+      <c r="Q7">
+        <v>2050.7512745866702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4">
-        <v>45674.87152777778</v>
+        <v>45674.871527777781</v>
       </c>
       <c r="D8" s="4">
-        <v>45675.54166666666</v>
+        <v>45675.541666666657</v>
       </c>
       <c r="E8">
         <v>104692.7</v>
@@ -845,19 +904,19 @@
         <v>104197.1529992671</v>
       </c>
       <c r="G8" s="1">
-        <v>106179.3410021986</v>
+        <v>106179.34100219861</v>
       </c>
       <c r="H8" s="1">
         <v>103424.59</v>
       </c>
       <c r="I8" s="1">
-        <v>0.2242526622872638</v>
+        <v>0.22425266228726379</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8">
-        <v>-284.3770435731022</v>
+        <v>18</v>
+      </c>
+      <c r="K8" s="7">
+        <v>-284.37704357310218</v>
       </c>
       <c r="L8" s="1">
         <v>10828.39637670869</v>
@@ -865,28 +924,31 @@
       <c r="M8" s="1">
         <v>111.1277342028179</v>
       </c>
-      <c r="N8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8">
-        <v>495.547000732884</v>
+      <c r="N8">
+        <v>111.1277342028179</v>
+      </c>
+      <c r="O8" t="s">
+        <v>20</v>
       </c>
       <c r="P8">
+        <v>495.54700073288399</v>
+      </c>
+      <c r="Q8">
         <v>1486.641002198638</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4">
-        <v>45675.70138888889</v>
+        <v>45675.701388888891</v>
       </c>
       <c r="D9" s="4">
-        <v>45676.54166666666</v>
+        <v>45676.541666666657</v>
       </c>
       <c r="E9">
         <v>103240.85</v>
@@ -895,7 +957,7 @@
         <v>102688.8552242209</v>
       </c>
       <c r="G9" s="1">
-        <v>104896.8343273375</v>
+        <v>104896.83432733751</v>
       </c>
       <c r="H9" s="1">
         <v>105157.8</v>
@@ -904,39 +966,42 @@
         <v>0.1961684575986099</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9">
-        <v>376.0451247936547</v>
+        <v>19</v>
+      </c>
+      <c r="K9" s="7">
+        <v>376.04512479365468</v>
       </c>
       <c r="L9" s="1">
-        <v>11204.44150150234</v>
+        <v>11204.441501502341</v>
       </c>
       <c r="M9" s="1">
         <v>108.2839637670869</v>
       </c>
-      <c r="N9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9">
-        <v>551.9947757791524</v>
+      <c r="N9">
+        <v>108.2839637670869</v>
+      </c>
+      <c r="O9" t="s">
+        <v>20</v>
       </c>
       <c r="P9">
+        <v>551.99477577915241</v>
+      </c>
+      <c r="Q9">
         <v>1655.984327337472</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4">
-        <v>45677.65972222222</v>
+        <v>45677.659722222219</v>
       </c>
       <c r="D10" s="4">
-        <v>45677.67361111111</v>
+        <v>45677.673611111109</v>
       </c>
       <c r="E10">
         <v>105535.7</v>
@@ -945,7 +1010,7 @@
         <v>104427.1512541753</v>
       </c>
       <c r="G10" s="1">
-        <v>108861.3462374741</v>
+        <v>108861.34623747411</v>
       </c>
       <c r="H10" s="1">
         <v>103708</v>
@@ -954,9 +1019,9 @@
         <v>0.1010730610061438</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10">
+        <v>18</v>
+      </c>
+      <c r="K10" s="7">
         <v>-184.7312336009287</v>
       </c>
       <c r="L10" s="1">
@@ -965,28 +1030,31 @@
       <c r="M10" s="1">
         <v>112.0444150150234</v>
       </c>
-      <c r="N10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10">
+      <c r="N10">
+        <v>112.0444150150234</v>
+      </c>
+      <c r="O10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10">
         <v>1108.548745824693</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>3325.64623747408</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
-        <v>45678.62847222222</v>
+        <v>45678.628472222219</v>
       </c>
       <c r="D11" s="4">
-        <v>45678.67361111111</v>
+        <v>45678.673611111109</v>
       </c>
       <c r="E11">
         <v>103281.22</v>
@@ -1004,45 +1072,48 @@
         <v>0.1152930814464031</v>
       </c>
       <c r="J11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11">
-        <v>348.0444484087726</v>
+        <v>19</v>
+      </c>
+      <c r="K11" s="7">
+        <v>348.04444840877261</v>
       </c>
       <c r="L11" s="1">
-        <v>11367.75471631018</v>
+        <v>11367.754716310181</v>
       </c>
       <c r="M11" s="1">
-        <v>110.1971026790141</v>
-      </c>
-      <c r="N11" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11">
-        <v>955.7997869129904</v>
+        <v>110.19710267901409</v>
+      </c>
+      <c r="N11">
+        <v>110.19710267901409</v>
+      </c>
+      <c r="O11" t="s">
+        <v>20</v>
       </c>
       <c r="P11">
-        <v>2867.399360738986</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>955.79978691299038</v>
+      </c>
+      <c r="Q11">
+        <v>2867.3993607389862</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4">
-        <v>45678.86111111111</v>
+        <v>45678.861111111109</v>
       </c>
       <c r="D12" s="4">
-        <v>45679.54166666666</v>
+        <v>45679.541666666657</v>
       </c>
       <c r="E12">
         <v>106072</v>
       </c>
       <c r="F12" s="1">
-        <v>105391.0783661026</v>
+        <v>105391.07836610261</v>
       </c>
       <c r="G12" s="1">
         <v>108114.7649016923</v>
@@ -1051,48 +1122,51 @@
         <v>105039.74</v>
       </c>
       <c r="I12" s="1">
-        <v>0.1669465934169848</v>
+        <v>0.16694659341698481</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12">
+        <v>18</v>
+      </c>
+      <c r="K12" s="7">
         <v>-172.3322905206158</v>
       </c>
       <c r="L12" s="1">
-        <v>11195.42242578957</v>
+        <v>11195.422425789569</v>
       </c>
       <c r="M12" s="1">
-        <v>113.6775471631018</v>
-      </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12">
+        <v>113.67754716310181</v>
+      </c>
+      <c r="N12">
+        <v>113.67754716310181</v>
+      </c>
+      <c r="O12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12">
         <v>680.921633897422</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2042.764901692251</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4">
-        <v>45679.54861111111</v>
+        <v>45679.548611111109</v>
       </c>
       <c r="D13" s="4">
-        <v>45679.56597222222</v>
+        <v>45679.565972222219</v>
       </c>
       <c r="E13">
         <v>104947.17</v>
       </c>
       <c r="F13" s="1">
-        <v>104638.4792248785</v>
+        <v>104638.47922487849</v>
       </c>
       <c r="G13" s="1">
         <v>105873.2423253646</v>
@@ -1101,48 +1175,51 @@
         <v>104283.67</v>
       </c>
       <c r="I13" s="1">
-        <v>0.3626743436496069</v>
+        <v>0.36267434364960688</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13">
-        <v>-240.6344270115142</v>
+        <v>18</v>
+      </c>
+      <c r="K13" s="7">
+        <v>-240.63442701151419</v>
       </c>
       <c r="L13" s="1">
-        <v>10954.78799877805</v>
+        <v>10954.787998778051</v>
       </c>
       <c r="M13" s="1">
         <v>111.9542242578957</v>
       </c>
-      <c r="N13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13">
-        <v>308.6907751215476</v>
+      <c r="N13">
+        <v>111.9542242578957</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
       </c>
       <c r="P13">
-        <v>926.0723253646429</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>308.69077512154757</v>
+      </c>
+      <c r="Q13">
+        <v>926.07232536464289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4">
-        <v>45679.57986111111</v>
+        <v>45679.579861111109</v>
       </c>
       <c r="D14" s="4">
-        <v>45679.69444444445</v>
+        <v>45679.694444444453</v>
       </c>
       <c r="E14">
         <v>104073.94</v>
       </c>
       <c r="F14" s="1">
-        <v>103607.8322012325</v>
+        <v>103607.83220123249</v>
       </c>
       <c r="G14" s="1">
         <v>105472.2633963026</v>
@@ -1151,42 +1228,45 @@
         <v>103339.12</v>
       </c>
       <c r="I14" s="1">
-        <v>0.2350269192608282</v>
+        <v>0.23502691926082819</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14">
-        <v>-172.7024808112434</v>
+        <v>18</v>
+      </c>
+      <c r="K14" s="7">
+        <v>-172.70248081124339</v>
       </c>
       <c r="L14" s="1">
-        <v>10782.08551796681</v>
+        <v>10782.085517966811</v>
       </c>
       <c r="M14" s="1">
         <v>109.5478799877805</v>
       </c>
-      <c r="N14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14">
-        <v>466.107798767538</v>
+      <c r="N14">
+        <v>109.5478799877805</v>
+      </c>
+      <c r="O14" t="s">
+        <v>20</v>
       </c>
       <c r="P14">
-        <v>1398.323396302614</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>466.10779876753799</v>
+      </c>
+      <c r="Q14">
+        <v>1398.3233963026139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4">
-        <v>45679.88194444445</v>
+        <v>45679.881944444453</v>
       </c>
       <c r="D15" s="4">
-        <v>45680.54166666666</v>
+        <v>45680.541666666657</v>
       </c>
       <c r="E15">
         <v>103891.76</v>
@@ -1201,13 +1281,13 @@
         <v>101592.48</v>
       </c>
       <c r="I15" s="1">
-        <v>0.2121359156868931</v>
+        <v>0.21213591568689311</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15">
-        <v>-487.7598682205594</v>
+        <v>18</v>
+      </c>
+      <c r="K15" s="7">
+        <v>-487.75986822055938</v>
       </c>
       <c r="L15" s="1">
         <v>10294.32564974625</v>
@@ -1215,28 +1295,31 @@
       <c r="M15" s="1">
         <v>107.8208551796681</v>
       </c>
-      <c r="N15" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15">
-        <v>508.2630860999925</v>
+      <c r="N15">
+        <v>107.8208551796681</v>
+      </c>
+      <c r="O15" t="s">
+        <v>20</v>
       </c>
       <c r="P15">
+        <v>508.26308609999251</v>
+      </c>
+      <c r="Q15">
         <v>1524.789258299978</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4">
-        <v>45680.82986111111</v>
+        <v>45680.829861111109</v>
       </c>
       <c r="D16" s="4">
-        <v>45680.85069444445</v>
+        <v>45680.850694444453</v>
       </c>
       <c r="E16">
         <v>103770.04</v>
@@ -1254,39 +1337,42 @@
         <v>0.1191027928070732</v>
       </c>
       <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16">
+        <v>19</v>
+      </c>
+      <c r="K16" s="7">
         <v>315.7403127036236</v>
       </c>
       <c r="L16" s="1">
-        <v>10610.06596244987</v>
+        <v>10610.065962449869</v>
       </c>
       <c r="M16" s="1">
         <v>102.9432564974625</v>
       </c>
-      <c r="N16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16">
-        <v>864.3227759084839</v>
+      <c r="N16">
+        <v>102.9432564974625</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
       </c>
       <c r="P16">
-        <v>2592.968327725452</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>864.32277590848389</v>
+      </c>
+      <c r="Q16">
+        <v>2592.9683277254521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="4">
-        <v>45681.82986111111</v>
+        <v>45681.829861111109</v>
       </c>
       <c r="D17" s="4">
-        <v>45681.84722222222</v>
+        <v>45681.847222222219</v>
       </c>
       <c r="E17">
         <v>105760.94</v>
@@ -1301,42 +1387,45 @@
         <v>105291.54</v>
       </c>
       <c r="I17" s="1">
-        <v>0.2274224285203547</v>
+        <v>0.22742242852035471</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17">
+        <v>18</v>
+      </c>
+      <c r="K17" s="7">
         <v>-106.7520879474565</v>
       </c>
       <c r="L17" s="1">
-        <v>10503.31387450242</v>
+        <v>10503.313874502421</v>
       </c>
       <c r="M17" s="1">
         <v>106.1006596244987</v>
       </c>
-      <c r="N17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17">
-        <v>466.535602116317</v>
+      <c r="N17">
+        <v>106.1006596244987</v>
+      </c>
+      <c r="O17" t="s">
+        <v>20</v>
       </c>
       <c r="P17">
-        <v>1399.606806348951</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>466.53560211631702</v>
+      </c>
+      <c r="Q17">
+        <v>1399.6068063489511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4">
-        <v>45681.85763888889</v>
+        <v>45681.857638888891</v>
       </c>
       <c r="D18" s="4">
-        <v>45682.58680555555</v>
+        <v>45682.586805555547</v>
       </c>
       <c r="E18">
         <v>105052.52</v>
@@ -1345,7 +1434,7 @@
         <v>104590.815085935</v>
       </c>
       <c r="G18" s="1">
-        <v>106437.6347421952</v>
+        <v>106437.63474219519</v>
       </c>
       <c r="H18" s="1">
         <v>104541.68</v>
@@ -1354,36 +1443,39 @@
         <v>0.2274897570837339</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18">
+        <v>18</v>
+      </c>
+      <c r="K18" s="7">
         <v>-116.2108675086571</v>
       </c>
       <c r="L18" s="1">
-        <v>10387.10300699376</v>
+        <v>10387.103006993761</v>
       </c>
       <c r="M18" s="1">
         <v>105.0331387450242</v>
       </c>
-      <c r="N18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18">
+      <c r="N18">
+        <v>105.0331387450242</v>
+      </c>
+      <c r="O18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18">
         <v>461.7049140650488</v>
       </c>
-      <c r="P18">
-        <v>1385.114742195161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>1385.1147421951609</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4">
-        <v>45683.88541666666</v>
+        <v>45683.885416666657</v>
       </c>
       <c r="D19" s="4">
         <v>45683.90625</v>
@@ -1395,19 +1487,19 @@
         <v>104635.5126717815</v>
       </c>
       <c r="G19" s="1">
-        <v>105275.6219846556</v>
+        <v>105275.62198465561</v>
       </c>
       <c r="H19" s="1">
         <v>104552.48</v>
       </c>
       <c r="I19" s="1">
-        <v>0.649083073661574</v>
+        <v>0.64908307366157403</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19">
-        <v>-157.7661318841807</v>
+        <v>18</v>
+      </c>
+      <c r="K19" s="7">
+        <v>-157.76613188418071</v>
       </c>
       <c r="L19" s="1">
         <v>10229.33687510958</v>
@@ -1415,28 +1507,31 @@
       <c r="M19" s="1">
         <v>103.8710300699376</v>
       </c>
-      <c r="N19" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19">
-        <v>160.0273282185371</v>
+      <c r="N19">
+        <v>103.8710300699376</v>
+      </c>
+      <c r="O19" t="s">
+        <v>20</v>
       </c>
       <c r="P19">
+        <v>160.02732821853709</v>
+      </c>
+      <c r="Q19">
         <v>480.0819846555969</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4">
-        <v>45684.54166666666</v>
+        <v>45684.541666666657</v>
       </c>
       <c r="D20" s="4">
-        <v>45684.54513888889</v>
+        <v>45684.545138888891</v>
       </c>
       <c r="E20">
         <v>100632.01</v>
@@ -1445,98 +1540,104 @@
         <v>101286.0915115136</v>
       </c>
       <c r="G20" s="1">
-        <v>98669.76546545928</v>
+        <v>98669.765465459277</v>
       </c>
       <c r="H20" s="1">
         <v>100622.87</v>
       </c>
       <c r="I20" s="1">
-        <v>0.1563923868057115</v>
+        <v>0.15639238680571149</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20">
-        <v>1.429426415404112</v>
+        <v>18</v>
+      </c>
+      <c r="K20" s="7">
+        <v>1.4294264154041121</v>
       </c>
       <c r="L20" s="1">
-        <v>10230.76630152499</v>
+        <v>10230.766301524989</v>
       </c>
       <c r="M20" s="1">
         <v>102.2933687510958</v>
       </c>
-      <c r="N20" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20">
-        <v>654.0815115135774</v>
+      <c r="N20">
+        <v>102.2933687510958</v>
+      </c>
+      <c r="O20" t="s">
+        <v>20</v>
       </c>
       <c r="P20">
+        <v>654.08151151357742</v>
+      </c>
+      <c r="Q20">
         <v>1962.244534540718</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4">
-        <v>45684.85069444445</v>
+        <v>45684.850694444453</v>
       </c>
       <c r="D21" s="4">
-        <v>45684.86458333334</v>
+        <v>45684.864583333343</v>
       </c>
       <c r="E21">
-        <v>100351.68</v>
+        <v>100351.67999999999</v>
       </c>
       <c r="F21" s="1">
         <v>100958.2739530618</v>
       </c>
       <c r="G21" s="1">
-        <v>98531.89814081455</v>
+        <v>98531.898140814548</v>
       </c>
       <c r="H21" s="1">
         <v>100932.23</v>
       </c>
       <c r="I21" s="1">
-        <v>0.1686592200579081</v>
+        <v>0.16865922005790809</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21">
-        <v>-97.91511020461905</v>
+        <v>18</v>
+      </c>
+      <c r="K21" s="7">
+        <v>-97.915110204619054</v>
       </c>
       <c r="L21" s="1">
-        <v>10132.85119132037</v>
+        <v>10132.851191320369</v>
       </c>
       <c r="M21" s="1">
         <v>102.3076630152499</v>
       </c>
-      <c r="N21" t="s">
-        <v>19</v>
-      </c>
-      <c r="O21">
-        <v>606.5939530618198</v>
+      <c r="N21">
+        <v>102.3076630152499</v>
+      </c>
+      <c r="O21" t="s">
+        <v>20</v>
       </c>
       <c r="P21">
+        <v>606.59395306181978</v>
+      </c>
+      <c r="Q21">
         <v>1819.781859185445</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="4">
-        <v>45684.87152777778</v>
+        <v>45684.871527777781</v>
       </c>
       <c r="D22" s="4">
-        <v>45684.87847222222</v>
+        <v>45684.878472222219</v>
       </c>
       <c r="E22">
         <v>101386.5</v>
@@ -1545,7 +1646,7 @@
         <v>102047.4840323447</v>
       </c>
       <c r="G22" s="1">
-        <v>99403.54790296599</v>
+        <v>99403.547902965991</v>
       </c>
       <c r="H22" s="1">
         <v>101604</v>
@@ -1554,36 +1655,39 @@
         <v>0.1532994852443969</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22">
-        <v>-33.34263804065633</v>
+        <v>18</v>
+      </c>
+      <c r="K22" s="7">
+        <v>-33.342638040656333</v>
       </c>
       <c r="L22" s="1">
-        <v>10099.50855327971</v>
+        <v>10099.508553279709</v>
       </c>
       <c r="M22" s="1">
         <v>101.3285119132037</v>
       </c>
-      <c r="N22" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22">
-        <v>660.9840323446697</v>
+      <c r="N22">
+        <v>101.3285119132037</v>
+      </c>
+      <c r="O22" t="s">
+        <v>20</v>
       </c>
       <c r="P22">
-        <v>1982.952097034009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>660.98403234466969</v>
+      </c>
+      <c r="Q22">
+        <v>1982.9520970340091</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4">
-        <v>45684.88194444445</v>
+        <v>45684.881944444453</v>
       </c>
       <c r="D23" s="4">
         <v>45685.625</v>
@@ -1601,48 +1705,51 @@
         <v>102625.01</v>
       </c>
       <c r="I23" s="1">
-        <v>0.141470392963317</v>
+        <v>0.14147039296331701</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23">
+        <v>18</v>
+      </c>
+      <c r="K23" s="7">
         <v>-46.66966793466856</v>
       </c>
       <c r="L23" s="1">
         <v>10052.83888534504</v>
       </c>
       <c r="M23" s="1">
-        <v>100.9950855327971</v>
-      </c>
-      <c r="N23" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23">
-        <v>713.8955608823744</v>
+        <v>100.99508553279711</v>
+      </c>
+      <c r="N23">
+        <v>100.99508553279711</v>
+      </c>
+      <c r="O23" t="s">
+        <v>20</v>
       </c>
       <c r="P23">
-        <v>2141.686682647123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>713.89556088237441</v>
+      </c>
+      <c r="Q23">
+        <v>2141.6866826471228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="4">
-        <v>45687.73611111111</v>
+        <v>45687.736111111109</v>
       </c>
       <c r="D24" s="4">
-        <v>45688.56597222222</v>
+        <v>45688.565972222219</v>
       </c>
       <c r="E24">
         <v>105018.14</v>
       </c>
       <c r="F24" s="1">
-        <v>104555.7455826141</v>
+        <v>104555.74558261409</v>
       </c>
       <c r="G24" s="1">
         <v>106405.3232521578</v>
@@ -1651,42 +1758,45 @@
         <v>104551.09</v>
       </c>
       <c r="I24" s="1">
-        <v>0.2174083100349117</v>
+        <v>0.21740831003491171</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24">
+        <v>18</v>
+      </c>
+      <c r="K24" s="7">
         <v>-101.5405512018061</v>
       </c>
       <c r="L24" s="1">
-        <v>9951.298334143235</v>
+        <v>9951.2983341432355</v>
       </c>
       <c r="M24" s="1">
-        <v>100.5283888534504</v>
-      </c>
-      <c r="N24" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24">
-        <v>462.39441738592</v>
+        <v>100.52838885345039</v>
+      </c>
+      <c r="N24">
+        <v>100.52838885345039</v>
+      </c>
+      <c r="O24" t="s">
+        <v>20</v>
       </c>
       <c r="P24">
-        <v>1387.183252157774</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>462.39441738592001</v>
+      </c>
+      <c r="Q24">
+        <v>1387.1832521577739</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4">
-        <v>45690.59027777778</v>
+        <v>45690.590277777781</v>
       </c>
       <c r="D25" s="4">
-        <v>45690.72222222222</v>
+        <v>45690.722222222219</v>
       </c>
       <c r="E25">
         <v>99272.12</v>
@@ -1695,19 +1805,19 @@
         <v>99715.13450807023</v>
       </c>
       <c r="G25" s="1">
-        <v>97943.07647578928</v>
+        <v>97943.076475789276</v>
       </c>
       <c r="H25" s="1">
         <v>97727</v>
       </c>
       <c r="I25" s="1">
-        <v>0.2246269174680295</v>
+        <v>0.22462691746802951</v>
       </c>
       <c r="J25" t="s">
-        <v>18</v>
-      </c>
-      <c r="K25">
-        <v>347.0755427182007</v>
+        <v>19</v>
+      </c>
+      <c r="K25" s="7">
+        <v>347.07554271820072</v>
       </c>
       <c r="L25" s="1">
         <v>10298.37387686144</v>
@@ -1715,49 +1825,52 @@
       <c r="M25" s="1">
         <v>99.51298334143236</v>
       </c>
-      <c r="N25" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25">
-        <v>443.014508070235</v>
+      <c r="N25">
+        <v>99.51298334143236</v>
+      </c>
+      <c r="O25" t="s">
+        <v>20</v>
       </c>
       <c r="P25">
-        <v>1329.04352421072</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>443.01450807023502</v>
+      </c>
+      <c r="Q25">
+        <v>1329.0435242107201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" s="4">
-        <v>45690.82291666666</v>
+        <v>45690.822916666657</v>
       </c>
       <c r="D26" s="4">
-        <v>45691.54166666666</v>
+        <v>45691.541666666657</v>
       </c>
       <c r="E26">
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
-        <v>99337.82221928821</v>
+        <v>99337.822219288209</v>
       </c>
       <c r="G26" s="1">
-        <v>96036.73334213537</v>
+        <v>96036.733342135369</v>
       </c>
       <c r="H26" s="1">
-        <v>94564.71000000001</v>
+        <v>94564.71</v>
       </c>
       <c r="I26" s="1">
         <v>0.1247875990027113</v>
       </c>
       <c r="J26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26">
-        <v>492.6414748468634</v>
+        <v>19</v>
+      </c>
+      <c r="K26" s="7">
+        <v>492.64147484686339</v>
       </c>
       <c r="L26" s="1">
         <v>10791.0153517083</v>
@@ -1765,37 +1878,40 @@
       <c r="M26" s="1">
         <v>102.9837387686144</v>
       </c>
-      <c r="N26" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26">
-        <v>825.2722192882065</v>
+      <c r="N26">
+        <v>102.9837387686144</v>
+      </c>
+      <c r="O26" t="s">
+        <v>20</v>
       </c>
       <c r="P26">
-        <v>2475.816657864634</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>825.27221928820654</v>
+      </c>
+      <c r="Q26">
+        <v>2475.8166578646342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4">
-        <v>45691.61111111111</v>
+        <v>45691.611111111109</v>
       </c>
       <c r="D27" s="4">
-        <v>45691.63541666666</v>
+        <v>45691.635416666657</v>
       </c>
       <c r="E27">
         <v>96150.84</v>
       </c>
       <c r="F27" s="1">
-        <v>97150.404590042</v>
+        <v>97150.404590042002</v>
       </c>
       <c r="G27" s="1">
-        <v>93152.14622987396</v>
+        <v>93152.146229873964</v>
       </c>
       <c r="H27" s="1">
         <v>96570</v>
@@ -1804,9 +1920,9 @@
         <v>0.107957159139209</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27">
+        <v>18</v>
+      </c>
+      <c r="K27" s="7">
         <v>-45.25132282479121</v>
       </c>
       <c r="L27" s="1">
@@ -1815,99 +1931,105 @@
       <c r="M27" s="1">
         <v>107.910153517083</v>
       </c>
-      <c r="N27" t="s">
-        <v>19</v>
-      </c>
-      <c r="O27">
-        <v>999.5645900420059</v>
+      <c r="N27">
+        <v>107.910153517083</v>
+      </c>
+      <c r="O27" t="s">
+        <v>20</v>
       </c>
       <c r="P27">
-        <v>2998.693770126032</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>999.56459004200588</v>
+      </c>
+      <c r="Q27">
+        <v>2998.6937701260322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="4">
-        <v>45691.66666666666</v>
+        <v>45691.666666666657</v>
       </c>
       <c r="D28" s="4">
-        <v>45691.78472222222</v>
+        <v>45691.784722222219</v>
       </c>
       <c r="E28">
-        <v>98730.92999999999</v>
+        <v>98730.93</v>
       </c>
       <c r="F28" s="1">
-        <v>99908.6225083747</v>
+        <v>99908.622508374698</v>
       </c>
       <c r="G28" s="1">
-        <v>95197.85247487589</v>
+        <v>95197.852474875894</v>
       </c>
       <c r="H28" s="1">
         <v>99795.94</v>
       </c>
       <c r="I28" s="1">
-        <v>0.09124422506273212</v>
+        <v>9.1244225062732123E-2</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28">
-        <v>-97.17601213406118</v>
+        <v>18</v>
+      </c>
+      <c r="K28" s="7">
+        <v>-97.176012134061182</v>
       </c>
       <c r="L28" s="1">
-        <v>10648.58801674945</v>
+        <v>10648.588016749451</v>
       </c>
       <c r="M28" s="1">
-        <v>107.4576402888351</v>
-      </c>
-      <c r="N28" t="s">
-        <v>19</v>
-      </c>
-      <c r="O28">
-        <v>1177.692508374705</v>
+        <v>107.45764028883509</v>
+      </c>
+      <c r="N28">
+        <v>107.45764028883509</v>
+      </c>
+      <c r="O28" t="s">
+        <v>20</v>
       </c>
       <c r="P28">
-        <v>3533.077525124099</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>1177.6925083747051</v>
+      </c>
+      <c r="Q28">
+        <v>3533.0775251240989</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4">
-        <v>45693.57638888889</v>
+        <v>45693.576388888891</v>
       </c>
       <c r="D29" s="4">
-        <v>45693.61111111111</v>
+        <v>45693.611111111109</v>
       </c>
       <c r="E29">
-        <v>98581.99000000001</v>
+        <v>98581.99</v>
       </c>
       <c r="F29" s="1">
-        <v>98923.60589796901</v>
+        <v>98923.605897969013</v>
       </c>
       <c r="G29" s="1">
-        <v>97557.14230609298</v>
+        <v>97557.142306092981</v>
       </c>
       <c r="H29" s="1">
-        <v>98746.92999999999</v>
+        <v>98746.93</v>
       </c>
       <c r="I29" s="1">
-        <v>0.3117123084744582</v>
+        <v>0.31171230847445819</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29">
-        <v>-51.41382815977332</v>
+        <v>18</v>
+      </c>
+      <c r="K29" s="7">
+        <v>-51.413828159773317</v>
       </c>
       <c r="L29" s="1">
         <v>10597.17418858967</v>
@@ -1915,87 +2037,93 @@
       <c r="M29" s="1">
         <v>106.4858801674945</v>
       </c>
-      <c r="N29" t="s">
-        <v>19</v>
-      </c>
-      <c r="O29">
-        <v>341.6158979690081</v>
+      <c r="N29">
+        <v>106.4858801674945</v>
+      </c>
+      <c r="O29" t="s">
+        <v>20</v>
       </c>
       <c r="P29">
+        <v>341.61589796900807</v>
+      </c>
+      <c r="Q29">
         <v>1024.847693907024</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" s="4">
-        <v>45694.86458333334</v>
+        <v>45694.864583333343</v>
       </c>
       <c r="D30" s="4">
-        <v>45695.54166666666</v>
+        <v>45695.541666666657</v>
       </c>
       <c r="E30">
-        <v>96870.89999999999</v>
+        <v>96870.9</v>
       </c>
       <c r="F30" s="1">
-        <v>97360.8412369147</v>
+        <v>97360.841236914697</v>
       </c>
       <c r="G30" s="1">
-        <v>95401.07628925589</v>
+        <v>95401.076289255885</v>
       </c>
       <c r="H30" s="1">
         <v>97900</v>
       </c>
       <c r="I30" s="1">
-        <v>0.2162948000728218</v>
+        <v>0.21629480007282181</v>
       </c>
       <c r="J30" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30">
-        <v>-222.5889787549422</v>
+        <v>18</v>
+      </c>
+      <c r="K30" s="7">
+        <v>-222.58897875494219</v>
       </c>
       <c r="L30" s="1">
         <v>10374.58520983473</v>
       </c>
       <c r="M30" s="1">
-        <v>105.9717418858967</v>
-      </c>
-      <c r="N30" t="s">
-        <v>19</v>
-      </c>
-      <c r="O30">
-        <v>489.941236914703</v>
+        <v>105.97174188589671</v>
+      </c>
+      <c r="N30">
+        <v>105.97174188589671</v>
+      </c>
+      <c r="O30" t="s">
+        <v>20</v>
       </c>
       <c r="P30">
-        <v>1469.823710744109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>489.94123691470298</v>
+      </c>
+      <c r="Q30">
+        <v>1469.8237107441089</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31" s="4">
-        <v>45696.56944444445</v>
+        <v>45696.569444444453</v>
       </c>
       <c r="D31" s="4">
-        <v>45696.64583333334</v>
+        <v>45696.645833333343</v>
       </c>
       <c r="E31">
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
-        <v>96632.08010532602</v>
+        <v>96632.080105326022</v>
       </c>
       <c r="G31" s="1">
-        <v>95777.07968402194</v>
+        <v>95777.079684021941</v>
       </c>
       <c r="H31" s="1">
         <v>95688</v>
@@ -2004,10 +2132,10 @@
         <v>0.4853604724082356</v>
       </c>
       <c r="J31" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31">
-        <v>354.4733138139076</v>
+        <v>19</v>
+      </c>
+      <c r="K31" s="7">
+        <v>354.47331381390762</v>
       </c>
       <c r="L31" s="1">
         <v>10729.05852364864</v>
@@ -2015,149 +2143,158 @@
       <c r="M31" s="1">
         <v>103.7458520983473</v>
       </c>
-      <c r="N31" t="s">
-        <v>19</v>
-      </c>
-      <c r="O31">
+      <c r="N31">
+        <v>103.7458520983473</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31">
         <v>213.7501053260203</v>
       </c>
-      <c r="P31">
-        <v>641.2503159780608</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31">
+        <v>641.25031597806083</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" s="4">
-        <v>45696.71180555555</v>
+        <v>45696.711805555547</v>
       </c>
       <c r="D32" s="4">
-        <v>45696.77777777778</v>
+        <v>45696.777777777781</v>
       </c>
       <c r="E32">
-        <v>96282.74000000001</v>
+        <v>96282.74</v>
       </c>
       <c r="F32" s="1">
-        <v>96504.35545976873</v>
+        <v>96504.355459768733</v>
       </c>
       <c r="G32" s="1">
-        <v>95617.89362069382</v>
+        <v>95617.893620693823</v>
       </c>
       <c r="H32" s="1">
         <v>96423.03</v>
       </c>
       <c r="I32" s="1">
-        <v>0.4841295158219212</v>
+        <v>0.48412951582192121</v>
       </c>
       <c r="J32" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32">
-        <v>-67.91852977465422</v>
+        <v>18</v>
+      </c>
+      <c r="K32" s="7">
+        <v>-67.918529774654218</v>
       </c>
       <c r="L32" s="1">
-        <v>10661.13999387399</v>
+        <v>10661.139993873991</v>
       </c>
       <c r="M32" s="1">
-        <v>107.2905852364864</v>
-      </c>
-      <c r="N32" t="s">
-        <v>19</v>
-      </c>
-      <c r="O32">
-        <v>221.6154597687273</v>
+        <v>107.29058523648639</v>
+      </c>
+      <c r="N32">
+        <v>107.29058523648639</v>
+      </c>
+      <c r="O32" t="s">
+        <v>20</v>
       </c>
       <c r="P32">
-        <v>664.8463793061819</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>221.61545976872731</v>
+      </c>
+      <c r="Q32">
+        <v>664.84637930618192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="4">
-        <v>45696.80555555555</v>
+        <v>45696.805555555547</v>
       </c>
       <c r="D33" s="4">
-        <v>45697.57291666666</v>
+        <v>45697.572916666657</v>
       </c>
       <c r="E33">
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
-        <v>96814.10035087884</v>
+        <v>96814.100350878842</v>
       </c>
       <c r="G33" s="1">
-        <v>96048.25894736346</v>
+        <v>96048.258947363458</v>
       </c>
       <c r="H33" s="1">
         <v>95915.44</v>
       </c>
       <c r="I33" s="1">
-        <v>0.556832782606799</v>
+        <v>0.55683278260679903</v>
       </c>
       <c r="J33" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33">
-        <v>393.7921438595267</v>
+        <v>19</v>
+      </c>
+      <c r="K33" s="7">
+        <v>393.79214385952667</v>
       </c>
       <c r="L33" s="1">
-        <v>11054.93213773351</v>
+        <v>11054.932137733511</v>
       </c>
       <c r="M33" s="1">
-        <v>106.6113999387399</v>
-      </c>
-      <c r="N33" t="s">
-        <v>19</v>
-      </c>
-      <c r="O33">
-        <v>191.4603508788423</v>
+        <v>106.61139993873989</v>
+      </c>
+      <c r="N33">
+        <v>106.61139993873989</v>
+      </c>
+      <c r="O33" t="s">
+        <v>20</v>
       </c>
       <c r="P33">
-        <v>574.3810526365414</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+        <v>191.46035087884229</v>
+      </c>
+      <c r="Q33">
+        <v>574.38105263654143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" s="4">
-        <v>45697.65277777778</v>
+        <v>45697.652777777781</v>
       </c>
       <c r="D34" s="4">
-        <v>45697.89930555555</v>
+        <v>45697.899305555547</v>
       </c>
       <c r="E34">
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
-        <v>96880.50705339119</v>
+        <v>96880.507053391193</v>
       </c>
       <c r="G34" s="1">
-        <v>95806.67883982643</v>
+        <v>95806.678839826433</v>
       </c>
       <c r="H34" s="1">
-        <v>95376.64999999999</v>
+        <v>95376.65</v>
       </c>
       <c r="I34" s="1">
-        <v>0.4117951828080482</v>
+        <v>0.41179518280804822</v>
       </c>
       <c r="J34" t="s">
-        <v>18</v>
-      </c>
-      <c r="K34">
-        <v>508.7317688410664</v>
+        <v>19</v>
+      </c>
+      <c r="K34" s="7">
+        <v>508.73176884106641</v>
       </c>
       <c r="L34" s="1">
         <v>11563.66390657458</v>
@@ -2165,34 +2302,37 @@
       <c r="M34" s="1">
         <v>110.5493213773351</v>
       </c>
-      <c r="N34" t="s">
-        <v>19</v>
-      </c>
-      <c r="O34">
-        <v>268.4570533911901</v>
+      <c r="N34">
+        <v>110.5493213773351</v>
+      </c>
+      <c r="O34" t="s">
+        <v>20</v>
       </c>
       <c r="P34">
-        <v>805.3711601735704</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>268.45705339119007</v>
+      </c>
+      <c r="Q34">
+        <v>805.37116017357039</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" s="4">
-        <v>45699.88888888889</v>
+        <v>45699.888888888891</v>
       </c>
       <c r="D35" s="4">
-        <v>45699.89930555555</v>
+        <v>45699.899305555547</v>
       </c>
       <c r="E35">
         <v>95686.37</v>
       </c>
       <c r="F35" s="1">
-        <v>96056.14374028651</v>
+        <v>96056.143740286512</v>
       </c>
       <c r="G35" s="1">
         <v>94577.04877914043</v>
@@ -2201,13 +2341,13 @@
         <v>95959.38</v>
       </c>
       <c r="I35" s="1">
-        <v>0.3127226908437182</v>
+        <v>0.31272269084371818</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35">
-        <v>-85.37642182724643</v>
+        <v>18</v>
+      </c>
+      <c r="K35" s="7">
+        <v>-85.376421827246432</v>
       </c>
       <c r="L35" s="1">
         <v>11478.28748474733</v>
@@ -2215,22 +2355,25 @@
       <c r="M35" s="1">
         <v>115.6366390657458</v>
       </c>
-      <c r="N35" t="s">
-        <v>19</v>
-      </c>
-      <c r="O35">
-        <v>369.7737402865168</v>
+      <c r="N35">
+        <v>115.6366390657458</v>
+      </c>
+      <c r="O35" t="s">
+        <v>20</v>
       </c>
       <c r="P35">
-        <v>1109.321220859565</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+        <v>369.77374028651678</v>
+      </c>
+      <c r="Q35">
+        <v>1109.3212208595651</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="4">
         <v>45699.90625</v>
@@ -2242,72 +2385,75 @@
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
-        <v>96720.53183445179</v>
+        <v>96720.531834451787</v>
       </c>
       <c r="G36" s="1">
-        <v>95109.08449664462</v>
+        <v>95109.084496644617</v>
       </c>
       <c r="H36" s="1">
-        <v>94844.8</v>
+        <v>94844.800000000003</v>
       </c>
       <c r="I36" s="1">
-        <v>0.2849187116562403</v>
+        <v>0.28491871165624028</v>
       </c>
       <c r="J36" t="s">
-        <v>18</v>
-      </c>
-      <c r="K36">
-        <v>419.6482228371254</v>
+        <v>19</v>
+      </c>
+      <c r="K36" s="7">
+        <v>419.64822283712539</v>
       </c>
       <c r="L36" s="1">
         <v>11897.93570758446</v>
       </c>
       <c r="M36" s="1">
-        <v>114.7828748474733</v>
-      </c>
-      <c r="N36" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36">
-        <v>402.861834451789</v>
+        <v>114.78287484747329</v>
+      </c>
+      <c r="N36">
+        <v>114.78287484747329</v>
+      </c>
+      <c r="O36" t="s">
+        <v>20</v>
       </c>
       <c r="P36">
-        <v>1208.585503355382</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+        <v>402.86183445178898</v>
+      </c>
+      <c r="Q36">
+        <v>1208.5855033553819</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37" s="4">
-        <v>45701.79861111111</v>
+        <v>45701.798611111109</v>
       </c>
       <c r="D37" s="4">
-        <v>45701.89583333334</v>
+        <v>45701.895833333343</v>
       </c>
       <c r="E37">
         <v>96270.05</v>
       </c>
       <c r="F37" s="1">
-        <v>96701.70211287875</v>
+        <v>96701.702112878746</v>
       </c>
       <c r="G37" s="1">
         <v>94975.09366136376</v>
       </c>
       <c r="H37" s="1">
-        <v>96412.78999999999</v>
+        <v>96412.79</v>
       </c>
       <c r="I37" s="1">
-        <v>0.2756371474295727</v>
+        <v>0.27563714742957268</v>
       </c>
       <c r="J37" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37">
-        <v>-39.34444642409465</v>
+        <v>18</v>
+      </c>
+      <c r="K37" s="7">
+        <v>-39.344446424094649</v>
       </c>
       <c r="L37" s="1">
         <v>11858.59126116036</v>
@@ -2315,58 +2461,61 @@
       <c r="M37" s="1">
         <v>118.9793570758446</v>
       </c>
-      <c r="N37" t="s">
-        <v>19</v>
-      </c>
-      <c r="O37">
-        <v>431.6521128787426</v>
+      <c r="N37">
+        <v>118.9793570758446</v>
+      </c>
+      <c r="O37" t="s">
+        <v>20</v>
       </c>
       <c r="P37">
+        <v>431.65211287874263</v>
+      </c>
+      <c r="Q37">
         <v>1294.956338636242</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
-      <c r="A41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B42" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+        <v>11858.59126116036</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1">
-        <v>11858.59126116036</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+        <v>24</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0.18585912611603631</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0.1858591261160363</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="5">
+        <v>26</v>
+      </c>
+      <c r="B45" s="5">
         <v>0.3611111111111111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PnL fix and code refactor xlsx
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -493,26 +493,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
+    <col min="6" max="9" width="15.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
     <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -526,7 +525,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -579,7 +578,7 @@
       <c r="D2" s="4">
         <v>45666.645833333343</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>93188.2</v>
       </c>
       <c r="F2" s="1">
@@ -589,7 +588,7 @@
         <v>91348.750085215084</v>
       </c>
       <c r="H2" s="1">
-        <v>93452</v>
+        <v>93915.9</v>
       </c>
       <c r="I2" s="1">
         <v>0.16309223621077859</v>
@@ -598,10 +597,10 @@
         <v>18</v>
       </c>
       <c r="K2" s="7">
-        <v>-43.023731912403868</v>
+        <v>-100</v>
       </c>
       <c r="L2" s="1">
-        <v>9956.9762680875956</v>
+        <v>9900</v>
       </c>
       <c r="M2" s="1">
         <v>100</v>
@@ -632,7 +631,7 @@
       <c r="D3" s="4">
         <v>45666.659722222219</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>93739.87</v>
       </c>
       <c r="F3" s="1">
@@ -642,25 +641,25 @@
         <v>91830.553378379525</v>
       </c>
       <c r="H3" s="1">
-        <v>94100.49</v>
+        <v>94588.23</v>
       </c>
       <c r="I3" s="1">
-        <v>0.15644827298947961</v>
+        <v>0.15555303747784549</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
       </c>
       <c r="K3" s="7">
-        <v>-56.418376205467673</v>
+        <v>-99</v>
       </c>
       <c r="L3" s="1">
-        <v>9900.5578918821284</v>
+        <v>9801</v>
       </c>
       <c r="M3" s="1">
-        <v>99.569762680875954</v>
+        <v>99</v>
       </c>
       <c r="N3">
-        <v>99.569762680875954</v>
+        <v>99</v>
       </c>
       <c r="O3" t="s">
         <v>20</v>
@@ -685,7 +684,7 @@
       <c r="D4" s="4">
         <v>45666.822916666657</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
@@ -698,22 +697,22 @@
         <v>92106.85</v>
       </c>
       <c r="I4" s="1">
-        <v>0.14649616279484851</v>
+        <v>0.14502302872544071</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="7">
-        <v>313.08720424026609</v>
+        <v>309.93886630114969</v>
       </c>
       <c r="L4" s="1">
-        <v>10213.645096122391</v>
+        <v>10110.93886630115</v>
       </c>
       <c r="M4" s="1">
-        <v>99.005578918821286</v>
+        <v>98.01</v>
       </c>
       <c r="N4">
-        <v>99.005578918821286</v>
+        <v>98.01</v>
       </c>
       <c r="O4" t="s">
         <v>20</v>
@@ -738,7 +737,7 @@
       <c r="D5" s="4">
         <v>45670.541666666657</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
@@ -751,22 +750,22 @@
         <v>90583.24</v>
       </c>
       <c r="I5" s="1">
-        <v>0.1227647426767863</v>
+        <v>0.12153024669061829</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="7">
-        <v>601.97568806819379</v>
+        <v>595.92234934497867</v>
       </c>
       <c r="L5" s="1">
-        <v>10815.620784190591</v>
+        <v>10706.861215646129</v>
       </c>
       <c r="M5" s="1">
-        <v>102.1364509612239</v>
+        <v>101.1093886630115</v>
       </c>
       <c r="N5">
-        <v>102.1364509612239</v>
+        <v>101.1093886630115</v>
       </c>
       <c r="O5" t="s">
         <v>20</v>
@@ -791,7 +790,7 @@
       <c r="D6" s="4">
         <v>45670.868055555547</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="7">
         <v>92680.01</v>
       </c>
       <c r="F6" s="1">
@@ -801,25 +800,25 @@
         <v>89502.452628572224</v>
       </c>
       <c r="H6" s="1">
-        <v>93228.99</v>
+        <v>93783.12</v>
       </c>
       <c r="I6" s="1">
-        <v>0.10211259329046329</v>
+        <v>0.1010857708998836</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
       </c>
       <c r="K6" s="7">
-        <v>-56.057771464599632</v>
+        <v>-107.0686121564613</v>
       </c>
       <c r="L6" s="1">
-        <v>10759.56301272599</v>
+        <v>10599.79260348967</v>
       </c>
       <c r="M6" s="1">
-        <v>108.1562078419059</v>
+        <v>107.0686121564613</v>
       </c>
       <c r="N6">
-        <v>108.1562078419059</v>
+        <v>107.0686121564613</v>
       </c>
       <c r="O6" t="s">
         <v>20</v>
@@ -844,7 +843,7 @@
       <c r="D7" s="4">
         <v>45673.670138888891</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="7">
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
@@ -857,22 +856,22 @@
         <v>99815.27</v>
       </c>
       <c r="I7" s="1">
-        <v>0.15739933671226791</v>
+        <v>0.15506208970601851</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="7">
-        <v>353.21040755579878</v>
+        <v>347.96553178389507</v>
       </c>
       <c r="L7" s="1">
-        <v>11112.77342028179</v>
+        <v>10947.75813527356</v>
       </c>
       <c r="M7" s="1">
-        <v>107.59563012725989</v>
+        <v>105.99792603489669</v>
       </c>
       <c r="N7">
-        <v>107.59563012725989</v>
+        <v>105.99792603489669</v>
       </c>
       <c r="O7" t="s">
         <v>20</v>
@@ -897,7 +896,7 @@
       <c r="D8" s="4">
         <v>45675.541666666657</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7">
         <v>104692.7</v>
       </c>
       <c r="F8" s="1">
@@ -910,22 +909,22 @@
         <v>103424.59</v>
       </c>
       <c r="I8" s="1">
-        <v>0.22425266228726379</v>
+        <v>0.2209226999473812</v>
       </c>
       <c r="J8" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="7">
-        <v>-284.37704357310218</v>
+        <v>-109.4775813527356</v>
       </c>
       <c r="L8" s="1">
-        <v>10828.39637670869</v>
+        <v>10838.280553920829</v>
       </c>
       <c r="M8" s="1">
-        <v>111.1277342028179</v>
+        <v>109.4775813527356</v>
       </c>
       <c r="N8">
-        <v>111.1277342028179</v>
+        <v>109.4775813527356</v>
       </c>
       <c r="O8" t="s">
         <v>20</v>
@@ -950,7 +949,7 @@
       <c r="D9" s="4">
         <v>45676.541666666657</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="7">
         <v>103240.85</v>
       </c>
       <c r="F9" s="1">
@@ -963,22 +962,22 @@
         <v>105157.8</v>
       </c>
       <c r="I9" s="1">
-        <v>0.1961684575986099</v>
+        <v>0.19634752047467049</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="7">
-        <v>376.04512479365468</v>
+        <v>376.38837937391901</v>
       </c>
       <c r="L9" s="1">
-        <v>11204.441501502341</v>
+        <v>11214.66893329475</v>
       </c>
       <c r="M9" s="1">
-        <v>108.2839637670869</v>
+        <v>108.38280553920831</v>
       </c>
       <c r="N9">
-        <v>108.2839637670869</v>
+        <v>108.38280553920831</v>
       </c>
       <c r="O9" t="s">
         <v>20</v>
@@ -1003,7 +1002,7 @@
       <c r="D10" s="4">
         <v>45677.673611111109</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <v>105535.7</v>
       </c>
       <c r="F10" s="1">
@@ -1016,22 +1015,22 @@
         <v>103708</v>
       </c>
       <c r="I10" s="1">
-        <v>0.1010730610061438</v>
+        <v>0.10116532065490461</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="7">
-        <v>-184.7312336009287</v>
+        <v>-112.1466893329475</v>
       </c>
       <c r="L10" s="1">
-        <v>11019.71026790141</v>
+        <v>11102.522243961799</v>
       </c>
       <c r="M10" s="1">
-        <v>112.0444150150234</v>
+        <v>112.1466893329475</v>
       </c>
       <c r="N10">
-        <v>112.0444150150234</v>
+        <v>112.1466893329475</v>
       </c>
       <c r="O10" t="s">
         <v>20</v>
@@ -1056,7 +1055,7 @@
       <c r="D11" s="4">
         <v>45678.673611111109</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="7">
         <v>103281.22</v>
       </c>
       <c r="F11" s="1">
@@ -1069,22 +1068,22 @@
         <v>106300</v>
       </c>
       <c r="I11" s="1">
-        <v>0.1152930814464031</v>
+        <v>0.1161594969572064</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="7">
-        <v>348.04444840877261</v>
+        <v>350.65996622447528</v>
       </c>
       <c r="L11" s="1">
-        <v>11367.754716310181</v>
+        <v>11453.182210186271</v>
       </c>
       <c r="M11" s="1">
-        <v>110.19710267901409</v>
+        <v>111.02522243961801</v>
       </c>
       <c r="N11">
-        <v>110.19710267901409</v>
+        <v>111.02522243961801</v>
       </c>
       <c r="O11" t="s">
         <v>20</v>
@@ -1109,7 +1108,7 @@
       <c r="D12" s="4">
         <v>45679.541666666657</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <v>106072</v>
       </c>
       <c r="F12" s="1">
@@ -1122,22 +1121,22 @@
         <v>105039.74</v>
       </c>
       <c r="I12" s="1">
-        <v>0.16694659341698481</v>
+        <v>0.16820117969568951</v>
       </c>
       <c r="J12" t="s">
         <v>18</v>
       </c>
       <c r="K12" s="7">
-        <v>-172.3322905206158</v>
+        <v>-114.5318221018627</v>
       </c>
       <c r="L12" s="1">
-        <v>11195.422425789569</v>
+        <v>11338.65038808441</v>
       </c>
       <c r="M12" s="1">
-        <v>113.67754716310181</v>
+        <v>114.5318221018627</v>
       </c>
       <c r="N12">
-        <v>113.67754716310181</v>
+        <v>114.5318221018627</v>
       </c>
       <c r="O12" t="s">
         <v>20</v>
@@ -1162,7 +1161,7 @@
       <c r="D13" s="4">
         <v>45679.565972222219</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="7">
         <v>104947.17</v>
       </c>
       <c r="F13" s="1">
@@ -1175,22 +1174,22 @@
         <v>104283.67</v>
       </c>
       <c r="I13" s="1">
-        <v>0.36267434364960688</v>
+        <v>0.36731419601443532</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="7">
-        <v>-240.63442701151419</v>
+        <v>-113.3865038808441</v>
       </c>
       <c r="L13" s="1">
-        <v>10954.787998778051</v>
+        <v>11225.26388420357</v>
       </c>
       <c r="M13" s="1">
-        <v>111.9542242578957</v>
+        <v>113.3865038808441</v>
       </c>
       <c r="N13">
-        <v>111.9542242578957</v>
+        <v>113.3865038808441</v>
       </c>
       <c r="O13" t="s">
         <v>20</v>
@@ -1215,7 +1214,7 @@
       <c r="D14" s="4">
         <v>45679.694444444453</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <v>104073.94</v>
       </c>
       <c r="F14" s="1">
@@ -1228,22 +1227,22 @@
         <v>103339.12</v>
       </c>
       <c r="I14" s="1">
-        <v>0.23502691926082819</v>
+        <v>0.24082978044746139</v>
       </c>
       <c r="J14" t="s">
         <v>18</v>
       </c>
       <c r="K14" s="7">
-        <v>-172.70248081124339</v>
+        <v>-112.25263884203569</v>
       </c>
       <c r="L14" s="1">
-        <v>10782.085517966811</v>
+        <v>11113.011245361529</v>
       </c>
       <c r="M14" s="1">
-        <v>109.5478799877805</v>
+        <v>112.25263884203569</v>
       </c>
       <c r="N14">
-        <v>109.5478799877805</v>
+        <v>112.25263884203569</v>
       </c>
       <c r="O14" t="s">
         <v>20</v>
@@ -1268,7 +1267,7 @@
       <c r="D15" s="4">
         <v>45680.541666666657</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="7">
         <v>103891.76</v>
       </c>
       <c r="F15" s="1">
@@ -1281,22 +1280,22 @@
         <v>101592.48</v>
       </c>
       <c r="I15" s="1">
-        <v>0.21213591568689311</v>
+        <v>0.21864682974783711</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="7">
-        <v>-487.75986822055938</v>
+        <v>-111.1301124536153</v>
       </c>
       <c r="L15" s="1">
-        <v>10294.32564974625</v>
+        <v>11001.88113290792</v>
       </c>
       <c r="M15" s="1">
-        <v>107.8208551796681</v>
+        <v>111.1301124536153</v>
       </c>
       <c r="N15">
-        <v>107.8208551796681</v>
+        <v>111.1301124536153</v>
       </c>
       <c r="O15" t="s">
         <v>20</v>
@@ -1321,7 +1320,7 @@
       <c r="D16" s="4">
         <v>45680.850694444453</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="7">
         <v>103770.04</v>
       </c>
       <c r="F16" s="1">
@@ -1334,22 +1333,22 @@
         <v>106421.03</v>
       </c>
       <c r="I16" s="1">
-        <v>0.1191027928070732</v>
+        <v>0.12728903413824669</v>
       </c>
       <c r="J16" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="7">
-        <v>315.7403127036236</v>
+        <v>337.44195661015141</v>
       </c>
       <c r="L16" s="1">
-        <v>10610.065962449869</v>
+        <v>11339.32308951807</v>
       </c>
       <c r="M16" s="1">
-        <v>102.9432564974625</v>
+        <v>110.0188113290792</v>
       </c>
       <c r="N16">
-        <v>102.9432564974625</v>
+        <v>110.0188113290792</v>
       </c>
       <c r="O16" t="s">
         <v>20</v>
@@ -1374,7 +1373,7 @@
       <c r="D17" s="4">
         <v>45681.847222222219</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="7">
         <v>105760.94</v>
       </c>
       <c r="F17" s="1">
@@ -1387,22 +1386,22 @@
         <v>105291.54</v>
       </c>
       <c r="I17" s="1">
-        <v>0.22742242852035471</v>
+        <v>0.24305375705691459</v>
       </c>
       <c r="J17" t="s">
         <v>18</v>
       </c>
       <c r="K17" s="7">
-        <v>-106.7520879474565</v>
+        <v>-113.39323089518069</v>
       </c>
       <c r="L17" s="1">
-        <v>10503.313874502421</v>
+        <v>11225.929858622891</v>
       </c>
       <c r="M17" s="1">
-        <v>106.1006596244987</v>
+        <v>113.39323089518069</v>
       </c>
       <c r="N17">
-        <v>106.1006596244987</v>
+        <v>113.39323089518069</v>
       </c>
       <c r="O17" t="s">
         <v>20</v>
@@ -1427,7 +1426,7 @@
       <c r="D18" s="4">
         <v>45682.586805555547</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="7">
         <v>105052.52</v>
       </c>
       <c r="F18" s="1">
@@ -1440,22 +1439,22 @@
         <v>104541.68</v>
       </c>
       <c r="I18" s="1">
-        <v>0.2274897570837339</v>
+        <v>0.24314079223859611</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="7">
-        <v>-116.2108675086571</v>
+        <v>-112.25929858622889</v>
       </c>
       <c r="L18" s="1">
-        <v>10387.103006993761</v>
+        <v>11113.67056003666</v>
       </c>
       <c r="M18" s="1">
-        <v>105.0331387450242</v>
+        <v>112.25929858622889</v>
       </c>
       <c r="N18">
-        <v>105.0331387450242</v>
+        <v>112.25929858622889</v>
       </c>
       <c r="O18" t="s">
         <v>20</v>
@@ -1480,7 +1479,7 @@
       <c r="D19" s="4">
         <v>45683.90625</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="7">
         <v>104795.54</v>
       </c>
       <c r="F19" s="1">
@@ -1493,22 +1492,22 @@
         <v>104552.48</v>
       </c>
       <c r="I19" s="1">
-        <v>0.64908307366157403</v>
+        <v>0.69448579088064044</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
       </c>
       <c r="K19" s="7">
-        <v>-157.76613188418071</v>
+        <v>-111.1367056003666</v>
       </c>
       <c r="L19" s="1">
-        <v>10229.33687510958</v>
+        <v>11002.533854436289</v>
       </c>
       <c r="M19" s="1">
-        <v>103.8710300699376</v>
+        <v>111.1367056003666</v>
       </c>
       <c r="N19">
-        <v>103.8710300699376</v>
+        <v>111.1367056003666</v>
       </c>
       <c r="O19" t="s">
         <v>20</v>
@@ -1533,7 +1532,7 @@
       <c r="D20" s="4">
         <v>45684.545138888891</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="7">
         <v>100632.01</v>
       </c>
       <c r="F20" s="1">
@@ -1543,25 +1542,25 @@
         <v>98669.765465459277</v>
       </c>
       <c r="H20" s="1">
-        <v>100622.87</v>
+        <v>101360.94</v>
       </c>
       <c r="I20" s="1">
-        <v>0.15639238680571149</v>
+        <v>0.16821349725932291</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
       </c>
       <c r="K20" s="7">
-        <v>1.4294264154041121</v>
+        <v>-110.0253385443629</v>
       </c>
       <c r="L20" s="1">
-        <v>10230.766301524989</v>
+        <v>10892.50851589193</v>
       </c>
       <c r="M20" s="1">
-        <v>102.2933687510958</v>
+        <v>110.0253385443629</v>
       </c>
       <c r="N20">
-        <v>102.2933687510958</v>
+        <v>110.0253385443629</v>
       </c>
       <c r="O20" t="s">
         <v>20</v>
@@ -1586,7 +1585,7 @@
       <c r="D21" s="4">
         <v>45684.864583333343</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="7">
         <v>100351.67999999999</v>
       </c>
       <c r="F21" s="1">
@@ -1596,25 +1595,25 @@
         <v>98531.898140814548</v>
       </c>
       <c r="H21" s="1">
-        <v>100932.23</v>
+        <v>101356.8</v>
       </c>
       <c r="I21" s="1">
-        <v>0.16865922005790809</v>
+        <v>0.17956836630024639</v>
       </c>
       <c r="J21" t="s">
         <v>18</v>
       </c>
       <c r="K21" s="7">
-        <v>-97.915110204619054</v>
+        <v>-108.9250851589193</v>
       </c>
       <c r="L21" s="1">
-        <v>10132.851191320369</v>
+        <v>10783.58343073301</v>
       </c>
       <c r="M21" s="1">
-        <v>102.3076630152499</v>
+        <v>108.9250851589193</v>
       </c>
       <c r="N21">
-        <v>102.3076630152499</v>
+        <v>108.9250851589193</v>
       </c>
       <c r="O21" t="s">
         <v>20</v>
@@ -1639,7 +1638,7 @@
       <c r="D22" s="4">
         <v>45684.878472222219</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="7">
         <v>101386.5</v>
       </c>
       <c r="F22" s="1">
@@ -1649,25 +1648,25 @@
         <v>99403.547902965991</v>
       </c>
       <c r="H22" s="1">
-        <v>101604</v>
+        <v>102221.99</v>
       </c>
       <c r="I22" s="1">
-        <v>0.1532994852443969</v>
+        <v>0.16314438629449249</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="7">
-        <v>-33.342638040656333</v>
+        <v>-107.8358343073301</v>
       </c>
       <c r="L22" s="1">
-        <v>10099.508553279709</v>
+        <v>10675.747596425679</v>
       </c>
       <c r="M22" s="1">
-        <v>101.3285119132037</v>
+        <v>107.8358343073301</v>
       </c>
       <c r="N22">
-        <v>101.3285119132037</v>
+        <v>107.8358343073301</v>
       </c>
       <c r="O22" t="s">
         <v>20</v>
@@ -1692,7 +1691,7 @@
       <c r="D23" s="4">
         <v>45685.625</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="7">
         <v>102295.12</v>
       </c>
       <c r="F23" s="1">
@@ -1702,25 +1701,25 @@
         <v>100153.4333173529</v>
       </c>
       <c r="H23" s="1">
-        <v>102625.01</v>
+        <v>103315.79</v>
       </c>
       <c r="I23" s="1">
-        <v>0.14147039296331701</v>
+        <v>0.14954214847940031</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
       </c>
       <c r="K23" s="7">
-        <v>-46.66966793466856</v>
+        <v>-106.7574759642568</v>
       </c>
       <c r="L23" s="1">
-        <v>10052.83888534504</v>
+        <v>10568.99012046142</v>
       </c>
       <c r="M23" s="1">
-        <v>100.99508553279711</v>
+        <v>106.7574759642568</v>
       </c>
       <c r="N23">
-        <v>100.99508553279711</v>
+        <v>106.7574759642568</v>
       </c>
       <c r="O23" t="s">
         <v>20</v>
@@ -1745,7 +1744,7 @@
       <c r="D24" s="4">
         <v>45688.565972222219</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="7">
         <v>105018.14</v>
       </c>
       <c r="F24" s="1">
@@ -1758,22 +1757,22 @@
         <v>104551.09</v>
       </c>
       <c r="I24" s="1">
-        <v>0.21740831003491171</v>
+        <v>0.22857088500790479</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
       </c>
       <c r="K24" s="7">
-        <v>-101.5405512018061</v>
+        <v>-105.6899012046142</v>
       </c>
       <c r="L24" s="1">
-        <v>9951.2983341432355</v>
+        <v>10463.300219256809</v>
       </c>
       <c r="M24" s="1">
-        <v>100.52838885345039</v>
+        <v>105.6899012046142</v>
       </c>
       <c r="N24">
-        <v>100.52838885345039</v>
+        <v>105.6899012046142</v>
       </c>
       <c r="O24" t="s">
         <v>20</v>
@@ -1798,7 +1797,7 @@
       <c r="D25" s="4">
         <v>45690.722222222219</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="7">
         <v>99272.12</v>
       </c>
       <c r="F25" s="1">
@@ -1811,22 +1810,22 @@
         <v>97727</v>
       </c>
       <c r="I25" s="1">
-        <v>0.22462691746802951</v>
+        <v>0.2361841436036666</v>
       </c>
       <c r="J25" t="s">
         <v>19</v>
       </c>
       <c r="K25" s="7">
-        <v>347.07554271820072</v>
+        <v>364.93284396489622</v>
       </c>
       <c r="L25" s="1">
-        <v>10298.37387686144</v>
+        <v>10828.233063221711</v>
       </c>
       <c r="M25" s="1">
-        <v>99.51298334143236</v>
+        <v>104.6330021925681</v>
       </c>
       <c r="N25">
-        <v>99.51298334143236</v>
+        <v>104.6330021925681</v>
       </c>
       <c r="O25" t="s">
         <v>20</v>
@@ -1851,7 +1850,7 @@
       <c r="D26" s="4">
         <v>45691.541666666657</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="7">
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
@@ -1864,22 +1863,22 @@
         <v>94564.71</v>
       </c>
       <c r="I26" s="1">
-        <v>0.1247875990027113</v>
+        <v>0.13120801609632521</v>
       </c>
       <c r="J26" t="s">
         <v>19</v>
       </c>
       <c r="K26" s="7">
-        <v>492.64147484686339</v>
+        <v>517.98825426571614</v>
       </c>
       <c r="L26" s="1">
-        <v>10791.0153517083</v>
+        <v>11346.22131748742</v>
       </c>
       <c r="M26" s="1">
-        <v>102.9837387686144</v>
+        <v>108.2823306322171</v>
       </c>
       <c r="N26">
-        <v>102.9837387686144</v>
+        <v>108.2823306322171</v>
       </c>
       <c r="O26" t="s">
         <v>20</v>
@@ -1904,7 +1903,7 @@
       <c r="D27" s="4">
         <v>45691.635416666657</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="7">
         <v>96150.84</v>
       </c>
       <c r="F27" s="1">
@@ -1914,25 +1913,25 @@
         <v>93152.146229873964</v>
       </c>
       <c r="H27" s="1">
-        <v>96570</v>
+        <v>97200</v>
       </c>
       <c r="I27" s="1">
-        <v>0.107957159139209</v>
+        <v>0.1135116372720907</v>
       </c>
       <c r="J27" t="s">
         <v>18</v>
       </c>
       <c r="K27" s="7">
-        <v>-45.25132282479121</v>
+        <v>-113.46221317487419</v>
       </c>
       <c r="L27" s="1">
-        <v>10745.76402888351</v>
+        <v>11232.75910431255</v>
       </c>
       <c r="M27" s="1">
-        <v>107.910153517083</v>
+        <v>113.46221317487419</v>
       </c>
       <c r="N27">
-        <v>107.910153517083</v>
+        <v>113.46221317487419</v>
       </c>
       <c r="O27" t="s">
         <v>20</v>
@@ -1957,7 +1956,7 @@
       <c r="D28" s="4">
         <v>45691.784722222219</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="7">
         <v>98730.93</v>
       </c>
       <c r="F28" s="1">
@@ -1967,25 +1966,25 @@
         <v>95197.852474875894</v>
       </c>
       <c r="H28" s="1">
-        <v>99795.94</v>
+        <v>99943.63</v>
       </c>
       <c r="I28" s="1">
-        <v>9.1244225062732123E-2</v>
+        <v>9.5379388290535314E-2</v>
       </c>
       <c r="J28" t="s">
         <v>18</v>
       </c>
       <c r="K28" s="7">
-        <v>-97.176012134061182</v>
+        <v>-112.32759104312549</v>
       </c>
       <c r="L28" s="1">
-        <v>10648.588016749451</v>
+        <v>11120.431513269419</v>
       </c>
       <c r="M28" s="1">
-        <v>107.45764028883509</v>
+        <v>112.32759104312549</v>
       </c>
       <c r="N28">
-        <v>107.45764028883509</v>
+        <v>112.32759104312549</v>
       </c>
       <c r="O28" t="s">
         <v>20</v>
@@ -2010,7 +2009,7 @@
       <c r="D29" s="4">
         <v>45693.611111111109</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="7">
         <v>98581.99</v>
       </c>
       <c r="F29" s="1">
@@ -2020,25 +2019,25 @@
         <v>97557.142306092981</v>
       </c>
       <c r="H29" s="1">
-        <v>98746.93</v>
+        <v>99149</v>
       </c>
       <c r="I29" s="1">
-        <v>0.31171230847445819</v>
+        <v>0.32552441439005519</v>
       </c>
       <c r="J29" t="s">
         <v>18</v>
       </c>
       <c r="K29" s="7">
-        <v>-51.413828159773317</v>
+        <v>-111.20431513269421</v>
       </c>
       <c r="L29" s="1">
-        <v>10597.17418858967</v>
+        <v>11009.22719813673</v>
       </c>
       <c r="M29" s="1">
-        <v>106.4858801674945</v>
+        <v>111.20431513269421</v>
       </c>
       <c r="N29">
-        <v>106.4858801674945</v>
+        <v>111.20431513269421</v>
       </c>
       <c r="O29" t="s">
         <v>20</v>
@@ -2063,7 +2062,7 @@
       <c r="D30" s="4">
         <v>45695.541666666657</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="7">
         <v>96870.9</v>
       </c>
       <c r="F30" s="1">
@@ -2073,25 +2072,25 @@
         <v>95401.076289255885</v>
       </c>
       <c r="H30" s="1">
-        <v>97900</v>
+        <v>98007</v>
       </c>
       <c r="I30" s="1">
-        <v>0.21629480007282181</v>
+        <v>0.22470505376246569</v>
       </c>
       <c r="J30" t="s">
         <v>18</v>
       </c>
       <c r="K30" s="7">
-        <v>-222.58897875494219</v>
+        <v>-110.0922719813673</v>
       </c>
       <c r="L30" s="1">
-        <v>10374.58520983473</v>
+        <v>10899.134926155361</v>
       </c>
       <c r="M30" s="1">
-        <v>105.97174188589671</v>
+        <v>110.0922719813673</v>
       </c>
       <c r="N30">
-        <v>105.97174188589671</v>
+        <v>110.0922719813673</v>
       </c>
       <c r="O30" t="s">
         <v>20</v>
@@ -2116,7 +2115,7 @@
       <c r="D31" s="4">
         <v>45696.645833333343</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="7">
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
@@ -2129,22 +2128,22 @@
         <v>95688</v>
       </c>
       <c r="I31" s="1">
-        <v>0.4853604724082356</v>
+        <v>0.5099007979215523</v>
       </c>
       <c r="J31" t="s">
         <v>19</v>
       </c>
       <c r="K31" s="7">
-        <v>354.47331381390762</v>
+        <v>372.39584974604821</v>
       </c>
       <c r="L31" s="1">
-        <v>10729.05852364864</v>
+        <v>11271.53077590141</v>
       </c>
       <c r="M31" s="1">
-        <v>103.7458520983473</v>
+        <v>108.99134926155359</v>
       </c>
       <c r="N31">
-        <v>103.7458520983473</v>
+        <v>108.99134926155359</v>
       </c>
       <c r="O31" t="s">
         <v>20</v>
@@ -2169,7 +2168,7 @@
       <c r="D32" s="4">
         <v>45696.777777777781</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="7">
         <v>96282.74</v>
       </c>
       <c r="F32" s="1">
@@ -2179,25 +2178,25 @@
         <v>95617.893620693823</v>
       </c>
       <c r="H32" s="1">
-        <v>96423.03</v>
+        <v>96526.59</v>
       </c>
       <c r="I32" s="1">
-        <v>0.48412951582192121</v>
+        <v>0.50860760290207696</v>
       </c>
       <c r="J32" t="s">
         <v>18</v>
       </c>
       <c r="K32" s="7">
-        <v>-67.918529774654218</v>
+        <v>-112.7153077590141</v>
       </c>
       <c r="L32" s="1">
-        <v>10661.139993873991</v>
+        <v>11158.815468142389</v>
       </c>
       <c r="M32" s="1">
-        <v>107.29058523648639</v>
+        <v>112.7153077590141</v>
       </c>
       <c r="N32">
-        <v>107.29058523648639</v>
+        <v>112.7153077590141</v>
       </c>
       <c r="O32" t="s">
         <v>20</v>
@@ -2222,7 +2221,7 @@
       <c r="D33" s="4">
         <v>45697.572916666657</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="7">
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
@@ -2235,22 +2234,22 @@
         <v>95915.44</v>
       </c>
       <c r="I33" s="1">
-        <v>0.55683278260679903</v>
+        <v>0.58282643988278204</v>
       </c>
       <c r="J33" t="s">
         <v>19</v>
       </c>
       <c r="K33" s="7">
-        <v>393.79214385952667</v>
+        <v>412.17485828510178</v>
       </c>
       <c r="L33" s="1">
-        <v>11054.932137733511</v>
+        <v>11570.990326427491</v>
       </c>
       <c r="M33" s="1">
-        <v>106.61139993873989</v>
+        <v>111.5881546814239</v>
       </c>
       <c r="N33">
-        <v>106.61139993873989</v>
+        <v>111.5881546814239</v>
       </c>
       <c r="O33" t="s">
         <v>20</v>
@@ -2275,7 +2274,7 @@
       <c r="D34" s="4">
         <v>45697.899305555547</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="7">
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
@@ -2288,22 +2287,22 @@
         <v>95376.65</v>
       </c>
       <c r="I34" s="1">
-        <v>0.41179518280804822</v>
+        <v>0.43101830182001161</v>
       </c>
       <c r="J34" t="s">
         <v>19</v>
       </c>
       <c r="K34" s="7">
-        <v>508.73176884106641</v>
+        <v>532.48001006844606</v>
       </c>
       <c r="L34" s="1">
-        <v>11563.66390657458</v>
+        <v>12103.470336495941</v>
       </c>
       <c r="M34" s="1">
-        <v>110.5493213773351</v>
+        <v>115.7099032642749</v>
       </c>
       <c r="N34">
-        <v>110.5493213773351</v>
+        <v>115.7099032642749</v>
       </c>
       <c r="O34" t="s">
         <v>20</v>
@@ -2328,7 +2327,7 @@
       <c r="D35" s="4">
         <v>45699.899305555547</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="7">
         <v>95686.37</v>
       </c>
       <c r="F35" s="1">
@@ -2338,25 +2337,25 @@
         <v>94577.04877914043</v>
       </c>
       <c r="H35" s="1">
-        <v>95959.38</v>
+        <v>96155.59</v>
       </c>
       <c r="I35" s="1">
-        <v>0.31272269084371818</v>
+        <v>0.32732098085487749</v>
       </c>
       <c r="J35" t="s">
         <v>18</v>
       </c>
       <c r="K35" s="7">
-        <v>-85.376421827246432</v>
+        <v>-121.0347033649594</v>
       </c>
       <c r="L35" s="1">
-        <v>11478.28748474733</v>
+        <v>11982.435633130979</v>
       </c>
       <c r="M35" s="1">
-        <v>115.6366390657458</v>
+        <v>121.0347033649594</v>
       </c>
       <c r="N35">
-        <v>115.6366390657458</v>
+        <v>121.0347033649594</v>
       </c>
       <c r="O35" t="s">
         <v>20</v>
@@ -2381,7 +2380,7 @@
       <c r="D36" s="4">
         <v>45700.5625</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="7">
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
@@ -2394,22 +2393,22 @@
         <v>94844.800000000003</v>
       </c>
       <c r="I36" s="1">
-        <v>0.28491871165624028</v>
+        <v>0.29743288165871012</v>
       </c>
       <c r="J36" t="s">
         <v>19</v>
       </c>
       <c r="K36" s="7">
-        <v>419.64822283712539</v>
+        <v>438.07996840866292</v>
       </c>
       <c r="L36" s="1">
-        <v>11897.93570758446</v>
+        <v>12420.515601539641</v>
       </c>
       <c r="M36" s="1">
-        <v>114.78287484747329</v>
+        <v>119.8243563313098</v>
       </c>
       <c r="N36">
-        <v>114.78287484747329</v>
+        <v>119.8243563313098</v>
       </c>
       <c r="O36" t="s">
         <v>20</v>
@@ -2434,7 +2433,7 @@
       <c r="D37" s="4">
         <v>45701.895833333343</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="7">
         <v>96270.05</v>
       </c>
       <c r="F37" s="1">
@@ -2444,25 +2443,25 @@
         <v>94975.09366136376</v>
       </c>
       <c r="H37" s="1">
-        <v>96412.79</v>
+        <v>96774.71</v>
       </c>
       <c r="I37" s="1">
-        <v>0.27563714742957268</v>
+        <v>0.28774365353399178</v>
       </c>
       <c r="J37" t="s">
         <v>18</v>
       </c>
       <c r="K37" s="7">
-        <v>-39.344446424094649</v>
+        <v>-124.2051560153964</v>
       </c>
       <c r="L37" s="1">
-        <v>11858.59126116036</v>
+        <v>12296.31044552425</v>
       </c>
       <c r="M37" s="1">
-        <v>118.9793570758446</v>
+        <v>124.2051560153964</v>
       </c>
       <c r="N37">
-        <v>118.9793570758446</v>
+        <v>124.2051560153964</v>
       </c>
       <c r="O37" t="s">
         <v>20</v>
@@ -2474,49 +2473,49 @@
         <v>1294.956338636242</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="1">
-        <v>10000</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1">
-        <v>11858.59126116036</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="5">
-        <v>0.18585912611603631</v>
+        <v>23</v>
+      </c>
+      <c r="B43" s="1">
+        <v>12296.31044552425</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0.22963104455242481</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="5">
-        <v>0.3611111111111111</v>
+      <c r="B46" s="5">
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
format xlsx with correct data
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
   <si>
     <t>Position</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Risk Amount ($)</t>
-  </si>
-  <si>
-    <t>Actual Risk ($)</t>
   </si>
   <si>
     <t>Risk-Reward Ratio</t>
@@ -106,12 +103,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,13 +117,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,11 +162,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -186,11 +174,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,18 +489,11 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
-    <col min="6" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="7" customWidth="1"/>
-    <col min="12" max="13" width="18.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +503,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -543,7 +521,7 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -561,16 +539,13 @@
       <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4">
         <v>45666.635416666657</v>
@@ -578,7 +553,7 @@
       <c r="D2" s="4">
         <v>45666.645833333343</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="1">
         <v>93188.2</v>
       </c>
       <c r="F2" s="1">
@@ -593,10 +568,10 @@
       <c r="I2" s="1">
         <v>0.16309223621077859</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="7">
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1">
         <v>-100</v>
       </c>
       <c r="L2" s="1">
@@ -605,25 +580,22 @@
       <c r="M2" s="1">
         <v>100</v>
       </c>
-      <c r="N2">
-        <v>99.999999999999986</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2">
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1">
         <v>613.1499715949758</v>
       </c>
-      <c r="Q2">
+      <c r="P2" s="1">
         <v>1839.4499147849131</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
         <v>45666.649305555547</v>
@@ -631,7 +603,7 @@
       <c r="D3" s="4">
         <v>45666.659722222219</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="1">
         <v>93739.87</v>
       </c>
       <c r="F3" s="1">
@@ -646,10 +618,10 @@
       <c r="I3" s="1">
         <v>0.15555303747784549</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="7">
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1">
         <v>-99</v>
       </c>
       <c r="L3" s="1">
@@ -658,25 +630,22 @@
       <c r="M3" s="1">
         <v>99</v>
       </c>
-      <c r="N3">
-        <v>99</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3">
+      <c r="N3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="1">
         <v>636.43887387348514</v>
       </c>
-      <c r="Q3">
+      <c r="P3" s="1">
         <v>1909.31662162047</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4">
         <v>45666.663194444453</v>
@@ -684,7 +653,7 @@
       <c r="D4" s="4">
         <v>45666.822916666657</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="1">
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
@@ -699,10 +668,10 @@
       <c r="I4" s="1">
         <v>0.14502302872544071</v>
       </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="7">
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1">
         <v>309.93886630114969</v>
       </c>
       <c r="L4" s="1">
@@ -711,25 +680,22 @@
       <c r="M4" s="1">
         <v>98.01</v>
       </c>
-      <c r="N4">
-        <v>98.01</v>
-      </c>
-      <c r="O4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4">
+      <c r="N4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="1">
         <v>675.82370097616513</v>
       </c>
-      <c r="Q4">
+      <c r="P4" s="1">
         <v>2027.4711029285099</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>45667.75</v>
@@ -737,7 +703,7 @@
       <c r="D5" s="4">
         <v>45670.541666666657</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="1">
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
@@ -752,10 +718,10 @@
       <c r="I5" s="1">
         <v>0.12153024669061829</v>
       </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="1">
         <v>595.92234934497867</v>
       </c>
       <c r="L5" s="1">
@@ -764,25 +730,22 @@
       <c r="M5" s="1">
         <v>101.1093886630115</v>
       </c>
-      <c r="N5">
-        <v>101.1093886630115</v>
-      </c>
-      <c r="O5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5">
+      <c r="N5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="1">
         <v>831.96892474354536</v>
       </c>
-      <c r="Q5">
+      <c r="P5" s="1">
         <v>2495.9067742306361</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>45670.635416666657</v>
@@ -790,7 +753,7 @@
       <c r="D6" s="4">
         <v>45670.868055555547</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="1">
         <v>92680.01</v>
       </c>
       <c r="F6" s="1">
@@ -805,10 +768,10 @@
       <c r="I6" s="1">
         <v>0.1010857708998836</v>
       </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1">
         <v>-107.0686121564613</v>
       </c>
       <c r="L6" s="1">
@@ -817,25 +780,22 @@
       <c r="M6" s="1">
         <v>107.0686121564613</v>
       </c>
-      <c r="N6">
-        <v>107.0686121564613</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6">
+      <c r="N6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="1">
         <v>1059.185790475924</v>
       </c>
-      <c r="Q6">
+      <c r="P6" s="1">
         <v>3177.5573714277712</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4">
         <v>45673.625</v>
@@ -843,7 +803,7 @@
       <c r="D7" s="4">
         <v>45673.670138888891</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="1">
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
@@ -858,10 +818,10 @@
       <c r="I7" s="1">
         <v>0.15506208970601851</v>
       </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="J7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="1">
         <v>347.96553178389507</v>
       </c>
       <c r="L7" s="1">
@@ -870,25 +830,22 @@
       <c r="M7" s="1">
         <v>105.99792603489669</v>
       </c>
-      <c r="N7">
-        <v>105.99792603489669</v>
-      </c>
-      <c r="O7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7">
+      <c r="N7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="1">
         <v>683.58375819555658</v>
       </c>
-      <c r="Q7">
+      <c r="P7" s="1">
         <v>2050.7512745866702</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4">
         <v>45674.871527777781</v>
@@ -896,7 +853,7 @@
       <c r="D8" s="4">
         <v>45675.541666666657</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="1">
         <v>104692.7</v>
       </c>
       <c r="F8" s="1">
@@ -911,10 +868,10 @@
       <c r="I8" s="1">
         <v>0.2209226999473812</v>
       </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1">
         <v>-109.4775813527356</v>
       </c>
       <c r="L8" s="1">
@@ -923,25 +880,22 @@
       <c r="M8" s="1">
         <v>109.4775813527356</v>
       </c>
-      <c r="N8">
-        <v>109.4775813527356</v>
-      </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8">
+      <c r="N8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="1">
         <v>495.54700073288399</v>
       </c>
-      <c r="Q8">
+      <c r="P8" s="1">
         <v>1486.641002198638</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4">
         <v>45675.701388888891</v>
@@ -949,7 +903,7 @@
       <c r="D9" s="4">
         <v>45676.541666666657</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="1">
         <v>103240.85</v>
       </c>
       <c r="F9" s="1">
@@ -964,10 +918,10 @@
       <c r="I9" s="1">
         <v>0.19634752047467049</v>
       </c>
-      <c r="J9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1">
         <v>376.38837937391901</v>
       </c>
       <c r="L9" s="1">
@@ -976,25 +930,22 @@
       <c r="M9" s="1">
         <v>108.38280553920831</v>
       </c>
-      <c r="N9">
-        <v>108.38280553920831</v>
-      </c>
-      <c r="O9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9">
+      <c r="N9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="1">
         <v>551.99477577915241</v>
       </c>
-      <c r="Q9">
+      <c r="P9" s="1">
         <v>1655.984327337472</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4">
         <v>45677.659722222219</v>
@@ -1002,7 +953,7 @@
       <c r="D10" s="4">
         <v>45677.673611111109</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="1">
         <v>105535.7</v>
       </c>
       <c r="F10" s="1">
@@ -1017,10 +968,10 @@
       <c r="I10" s="1">
         <v>0.10116532065490461</v>
       </c>
-      <c r="J10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="1">
         <v>-112.1466893329475</v>
       </c>
       <c r="L10" s="1">
@@ -1029,25 +980,22 @@
       <c r="M10" s="1">
         <v>112.1466893329475</v>
       </c>
-      <c r="N10">
-        <v>112.1466893329475</v>
-      </c>
-      <c r="O10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10">
+      <c r="N10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="1">
         <v>1108.548745824693</v>
       </c>
-      <c r="Q10">
+      <c r="P10" s="1">
         <v>3325.64623747408</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4">
         <v>45678.628472222219</v>
@@ -1055,7 +1003,7 @@
       <c r="D11" s="4">
         <v>45678.673611111109</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="1">
         <v>103281.22</v>
       </c>
       <c r="F11" s="1">
@@ -1070,10 +1018,10 @@
       <c r="I11" s="1">
         <v>0.1161594969572064</v>
       </c>
-      <c r="J11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="7">
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="1">
         <v>350.65996622447528</v>
       </c>
       <c r="L11" s="1">
@@ -1082,25 +1030,22 @@
       <c r="M11" s="1">
         <v>111.02522243961801</v>
       </c>
-      <c r="N11">
-        <v>111.02522243961801</v>
-      </c>
-      <c r="O11" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11">
+      <c r="N11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="1">
         <v>955.79978691299038</v>
       </c>
-      <c r="Q11">
+      <c r="P11" s="1">
         <v>2867.3993607389862</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4">
         <v>45678.861111111109</v>
@@ -1108,7 +1053,7 @@
       <c r="D12" s="4">
         <v>45679.541666666657</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="1">
         <v>106072</v>
       </c>
       <c r="F12" s="1">
@@ -1123,10 +1068,10 @@
       <c r="I12" s="1">
         <v>0.16820117969568951</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="7">
+      <c r="J12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="1">
         <v>-114.5318221018627</v>
       </c>
       <c r="L12" s="1">
@@ -1135,25 +1080,22 @@
       <c r="M12" s="1">
         <v>114.5318221018627</v>
       </c>
-      <c r="N12">
-        <v>114.5318221018627</v>
-      </c>
-      <c r="O12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12">
+      <c r="N12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="1">
         <v>680.921633897422</v>
       </c>
-      <c r="Q12">
+      <c r="P12" s="1">
         <v>2042.764901692251</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4">
         <v>45679.548611111109</v>
@@ -1161,7 +1103,7 @@
       <c r="D13" s="4">
         <v>45679.565972222219</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="1">
         <v>104947.17</v>
       </c>
       <c r="F13" s="1">
@@ -1176,10 +1118,10 @@
       <c r="I13" s="1">
         <v>0.36731419601443532</v>
       </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="1">
         <v>-113.3865038808441</v>
       </c>
       <c r="L13" s="1">
@@ -1188,25 +1130,22 @@
       <c r="M13" s="1">
         <v>113.3865038808441</v>
       </c>
-      <c r="N13">
-        <v>113.3865038808441</v>
-      </c>
-      <c r="O13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13">
+      <c r="N13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="1">
         <v>308.69077512154757</v>
       </c>
-      <c r="Q13">
+      <c r="P13" s="1">
         <v>926.07232536464289</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4">
         <v>45679.579861111109</v>
@@ -1214,7 +1153,7 @@
       <c r="D14" s="4">
         <v>45679.694444444453</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="1">
         <v>104073.94</v>
       </c>
       <c r="F14" s="1">
@@ -1229,10 +1168,10 @@
       <c r="I14" s="1">
         <v>0.24082978044746139</v>
       </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1">
         <v>-112.25263884203569</v>
       </c>
       <c r="L14" s="1">
@@ -1241,25 +1180,22 @@
       <c r="M14" s="1">
         <v>112.25263884203569</v>
       </c>
-      <c r="N14">
-        <v>112.25263884203569</v>
-      </c>
-      <c r="O14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14">
+      <c r="N14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="1">
         <v>466.10779876753799</v>
       </c>
-      <c r="Q14">
+      <c r="P14" s="1">
         <v>1398.3233963026139</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4">
         <v>45679.881944444453</v>
@@ -1267,7 +1203,7 @@
       <c r="D15" s="4">
         <v>45680.541666666657</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="1">
         <v>103891.76</v>
       </c>
       <c r="F15" s="1">
@@ -1282,10 +1218,10 @@
       <c r="I15" s="1">
         <v>0.21864682974783711</v>
       </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="7">
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1">
         <v>-111.1301124536153</v>
       </c>
       <c r="L15" s="1">
@@ -1294,25 +1230,22 @@
       <c r="M15" s="1">
         <v>111.1301124536153</v>
       </c>
-      <c r="N15">
-        <v>111.1301124536153</v>
-      </c>
-      <c r="O15" t="s">
-        <v>20</v>
-      </c>
-      <c r="P15">
+      <c r="N15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="1">
         <v>508.26308609999251</v>
       </c>
-      <c r="Q15">
+      <c r="P15" s="1">
         <v>1524.789258299978</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4">
         <v>45680.829861111109</v>
@@ -1320,7 +1253,7 @@
       <c r="D16" s="4">
         <v>45680.850694444453</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="1">
         <v>103770.04</v>
       </c>
       <c r="F16" s="1">
@@ -1335,10 +1268,10 @@
       <c r="I16" s="1">
         <v>0.12728903413824669</v>
       </c>
-      <c r="J16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="J16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="1">
         <v>337.44195661015141</v>
       </c>
       <c r="L16" s="1">
@@ -1347,25 +1280,22 @@
       <c r="M16" s="1">
         <v>110.0188113290792</v>
       </c>
-      <c r="N16">
-        <v>110.0188113290792</v>
-      </c>
-      <c r="O16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P16">
+      <c r="N16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="1">
         <v>864.32277590848389</v>
       </c>
-      <c r="Q16">
+      <c r="P16" s="1">
         <v>2592.9683277254521</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4">
         <v>45681.829861111109</v>
@@ -1373,7 +1303,7 @@
       <c r="D17" s="4">
         <v>45681.847222222219</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="1">
         <v>105760.94</v>
       </c>
       <c r="F17" s="1">
@@ -1388,10 +1318,10 @@
       <c r="I17" s="1">
         <v>0.24305375705691459</v>
       </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="7">
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1">
         <v>-113.39323089518069</v>
       </c>
       <c r="L17" s="1">
@@ -1400,25 +1330,22 @@
       <c r="M17" s="1">
         <v>113.39323089518069</v>
       </c>
-      <c r="N17">
-        <v>113.39323089518069</v>
-      </c>
-      <c r="O17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P17">
+      <c r="N17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="1">
         <v>466.53560211631702</v>
       </c>
-      <c r="Q17">
+      <c r="P17" s="1">
         <v>1399.6068063489511</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4">
         <v>45681.857638888891</v>
@@ -1426,7 +1353,7 @@
       <c r="D18" s="4">
         <v>45682.586805555547</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="1">
         <v>105052.52</v>
       </c>
       <c r="F18" s="1">
@@ -1441,10 +1368,10 @@
       <c r="I18" s="1">
         <v>0.24314079223859611</v>
       </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="7">
+      <c r="J18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="1">
         <v>-112.25929858622889</v>
       </c>
       <c r="L18" s="1">
@@ -1453,25 +1380,22 @@
       <c r="M18" s="1">
         <v>112.25929858622889</v>
       </c>
-      <c r="N18">
-        <v>112.25929858622889</v>
-      </c>
-      <c r="O18" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18">
+      <c r="N18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="1">
         <v>461.7049140650488</v>
       </c>
-      <c r="Q18">
+      <c r="P18" s="1">
         <v>1385.1147421951609</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4">
         <v>45683.885416666657</v>
@@ -1479,7 +1403,7 @@
       <c r="D19" s="4">
         <v>45683.90625</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="1">
         <v>104795.54</v>
       </c>
       <c r="F19" s="1">
@@ -1494,10 +1418,10 @@
       <c r="I19" s="1">
         <v>0.69448579088064044</v>
       </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="7">
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1">
         <v>-111.1367056003666</v>
       </c>
       <c r="L19" s="1">
@@ -1506,25 +1430,22 @@
       <c r="M19" s="1">
         <v>111.1367056003666</v>
       </c>
-      <c r="N19">
-        <v>111.1367056003666</v>
-      </c>
-      <c r="O19" t="s">
-        <v>20</v>
-      </c>
-      <c r="P19">
+      <c r="N19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="1">
         <v>160.02732821853709</v>
       </c>
-      <c r="Q19">
+      <c r="P19" s="1">
         <v>480.0819846555969</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="4">
         <v>45684.541666666657</v>
@@ -1532,7 +1453,7 @@
       <c r="D20" s="4">
         <v>45684.545138888891</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="1">
         <v>100632.01</v>
       </c>
       <c r="F20" s="1">
@@ -1547,10 +1468,10 @@
       <c r="I20" s="1">
         <v>0.16821349725932291</v>
       </c>
-      <c r="J20" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="7">
+      <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="1">
         <v>-110.0253385443629</v>
       </c>
       <c r="L20" s="1">
@@ -1559,25 +1480,22 @@
       <c r="M20" s="1">
         <v>110.0253385443629</v>
       </c>
-      <c r="N20">
-        <v>110.0253385443629</v>
-      </c>
-      <c r="O20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P20">
+      <c r="N20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" s="1">
         <v>654.08151151357742</v>
       </c>
-      <c r="Q20">
+      <c r="P20" s="1">
         <v>1962.244534540718</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="4">
         <v>45684.850694444453</v>
@@ -1585,7 +1503,7 @@
       <c r="D21" s="4">
         <v>45684.864583333343</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="1">
         <v>100351.67999999999</v>
       </c>
       <c r="F21" s="1">
@@ -1600,10 +1518,10 @@
       <c r="I21" s="1">
         <v>0.17956836630024639</v>
       </c>
-      <c r="J21" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="7">
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="1">
         <v>-108.9250851589193</v>
       </c>
       <c r="L21" s="1">
@@ -1612,25 +1530,22 @@
       <c r="M21" s="1">
         <v>108.9250851589193</v>
       </c>
-      <c r="N21">
-        <v>108.9250851589193</v>
-      </c>
-      <c r="O21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P21">
+      <c r="N21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="1">
         <v>606.59395306181978</v>
       </c>
-      <c r="Q21">
+      <c r="P21" s="1">
         <v>1819.781859185445</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4">
         <v>45684.871527777781</v>
@@ -1638,7 +1553,7 @@
       <c r="D22" s="4">
         <v>45684.878472222219</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="1">
         <v>101386.5</v>
       </c>
       <c r="F22" s="1">
@@ -1653,10 +1568,10 @@
       <c r="I22" s="1">
         <v>0.16314438629449249</v>
       </c>
-      <c r="J22" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="1">
         <v>-107.8358343073301</v>
       </c>
       <c r="L22" s="1">
@@ -1665,25 +1580,22 @@
       <c r="M22" s="1">
         <v>107.8358343073301</v>
       </c>
-      <c r="N22">
-        <v>107.8358343073301</v>
-      </c>
-      <c r="O22" t="s">
-        <v>20</v>
-      </c>
-      <c r="P22">
+      <c r="N22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O22" s="1">
         <v>660.98403234466969</v>
       </c>
-      <c r="Q22">
+      <c r="P22" s="1">
         <v>1982.9520970340091</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4">
         <v>45684.881944444453</v>
@@ -1691,7 +1603,7 @@
       <c r="D23" s="4">
         <v>45685.625</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="1">
         <v>102295.12</v>
       </c>
       <c r="F23" s="1">
@@ -1706,10 +1618,10 @@
       <c r="I23" s="1">
         <v>0.14954214847940031</v>
       </c>
-      <c r="J23" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="7">
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="1">
         <v>-106.7574759642568</v>
       </c>
       <c r="L23" s="1">
@@ -1718,25 +1630,22 @@
       <c r="M23" s="1">
         <v>106.7574759642568</v>
       </c>
-      <c r="N23">
-        <v>106.7574759642568</v>
-      </c>
-      <c r="O23" t="s">
-        <v>20</v>
-      </c>
-      <c r="P23">
+      <c r="N23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="1">
         <v>713.89556088237441</v>
       </c>
-      <c r="Q23">
+      <c r="P23" s="1">
         <v>2141.6866826471228</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4">
         <v>45687.736111111109</v>
@@ -1744,7 +1653,7 @@
       <c r="D24" s="4">
         <v>45688.565972222219</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="1">
         <v>105018.14</v>
       </c>
       <c r="F24" s="1">
@@ -1759,10 +1668,10 @@
       <c r="I24" s="1">
         <v>0.22857088500790479</v>
       </c>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24" s="7">
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="1">
         <v>-105.6899012046142</v>
       </c>
       <c r="L24" s="1">
@@ -1771,25 +1680,22 @@
       <c r="M24" s="1">
         <v>105.6899012046142</v>
       </c>
-      <c r="N24">
-        <v>105.6899012046142</v>
-      </c>
-      <c r="O24" t="s">
-        <v>20</v>
-      </c>
-      <c r="P24">
+      <c r="N24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O24" s="1">
         <v>462.39441738592001</v>
       </c>
-      <c r="Q24">
+      <c r="P24" s="1">
         <v>1387.1832521577739</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="4">
         <v>45690.590277777781</v>
@@ -1797,7 +1703,7 @@
       <c r="D25" s="4">
         <v>45690.722222222219</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="1">
         <v>99272.12</v>
       </c>
       <c r="F25" s="1">
@@ -1812,10 +1718,10 @@
       <c r="I25" s="1">
         <v>0.2361841436036666</v>
       </c>
-      <c r="J25" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="7">
+      <c r="J25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="1">
         <v>364.93284396489622</v>
       </c>
       <c r="L25" s="1">
@@ -1824,25 +1730,22 @@
       <c r="M25" s="1">
         <v>104.6330021925681</v>
       </c>
-      <c r="N25">
-        <v>104.6330021925681</v>
-      </c>
-      <c r="O25" t="s">
-        <v>20</v>
-      </c>
-      <c r="P25">
+      <c r="N25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O25" s="1">
         <v>443.01450807023502</v>
       </c>
-      <c r="Q25">
+      <c r="P25" s="1">
         <v>1329.0435242107201</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="4">
         <v>45690.822916666657</v>
@@ -1850,7 +1753,7 @@
       <c r="D26" s="4">
         <v>45691.541666666657</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="1">
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
@@ -1865,10 +1768,10 @@
       <c r="I26" s="1">
         <v>0.13120801609632521</v>
       </c>
-      <c r="J26" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="7">
+      <c r="J26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="1">
         <v>517.98825426571614</v>
       </c>
       <c r="L26" s="1">
@@ -1877,25 +1780,22 @@
       <c r="M26" s="1">
         <v>108.2823306322171</v>
       </c>
-      <c r="N26">
-        <v>108.2823306322171</v>
-      </c>
-      <c r="O26" t="s">
-        <v>20</v>
-      </c>
-      <c r="P26">
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1">
         <v>825.27221928820654</v>
       </c>
-      <c r="Q26">
+      <c r="P26" s="1">
         <v>2475.8166578646342</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="4">
         <v>45691.611111111109</v>
@@ -1903,7 +1803,7 @@
       <c r="D27" s="4">
         <v>45691.635416666657</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="1">
         <v>96150.84</v>
       </c>
       <c r="F27" s="1">
@@ -1918,10 +1818,10 @@
       <c r="I27" s="1">
         <v>0.1135116372720907</v>
       </c>
-      <c r="J27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="7">
+      <c r="J27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="1">
         <v>-113.46221317487419</v>
       </c>
       <c r="L27" s="1">
@@ -1930,25 +1830,22 @@
       <c r="M27" s="1">
         <v>113.46221317487419</v>
       </c>
-      <c r="N27">
-        <v>113.46221317487419</v>
-      </c>
-      <c r="O27" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27">
+      <c r="N27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O27" s="1">
         <v>999.56459004200588</v>
       </c>
-      <c r="Q27">
+      <c r="P27" s="1">
         <v>2998.6937701260322</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="4">
         <v>45691.666666666657</v>
@@ -1956,7 +1853,7 @@
       <c r="D28" s="4">
         <v>45691.784722222219</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="1">
         <v>98730.93</v>
       </c>
       <c r="F28" s="1">
@@ -1971,10 +1868,10 @@
       <c r="I28" s="1">
         <v>9.5379388290535314E-2</v>
       </c>
-      <c r="J28" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="7">
+      <c r="J28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="1">
         <v>-112.32759104312549</v>
       </c>
       <c r="L28" s="1">
@@ -1983,25 +1880,22 @@
       <c r="M28" s="1">
         <v>112.32759104312549</v>
       </c>
-      <c r="N28">
-        <v>112.32759104312549</v>
-      </c>
-      <c r="O28" t="s">
-        <v>20</v>
-      </c>
-      <c r="P28">
+      <c r="N28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="1">
         <v>1177.6925083747051</v>
       </c>
-      <c r="Q28">
+      <c r="P28" s="1">
         <v>3533.0775251240989</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="4">
         <v>45693.576388888891</v>
@@ -2009,7 +1903,7 @@
       <c r="D29" s="4">
         <v>45693.611111111109</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="1">
         <v>98581.99</v>
       </c>
       <c r="F29" s="1">
@@ -2024,10 +1918,10 @@
       <c r="I29" s="1">
         <v>0.32552441439005519</v>
       </c>
-      <c r="J29" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="7">
+      <c r="J29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="1">
         <v>-111.20431513269421</v>
       </c>
       <c r="L29" s="1">
@@ -2036,25 +1930,22 @@
       <c r="M29" s="1">
         <v>111.20431513269421</v>
       </c>
-      <c r="N29">
-        <v>111.20431513269421</v>
-      </c>
-      <c r="O29" t="s">
-        <v>20</v>
-      </c>
-      <c r="P29">
+      <c r="N29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29" s="1">
         <v>341.61589796900807</v>
       </c>
-      <c r="Q29">
+      <c r="P29" s="1">
         <v>1024.847693907024</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="4">
         <v>45694.864583333343</v>
@@ -2062,7 +1953,7 @@
       <c r="D30" s="4">
         <v>45695.541666666657</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="1">
         <v>96870.9</v>
       </c>
       <c r="F30" s="1">
@@ -2077,10 +1968,10 @@
       <c r="I30" s="1">
         <v>0.22470505376246569</v>
       </c>
-      <c r="J30" t="s">
-        <v>18</v>
-      </c>
-      <c r="K30" s="7">
+      <c r="J30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="1">
         <v>-110.0922719813673</v>
       </c>
       <c r="L30" s="1">
@@ -2089,25 +1980,22 @@
       <c r="M30" s="1">
         <v>110.0922719813673</v>
       </c>
-      <c r="N30">
-        <v>110.0922719813673</v>
-      </c>
-      <c r="O30" t="s">
-        <v>20</v>
-      </c>
-      <c r="P30">
+      <c r="N30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O30" s="1">
         <v>489.94123691470298</v>
       </c>
-      <c r="Q30">
+      <c r="P30" s="1">
         <v>1469.8237107441089</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="4">
         <v>45696.569444444453</v>
@@ -2115,7 +2003,7 @@
       <c r="D31" s="4">
         <v>45696.645833333343</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="1">
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
@@ -2130,10 +2018,10 @@
       <c r="I31" s="1">
         <v>0.5099007979215523</v>
       </c>
-      <c r="J31" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="7">
+      <c r="J31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="1">
         <v>372.39584974604821</v>
       </c>
       <c r="L31" s="1">
@@ -2142,25 +2030,22 @@
       <c r="M31" s="1">
         <v>108.99134926155359</v>
       </c>
-      <c r="N31">
-        <v>108.99134926155359</v>
-      </c>
-      <c r="O31" t="s">
-        <v>20</v>
-      </c>
-      <c r="P31">
+      <c r="N31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O31" s="1">
         <v>213.7501053260203</v>
       </c>
-      <c r="Q31">
+      <c r="P31" s="1">
         <v>641.25031597806083</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="4">
         <v>45696.711805555547</v>
@@ -2168,7 +2053,7 @@
       <c r="D32" s="4">
         <v>45696.777777777781</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="1">
         <v>96282.74</v>
       </c>
       <c r="F32" s="1">
@@ -2183,10 +2068,10 @@
       <c r="I32" s="1">
         <v>0.50860760290207696</v>
       </c>
-      <c r="J32" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="7">
+      <c r="J32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="1">
         <v>-112.7153077590141</v>
       </c>
       <c r="L32" s="1">
@@ -2195,25 +2080,22 @@
       <c r="M32" s="1">
         <v>112.7153077590141</v>
       </c>
-      <c r="N32">
-        <v>112.7153077590141</v>
-      </c>
-      <c r="O32" t="s">
-        <v>20</v>
-      </c>
-      <c r="P32">
+      <c r="N32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" s="1">
         <v>221.61545976872731</v>
       </c>
-      <c r="Q32">
+      <c r="P32" s="1">
         <v>664.84637930618192</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="4">
         <v>45696.805555555547</v>
@@ -2221,7 +2103,7 @@
       <c r="D33" s="4">
         <v>45697.572916666657</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="1">
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
@@ -2236,10 +2118,10 @@
       <c r="I33" s="1">
         <v>0.58282643988278204</v>
       </c>
-      <c r="J33" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="7">
+      <c r="J33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="1">
         <v>412.17485828510178</v>
       </c>
       <c r="L33" s="1">
@@ -2248,25 +2130,22 @@
       <c r="M33" s="1">
         <v>111.5881546814239</v>
       </c>
-      <c r="N33">
-        <v>111.5881546814239</v>
-      </c>
-      <c r="O33" t="s">
-        <v>20</v>
-      </c>
-      <c r="P33">
+      <c r="N33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" s="1">
         <v>191.46035087884229</v>
       </c>
-      <c r="Q33">
+      <c r="P33" s="1">
         <v>574.38105263654143</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="4">
         <v>45697.652777777781</v>
@@ -2274,7 +2153,7 @@
       <c r="D34" s="4">
         <v>45697.899305555547</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="1">
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
@@ -2289,10 +2168,10 @@
       <c r="I34" s="1">
         <v>0.43101830182001161</v>
       </c>
-      <c r="J34" t="s">
-        <v>19</v>
-      </c>
-      <c r="K34" s="7">
+      <c r="J34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="1">
         <v>532.48001006844606</v>
       </c>
       <c r="L34" s="1">
@@ -2301,25 +2180,22 @@
       <c r="M34" s="1">
         <v>115.7099032642749</v>
       </c>
-      <c r="N34">
-        <v>115.7099032642749</v>
-      </c>
-      <c r="O34" t="s">
-        <v>20</v>
-      </c>
-      <c r="P34">
+      <c r="N34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" s="1">
         <v>268.45705339119007</v>
       </c>
-      <c r="Q34">
+      <c r="P34" s="1">
         <v>805.37116017357039</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="4">
         <v>45699.888888888891</v>
@@ -2327,7 +2203,7 @@
       <c r="D35" s="4">
         <v>45699.899305555547</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="1">
         <v>95686.37</v>
       </c>
       <c r="F35" s="1">
@@ -2342,10 +2218,10 @@
       <c r="I35" s="1">
         <v>0.32732098085487749</v>
       </c>
-      <c r="J35" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="7">
+      <c r="J35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="1">
         <v>-121.0347033649594</v>
       </c>
       <c r="L35" s="1">
@@ -2354,25 +2230,22 @@
       <c r="M35" s="1">
         <v>121.0347033649594</v>
       </c>
-      <c r="N35">
-        <v>121.0347033649594</v>
-      </c>
-      <c r="O35" t="s">
-        <v>20</v>
-      </c>
-      <c r="P35">
+      <c r="N35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" s="1">
         <v>369.77374028651678</v>
       </c>
-      <c r="Q35">
+      <c r="P35" s="1">
         <v>1109.3212208595651</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="4">
         <v>45699.90625</v>
@@ -2380,7 +2253,7 @@
       <c r="D36" s="4">
         <v>45700.5625</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="1">
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
@@ -2395,10 +2268,10 @@
       <c r="I36" s="1">
         <v>0.29743288165871012</v>
       </c>
-      <c r="J36" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="7">
+      <c r="J36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="1">
         <v>438.07996840866292</v>
       </c>
       <c r="L36" s="1">
@@ -2407,25 +2280,22 @@
       <c r="M36" s="1">
         <v>119.8243563313098</v>
       </c>
-      <c r="N36">
-        <v>119.8243563313098</v>
-      </c>
-      <c r="O36" t="s">
-        <v>20</v>
-      </c>
-      <c r="P36">
+      <c r="N36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O36" s="1">
         <v>402.86183445178898</v>
       </c>
-      <c r="Q36">
+      <c r="P36" s="1">
         <v>1208.5855033553819</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="4">
         <v>45701.798611111109</v>
@@ -2433,7 +2303,7 @@
       <c r="D37" s="4">
         <v>45701.895833333343</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="1">
         <v>96270.05</v>
       </c>
       <c r="F37" s="1">
@@ -2448,10 +2318,10 @@
       <c r="I37" s="1">
         <v>0.28774365353399178</v>
       </c>
-      <c r="J37" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="7">
+      <c r="J37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="1">
         <v>-124.2051560153964</v>
       </c>
       <c r="L37" s="1">
@@ -2460,59 +2330,56 @@
       <c r="M37" s="1">
         <v>124.2051560153964</v>
       </c>
-      <c r="N37">
-        <v>124.2051560153964</v>
-      </c>
-      <c r="O37" t="s">
+      <c r="N37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="1">
+        <v>431.65211287874263</v>
+      </c>
+      <c r="P37" s="1">
+        <v>1294.956338636242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P37">
-        <v>431.65211287874263</v>
-      </c>
-      <c r="Q37">
-        <v>1294.956338636242</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>22</v>
       </c>
       <c r="B42" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
         <v>12296.31044552425</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="5">
         <v>0.22963104455242481</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="5">
         <v>0.33333333333333331</v>

</xml_diff>

<commit_message>
fixed profits to be 1:3 RR (might change back)
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Backtesting\strategy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Trade History" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
   <si>
     <t>Position</t>
   </si>
@@ -102,12 +97,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,21 +169,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -234,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,10 +254,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,7 +288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,23 +463,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
     <col min="12" max="16" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -540,7 +526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -548,27 +534,27 @@
         <v>15</v>
       </c>
       <c r="C2" s="4">
-        <v>45666.635416666657</v>
+        <v>45666.63541666666</v>
       </c>
       <c r="D2" s="4">
-        <v>45666.645833333343</v>
+        <v>45666.64583333334</v>
       </c>
       <c r="E2" s="1">
         <v>93188.2</v>
       </c>
       <c r="F2" s="1">
-        <v>93801.349971594973</v>
+        <v>93801.34997159497</v>
       </c>
       <c r="G2" s="1">
-        <v>91348.750085215084</v>
+        <v>91348.75008521508</v>
       </c>
       <c r="H2" s="1">
-        <v>93915.9</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.16309223621077859</v>
-      </c>
-      <c r="J2" s="1" t="s">
+        <v>93915.89999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.1630922362107786</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1">
@@ -587,10 +573,10 @@
         <v>613.1499715949758</v>
       </c>
       <c r="P2" s="1">
-        <v>1839.4499147849131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1839.449914784913</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -598,10 +584,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>45666.649305555547</v>
+        <v>45666.64930555555</v>
       </c>
       <c r="D3" s="4">
-        <v>45666.659722222219</v>
+        <v>45666.65972222222</v>
       </c>
       <c r="E3" s="1">
         <v>93739.87</v>
@@ -610,15 +596,15 @@
         <v>94376.30887387348</v>
       </c>
       <c r="G3" s="1">
-        <v>91830.553378379525</v>
+        <v>91830.55337837953</v>
       </c>
       <c r="H3" s="1">
         <v>94588.23</v>
       </c>
-      <c r="I3" s="1">
-        <v>0.15555303747784549</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3">
+        <v>0.1555530374778455</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="1">
@@ -634,13 +620,13 @@
         <v>19</v>
       </c>
       <c r="O3" s="1">
-        <v>636.43887387348514</v>
+        <v>636.4388738734851</v>
       </c>
       <c r="P3" s="1">
         <v>1909.31662162047</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -648,49 +634,49 @@
         <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>45666.663194444453</v>
+        <v>45666.66319444445</v>
       </c>
       <c r="D4" s="4">
-        <v>45666.822916666657</v>
+        <v>45666.82291666666</v>
       </c>
       <c r="E4" s="1">
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
-        <v>94919.843700976169</v>
+        <v>94919.84370097617</v>
       </c>
       <c r="G4" s="1">
-        <v>92216.548897071494</v>
+        <v>92216.54889707149</v>
       </c>
       <c r="H4" s="1">
-        <v>92106.85</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.14502302872544071</v>
-      </c>
-      <c r="J4" s="1" t="s">
+        <v>92106.85000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.1450230287254407</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="1">
-        <v>309.93886630114969</v>
+        <v>294.03</v>
       </c>
       <c r="L4" s="1">
-        <v>10110.93886630115</v>
+        <v>10095.03</v>
       </c>
       <c r="M4" s="1">
-        <v>98.01</v>
+        <v>98.01000000000001</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O4" s="1">
-        <v>675.82370097616513</v>
+        <v>675.8237009761651</v>
       </c>
       <c r="P4" s="1">
-        <v>2027.4711029285099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2027.47110292851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -701,46 +687,46 @@
         <v>45667.75</v>
       </c>
       <c r="D5" s="4">
-        <v>45670.541666666657</v>
+        <v>45670.54166666666</v>
       </c>
       <c r="E5" s="1">
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
-        <v>96318.698924743541</v>
+        <v>96318.69892474354</v>
       </c>
       <c r="G5" s="1">
         <v>92990.82322576936</v>
       </c>
       <c r="H5" s="1">
-        <v>90583.24</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.12153024669061829</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>90583.24000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.1213390272132075</v>
+      </c>
+      <c r="J5" t="s">
         <v>18</v>
       </c>
       <c r="K5" s="1">
-        <v>595.92234934497867</v>
+        <v>302.8509</v>
       </c>
       <c r="L5" s="1">
-        <v>10706.861215646129</v>
+        <v>10397.8809</v>
       </c>
       <c r="M5" s="1">
-        <v>101.1093886630115</v>
+        <v>100.9503</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O5" s="1">
-        <v>831.96892474354536</v>
+        <v>831.9689247435454</v>
       </c>
       <c r="P5" s="1">
-        <v>2495.9067742306361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2495.906774230636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -748,37 +734,37 @@
         <v>15</v>
       </c>
       <c r="C6" s="4">
-        <v>45670.635416666657</v>
+        <v>45670.63541666666</v>
       </c>
       <c r="D6" s="4">
-        <v>45670.868055555547</v>
+        <v>45670.86805555555</v>
       </c>
       <c r="E6" s="1">
-        <v>92680.01</v>
+        <v>92680.00999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>93739.195790475918</v>
+        <v>93739.19579047592</v>
       </c>
       <c r="G6" s="1">
-        <v>89502.452628572224</v>
+        <v>89502.45262857222</v>
       </c>
       <c r="H6" s="1">
         <v>93783.12</v>
       </c>
-      <c r="I6" s="1">
-        <v>0.1010857708998836</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6">
+        <v>0.09816862153454611</v>
+      </c>
+      <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="1">
-        <v>-107.0686121564613</v>
+        <v>-103.978809</v>
       </c>
       <c r="L6" s="1">
-        <v>10599.79260348967</v>
+        <v>10293.902091</v>
       </c>
       <c r="M6" s="1">
-        <v>107.0686121564613</v>
+        <v>103.978809</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>19</v>
@@ -787,10 +773,10 @@
         <v>1059.185790475924</v>
       </c>
       <c r="P6" s="1">
-        <v>3177.5573714277712</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3177.557371427771</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -801,46 +787,46 @@
         <v>45673.625</v>
       </c>
       <c r="D7" s="4">
-        <v>45673.670138888891</v>
+        <v>45673.67013888889</v>
       </c>
       <c r="E7" s="1">
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
-        <v>96887.646241804439</v>
+        <v>96887.64624180444</v>
       </c>
       <c r="G7" s="1">
-        <v>99621.981274586666</v>
+        <v>99621.98127458667</v>
       </c>
       <c r="H7" s="1">
         <v>99815.27</v>
       </c>
-      <c r="I7" s="1">
-        <v>0.15506208970601851</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7">
+        <v>0.150587283088361</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="1">
-        <v>347.96553178389507</v>
+        <v>308.81706273</v>
       </c>
       <c r="L7" s="1">
-        <v>10947.75813527356</v>
+        <v>10602.71915373</v>
       </c>
       <c r="M7" s="1">
-        <v>105.99792603489669</v>
+        <v>102.93902091</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O7" s="1">
-        <v>683.58375819555658</v>
+        <v>683.5837581955566</v>
       </c>
       <c r="P7" s="1">
-        <v>2050.7512745866702</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2050.75127458667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -848,10 +834,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>45674.871527777781</v>
+        <v>45674.87152777778</v>
       </c>
       <c r="D8" s="4">
-        <v>45675.541666666657</v>
+        <v>45675.54166666666</v>
       </c>
       <c r="E8" s="1">
         <v>104692.7</v>
@@ -860,37 +846,37 @@
         <v>104197.1529992671</v>
       </c>
       <c r="G8" s="1">
-        <v>106179.34100219861</v>
+        <v>106179.3410021986</v>
       </c>
       <c r="H8" s="1">
         <v>103424.59</v>
       </c>
-      <c r="I8" s="1">
-        <v>0.2209226999473812</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8">
+        <v>0.2139599097169233</v>
+      </c>
+      <c r="J8" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1">
-        <v>-109.4775813527356</v>
+        <v>-106.0271915373</v>
       </c>
       <c r="L8" s="1">
-        <v>10838.280553920829</v>
+        <v>10496.6919621927</v>
       </c>
       <c r="M8" s="1">
-        <v>109.4775813527356</v>
+        <v>106.0271915373</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O8" s="1">
-        <v>495.54700073288399</v>
+        <v>495.547000732884</v>
       </c>
       <c r="P8" s="1">
         <v>1486.641002198638</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -898,10 +884,10 @@
         <v>16</v>
       </c>
       <c r="C9" s="4">
-        <v>45675.701388888891</v>
+        <v>45675.70138888889</v>
       </c>
       <c r="D9" s="4">
-        <v>45676.541666666657</v>
+        <v>45676.54166666666</v>
       </c>
       <c r="E9" s="1">
         <v>103240.85</v>
@@ -910,37 +896,37 @@
         <v>102688.8552242209</v>
       </c>
       <c r="G9" s="1">
-        <v>104896.83432733751</v>
+        <v>104896.8343273375</v>
       </c>
       <c r="H9" s="1">
         <v>105157.8</v>
       </c>
-      <c r="I9" s="1">
-        <v>0.19634752047467049</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9">
+        <v>0.1901592627824493</v>
+      </c>
+      <c r="J9" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="1">
-        <v>376.38837937391901</v>
+        <v>314.900758865781</v>
       </c>
       <c r="L9" s="1">
-        <v>11214.66893329475</v>
+        <v>10811.59272105848</v>
       </c>
       <c r="M9" s="1">
-        <v>108.38280553920831</v>
+        <v>104.966919621927</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O9" s="1">
-        <v>551.99477577915241</v>
+        <v>551.9947757791524</v>
       </c>
       <c r="P9" s="1">
         <v>1655.984327337472</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -948,10 +934,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>45677.659722222219</v>
+        <v>45677.65972222222</v>
       </c>
       <c r="D10" s="4">
-        <v>45677.673611111109</v>
+        <v>45677.67361111111</v>
       </c>
       <c r="E10" s="1">
         <v>105535.7</v>
@@ -960,25 +946,25 @@
         <v>104427.1512541753</v>
       </c>
       <c r="G10" s="1">
-        <v>108861.34623747411</v>
+        <v>108861.3462374741</v>
       </c>
       <c r="H10" s="1">
         <v>103708</v>
       </c>
-      <c r="I10" s="1">
-        <v>0.10116532065490461</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10">
+        <v>0.09752924949651455</v>
+      </c>
+      <c r="J10" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="1">
-        <v>-112.1466893329475</v>
+        <v>-108.1159272105848</v>
       </c>
       <c r="L10" s="1">
-        <v>11102.522243961799</v>
+        <v>10703.4767938479</v>
       </c>
       <c r="M10" s="1">
-        <v>112.1466893329475</v>
+        <v>108.1159272105848</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>19</v>
@@ -990,7 +976,7 @@
         <v>3325.64623747408</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -998,10 +984,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="4">
-        <v>45678.628472222219</v>
+        <v>45678.62847222222</v>
       </c>
       <c r="D11" s="4">
-        <v>45678.673611111109</v>
+        <v>45678.67361111111</v>
       </c>
       <c r="E11" s="1">
         <v>103281.22</v>
@@ -1015,32 +1001,32 @@
       <c r="H11" s="1">
         <v>106300</v>
       </c>
-      <c r="I11" s="1">
-        <v>0.1161594969572064</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11">
+        <v>0.1119845070108001</v>
+      </c>
+      <c r="J11" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="1">
-        <v>350.65996622447528</v>
+        <v>321.1043038154369</v>
       </c>
       <c r="L11" s="1">
-        <v>11453.182210186271</v>
+        <v>11024.58109766333</v>
       </c>
       <c r="M11" s="1">
-        <v>111.02522243961801</v>
+        <v>107.034767938479</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O11" s="1">
-        <v>955.79978691299038</v>
+        <v>955.7997869129904</v>
       </c>
       <c r="P11" s="1">
-        <v>2867.3993607389862</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2867.399360738986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1048,16 +1034,16 @@
         <v>16</v>
       </c>
       <c r="C12" s="4">
-        <v>45678.861111111109</v>
+        <v>45678.86111111111</v>
       </c>
       <c r="D12" s="4">
-        <v>45679.541666666657</v>
+        <v>45679.54166666666</v>
       </c>
       <c r="E12" s="1">
         <v>106072</v>
       </c>
       <c r="F12" s="1">
-        <v>105391.07836610261</v>
+        <v>105391.0783661026</v>
       </c>
       <c r="G12" s="1">
         <v>108114.7649016923</v>
@@ -1065,20 +1051,20 @@
       <c r="H12" s="1">
         <v>105039.74</v>
       </c>
-      <c r="I12" s="1">
-        <v>0.16820117969568951</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12">
+        <v>0.1619067532714659</v>
+      </c>
+      <c r="J12" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="1">
-        <v>-114.5318221018627</v>
+        <v>-110.2458109766333</v>
       </c>
       <c r="L12" s="1">
-        <v>11338.65038808441</v>
+        <v>10914.3352866867</v>
       </c>
       <c r="M12" s="1">
-        <v>114.5318221018627</v>
+        <v>110.2458109766333</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>19</v>
@@ -1090,7 +1076,7 @@
         <v>2042.764901692251</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1098,16 +1084,16 @@
         <v>16</v>
       </c>
       <c r="C13" s="4">
-        <v>45679.548611111109</v>
+        <v>45679.54861111111</v>
       </c>
       <c r="D13" s="4">
-        <v>45679.565972222219</v>
+        <v>45679.56597222222</v>
       </c>
       <c r="E13" s="1">
         <v>104947.17</v>
       </c>
       <c r="F13" s="1">
-        <v>104638.47922487849</v>
+        <v>104638.4792248785</v>
       </c>
       <c r="G13" s="1">
         <v>105873.2423253646</v>
@@ -1115,32 +1101,32 @@
       <c r="H13" s="1">
         <v>104283.67</v>
       </c>
-      <c r="I13" s="1">
-        <v>0.36731419601443532</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13">
+        <v>0.3535685600708073</v>
+      </c>
+      <c r="J13" t="s">
         <v>17</v>
       </c>
       <c r="K13" s="1">
-        <v>-113.3865038808441</v>
+        <v>-109.143352866867</v>
       </c>
       <c r="L13" s="1">
-        <v>11225.26388420357</v>
+        <v>10805.19193381983</v>
       </c>
       <c r="M13" s="1">
-        <v>113.3865038808441</v>
+        <v>109.143352866867</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O13" s="1">
-        <v>308.69077512154757</v>
+        <v>308.6907751215476</v>
       </c>
       <c r="P13" s="1">
-        <v>926.07232536464289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>926.0723253646429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1148,16 +1134,16 @@
         <v>16</v>
       </c>
       <c r="C14" s="4">
-        <v>45679.579861111109</v>
+        <v>45679.57986111111</v>
       </c>
       <c r="D14" s="4">
-        <v>45679.694444444453</v>
+        <v>45679.69444444445</v>
       </c>
       <c r="E14" s="1">
         <v>104073.94</v>
       </c>
       <c r="F14" s="1">
-        <v>103607.83220123249</v>
+        <v>103607.8322012325</v>
       </c>
       <c r="G14" s="1">
         <v>105472.2633963026</v>
@@ -1165,32 +1151,32 @@
       <c r="H14" s="1">
         <v>103339.12</v>
       </c>
-      <c r="I14" s="1">
-        <v>0.24082978044746139</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14">
+        <v>0.2318174457151425</v>
+      </c>
+      <c r="J14" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="1">
-        <v>-112.25263884203569</v>
+        <v>-108.0519193381983</v>
       </c>
       <c r="L14" s="1">
-        <v>11113.011245361529</v>
+        <v>10697.14001448163</v>
       </c>
       <c r="M14" s="1">
-        <v>112.25263884203569</v>
+        <v>108.0519193381983</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O14" s="1">
-        <v>466.10779876753799</v>
+        <v>466.107798767538</v>
       </c>
       <c r="P14" s="1">
-        <v>1398.3233963026139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1398.323396302614</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1198,10 +1184,10 @@
         <v>16</v>
       </c>
       <c r="C15" s="4">
-        <v>45679.881944444453</v>
+        <v>45679.88194444445</v>
       </c>
       <c r="D15" s="4">
-        <v>45680.541666666657</v>
+        <v>45680.54166666666</v>
       </c>
       <c r="E15" s="1">
         <v>103891.76</v>
@@ -1215,32 +1201,32 @@
       <c r="H15" s="1">
         <v>101592.48</v>
       </c>
-      <c r="I15" s="1">
-        <v>0.21864682974783711</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="I15">
+        <v>0.2104646256442307</v>
+      </c>
+      <c r="J15" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="1">
-        <v>-111.1301124536153</v>
+        <v>-106.9714001448163</v>
       </c>
       <c r="L15" s="1">
-        <v>11001.88113290792</v>
+        <v>10590.16861433682</v>
       </c>
       <c r="M15" s="1">
-        <v>111.1301124536153</v>
+        <v>106.9714001448163</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O15" s="1">
-        <v>508.26308609999251</v>
+        <v>508.2630860999925</v>
       </c>
       <c r="P15" s="1">
         <v>1524.789258299978</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1248,10 +1234,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>45680.829861111109</v>
+        <v>45680.82986111111</v>
       </c>
       <c r="D16" s="4">
-        <v>45680.850694444453</v>
+        <v>45680.85069444445</v>
       </c>
       <c r="E16" s="1">
         <v>103770.04</v>
@@ -1265,32 +1251,32 @@
       <c r="H16" s="1">
         <v>106421.03</v>
       </c>
-      <c r="I16" s="1">
-        <v>0.12728903413824669</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="I16">
+        <v>0.1225256224817813</v>
+      </c>
+      <c r="J16" t="s">
         <v>18</v>
       </c>
       <c r="K16" s="1">
-        <v>337.44195661015141</v>
+        <v>317.7050584301045</v>
       </c>
       <c r="L16" s="1">
-        <v>11339.32308951807</v>
+        <v>10907.87367276692</v>
       </c>
       <c r="M16" s="1">
-        <v>110.0188113290792</v>
+        <v>105.9016861433682</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O16" s="1">
-        <v>864.32277590848389</v>
+        <v>864.3227759084839</v>
       </c>
       <c r="P16" s="1">
-        <v>2592.9683277254521</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2592.968327725452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1298,10 +1284,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="4">
-        <v>45681.829861111109</v>
+        <v>45681.82986111111</v>
       </c>
       <c r="D17" s="4">
-        <v>45681.847222222219</v>
+        <v>45681.84722222222</v>
       </c>
       <c r="E17" s="1">
         <v>105760.94</v>
@@ -1315,32 +1301,32 @@
       <c r="H17" s="1">
         <v>105291.54</v>
       </c>
-      <c r="I17" s="1">
-        <v>0.24305375705691459</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="I17">
+        <v>0.233805815103632</v>
+      </c>
+      <c r="J17" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="1">
-        <v>-113.39323089518069</v>
+        <v>-109.0787367276692</v>
       </c>
       <c r="L17" s="1">
-        <v>11225.929858622891</v>
+        <v>10798.79493603925</v>
       </c>
       <c r="M17" s="1">
-        <v>113.39323089518069</v>
+        <v>109.0787367276692</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O17" s="1">
-        <v>466.53560211631702</v>
+        <v>466.535602116317</v>
       </c>
       <c r="P17" s="1">
-        <v>1399.6068063489511</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1399.606806348951</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1348,10 +1334,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <v>45681.857638888891</v>
+        <v>45681.85763888889</v>
       </c>
       <c r="D18" s="4">
-        <v>45682.586805555547</v>
+        <v>45682.58680555555</v>
       </c>
       <c r="E18" s="1">
         <v>105052.52</v>
@@ -1360,25 +1346,25 @@
         <v>104590.815085935</v>
       </c>
       <c r="G18" s="1">
-        <v>106437.63474219519</v>
+        <v>106437.6347421952</v>
       </c>
       <c r="H18" s="1">
         <v>104541.68</v>
       </c>
-      <c r="I18" s="1">
-        <v>0.24314079223859611</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18">
+        <v>0.2338895386874273</v>
+      </c>
+      <c r="J18" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="1">
-        <v>-112.25929858622889</v>
+        <v>-107.9879493603925</v>
       </c>
       <c r="L18" s="1">
-        <v>11113.67056003666</v>
+        <v>10690.80698667886</v>
       </c>
       <c r="M18" s="1">
-        <v>112.25929858622889</v>
+        <v>107.9879493603925</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>19</v>
@@ -1387,10 +1373,10 @@
         <v>461.7049140650488</v>
       </c>
       <c r="P18" s="1">
-        <v>1385.1147421951609</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1385.114742195161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1398,7 +1384,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="4">
-        <v>45683.885416666657</v>
+        <v>45683.88541666666</v>
       </c>
       <c r="D19" s="4">
         <v>45683.90625</v>
@@ -1410,37 +1396,37 @@
         <v>104635.5126717815</v>
       </c>
       <c r="G19" s="1">
-        <v>105275.62198465561</v>
+        <v>105275.6219846556</v>
       </c>
       <c r="H19" s="1">
         <v>104552.48</v>
       </c>
-      <c r="I19" s="1">
-        <v>0.69448579088064044</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I19">
+        <v>0.6680613308796381</v>
+      </c>
+      <c r="J19" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="1">
-        <v>-111.1367056003666</v>
+        <v>-106.9080698667886</v>
       </c>
       <c r="L19" s="1">
-        <v>11002.533854436289</v>
+        <v>10583.89891681207</v>
       </c>
       <c r="M19" s="1">
-        <v>111.1367056003666</v>
+        <v>106.9080698667886</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O19" s="1">
-        <v>160.02732821853709</v>
+        <v>160.0273282185371</v>
       </c>
       <c r="P19" s="1">
         <v>480.0819846555969</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1448,10 +1434,10 @@
         <v>15</v>
       </c>
       <c r="C20" s="4">
-        <v>45684.541666666657</v>
+        <v>45684.54166666666</v>
       </c>
       <c r="D20" s="4">
-        <v>45684.545138888891</v>
+        <v>45684.54513888889</v>
       </c>
       <c r="E20" s="1">
         <v>100632.01</v>
@@ -1460,37 +1446,37 @@
         <v>101286.0915115136</v>
       </c>
       <c r="G20" s="1">
-        <v>98669.765465459277</v>
+        <v>98669.76546545928</v>
       </c>
       <c r="H20" s="1">
         <v>101360.94</v>
       </c>
-      <c r="I20" s="1">
-        <v>0.16821349725932291</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="I20">
+        <v>0.1618131491336668</v>
+      </c>
+      <c r="J20" t="s">
         <v>17</v>
       </c>
       <c r="K20" s="1">
-        <v>-110.0253385443629</v>
+        <v>-105.8389891681207</v>
       </c>
       <c r="L20" s="1">
-        <v>10892.50851589193</v>
+        <v>10478.05992764395</v>
       </c>
       <c r="M20" s="1">
-        <v>110.0253385443629</v>
+        <v>105.8389891681207</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O20" s="1">
-        <v>654.08151151357742</v>
+        <v>654.0815115135774</v>
       </c>
       <c r="P20" s="1">
         <v>1962.244534540718</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1498,49 +1484,49 @@
         <v>15</v>
       </c>
       <c r="C21" s="4">
-        <v>45684.850694444453</v>
+        <v>45684.85069444445</v>
       </c>
       <c r="D21" s="4">
-        <v>45684.864583333343</v>
+        <v>45684.86458333334</v>
       </c>
       <c r="E21" s="1">
-        <v>100351.67999999999</v>
+        <v>100351.68</v>
       </c>
       <c r="F21" s="1">
         <v>100958.2739530618</v>
       </c>
       <c r="G21" s="1">
-        <v>98531.898140814548</v>
+        <v>98531.89814081455</v>
       </c>
       <c r="H21" s="1">
         <v>101356.8</v>
       </c>
-      <c r="I21" s="1">
-        <v>0.17956836630024639</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="I21">
+        <v>0.1727359772506024</v>
+      </c>
+      <c r="J21" t="s">
         <v>17</v>
       </c>
       <c r="K21" s="1">
-        <v>-108.9250851589193</v>
+        <v>-104.7805992764395</v>
       </c>
       <c r="L21" s="1">
-        <v>10783.58343073301</v>
+        <v>10373.27932836751</v>
       </c>
       <c r="M21" s="1">
-        <v>108.9250851589193</v>
+        <v>104.7805992764395</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O21" s="1">
-        <v>606.59395306181978</v>
+        <v>606.5939530618198</v>
       </c>
       <c r="P21" s="1">
         <v>1819.781859185445</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1548,10 +1534,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="4">
-        <v>45684.871527777781</v>
+        <v>45684.87152777778</v>
       </c>
       <c r="D22" s="4">
-        <v>45684.878472222219</v>
+        <v>45684.87847222222</v>
       </c>
       <c r="E22" s="1">
         <v>101386.5</v>
@@ -1560,37 +1546,37 @@
         <v>102047.4840323447</v>
       </c>
       <c r="G22" s="1">
-        <v>99403.547902965991</v>
+        <v>99403.54790296599</v>
       </c>
       <c r="H22" s="1">
         <v>102221.99</v>
       </c>
-      <c r="I22" s="1">
-        <v>0.16314438629449249</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="I22">
+        <v>0.1569369125540142</v>
+      </c>
+      <c r="J22" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="1">
-        <v>-107.8358343073301</v>
+        <v>-103.7327932836751</v>
       </c>
       <c r="L22" s="1">
-        <v>10675.747596425679</v>
+        <v>10269.54653508384</v>
       </c>
       <c r="M22" s="1">
-        <v>107.8358343073301</v>
+        <v>103.7327932836751</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O22" s="1">
-        <v>660.98403234466969</v>
+        <v>660.9840323446697</v>
       </c>
       <c r="P22" s="1">
-        <v>1982.9520970340091</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1982.952097034009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1598,7 +1584,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="4">
-        <v>45684.881944444453</v>
+        <v>45684.88194444445</v>
       </c>
       <c r="D23" s="4">
         <v>45685.625</v>
@@ -1615,32 +1601,32 @@
       <c r="H23" s="1">
         <v>103315.79</v>
       </c>
-      <c r="I23" s="1">
-        <v>0.14954214847940031</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="I23">
+        <v>0.143852225700783</v>
+      </c>
+      <c r="J23" t="s">
         <v>17</v>
       </c>
       <c r="K23" s="1">
-        <v>-106.7574759642568</v>
+        <v>-102.6954653508384</v>
       </c>
       <c r="L23" s="1">
-        <v>10568.99012046142</v>
+        <v>10166.851069733</v>
       </c>
       <c r="M23" s="1">
-        <v>106.7574759642568</v>
+        <v>102.6954653508384</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O23" s="1">
-        <v>713.89556088237441</v>
+        <v>713.8955608823744</v>
       </c>
       <c r="P23" s="1">
-        <v>2141.6866826471228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2141.686682647123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1648,16 +1634,16 @@
         <v>16</v>
       </c>
       <c r="C24" s="4">
-        <v>45687.736111111109</v>
+        <v>45687.73611111111</v>
       </c>
       <c r="D24" s="4">
-        <v>45688.565972222219</v>
+        <v>45688.56597222222</v>
       </c>
       <c r="E24" s="1">
         <v>105018.14</v>
       </c>
       <c r="F24" s="1">
-        <v>104555.74558261409</v>
+        <v>104555.7455826141</v>
       </c>
       <c r="G24" s="1">
         <v>106405.3232521578</v>
@@ -1665,32 +1651,32 @@
       <c r="H24" s="1">
         <v>104551.09</v>
       </c>
-      <c r="I24" s="1">
-        <v>0.22857088500790479</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="I24">
+        <v>0.2198740012305906</v>
+      </c>
+      <c r="J24" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="1">
-        <v>-105.6899012046142</v>
+        <v>-101.66851069733</v>
       </c>
       <c r="L24" s="1">
-        <v>10463.300219256809</v>
+        <v>10065.18255903567</v>
       </c>
       <c r="M24" s="1">
-        <v>105.6899012046142</v>
+        <v>101.66851069733</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O24" s="1">
-        <v>462.39441738592001</v>
+        <v>462.39441738592</v>
       </c>
       <c r="P24" s="1">
-        <v>1387.1832521577739</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1387.183252157774</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1698,10 +1684,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="4">
-        <v>45690.590277777781</v>
+        <v>45690.59027777778</v>
       </c>
       <c r="D25" s="4">
-        <v>45690.722222222219</v>
+        <v>45690.72222222222</v>
       </c>
       <c r="E25" s="1">
         <v>99272.12</v>
@@ -1710,37 +1696,37 @@
         <v>99715.13450807023</v>
       </c>
       <c r="G25" s="1">
-        <v>97943.076475789276</v>
+        <v>97943.07647578928</v>
       </c>
       <c r="H25" s="1">
         <v>97727</v>
       </c>
-      <c r="I25" s="1">
-        <v>0.2361841436036666</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="I25">
+        <v>0.2271975832773392</v>
+      </c>
+      <c r="J25" t="s">
         <v>18</v>
       </c>
       <c r="K25" s="1">
-        <v>364.93284396489622</v>
+        <v>301.9554767710701</v>
       </c>
       <c r="L25" s="1">
-        <v>10828.233063221711</v>
+        <v>10367.13803580674</v>
       </c>
       <c r="M25" s="1">
-        <v>104.6330021925681</v>
+        <v>100.6518255903567</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O25" s="1">
-        <v>443.01450807023502</v>
+        <v>443.014508070235</v>
       </c>
       <c r="P25" s="1">
-        <v>1329.0435242107201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1329.04352421072</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1748,49 +1734,49 @@
         <v>15</v>
       </c>
       <c r="C26" s="4">
-        <v>45690.822916666657</v>
+        <v>45690.82291666666</v>
       </c>
       <c r="D26" s="4">
-        <v>45691.541666666657</v>
+        <v>45691.54166666666</v>
       </c>
       <c r="E26" s="1">
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
-        <v>99337.822219288209</v>
+        <v>99337.82221928821</v>
       </c>
       <c r="G26" s="1">
-        <v>96036.733342135369</v>
+        <v>96036.73334213537</v>
       </c>
       <c r="H26" s="1">
-        <v>94564.71</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0.13120801609632521</v>
-      </c>
-      <c r="J26" s="1" t="s">
+        <v>94564.71000000001</v>
+      </c>
+      <c r="I26">
+        <v>0.125620829024735</v>
+      </c>
+      <c r="J26" t="s">
         <v>18</v>
       </c>
       <c r="K26" s="1">
-        <v>517.98825426571614</v>
+        <v>311.0141410742022</v>
       </c>
       <c r="L26" s="1">
-        <v>11346.22131748742</v>
+        <v>10678.15217688094</v>
       </c>
       <c r="M26" s="1">
-        <v>108.2823306322171</v>
+        <v>103.6713803580674</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O26" s="1">
-        <v>825.27221928820654</v>
+        <v>825.2722192882065</v>
       </c>
       <c r="P26" s="1">
-        <v>2475.8166578646342</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2475.816657864634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1798,49 +1784,49 @@
         <v>15</v>
       </c>
       <c r="C27" s="4">
-        <v>45691.611111111109</v>
+        <v>45691.61111111111</v>
       </c>
       <c r="D27" s="4">
-        <v>45691.635416666657</v>
+        <v>45691.63541666666</v>
       </c>
       <c r="E27" s="1">
         <v>96150.84</v>
       </c>
       <c r="F27" s="1">
-        <v>97150.404590042002</v>
+        <v>97150.404590042</v>
       </c>
       <c r="G27" s="1">
-        <v>93152.146229873964</v>
+        <v>93152.14622987396</v>
       </c>
       <c r="H27" s="1">
         <v>97200</v>
       </c>
-      <c r="I27" s="1">
-        <v>0.1135116372720907</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="I27">
+        <v>0.106828035759372</v>
+      </c>
+      <c r="J27" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="1">
-        <v>-113.46221317487419</v>
+        <v>-106.7815217688094</v>
       </c>
       <c r="L27" s="1">
-        <v>11232.75910431255</v>
+        <v>10571.37065511213</v>
       </c>
       <c r="M27" s="1">
-        <v>113.46221317487419</v>
+        <v>106.7815217688094</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O27" s="1">
-        <v>999.56459004200588</v>
+        <v>999.5645900420059</v>
       </c>
       <c r="P27" s="1">
-        <v>2998.6937701260322</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2998.693770126032</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1848,49 +1834,49 @@
         <v>15</v>
       </c>
       <c r="C28" s="4">
-        <v>45691.666666666657</v>
+        <v>45691.66666666666</v>
       </c>
       <c r="D28" s="4">
-        <v>45691.784722222219</v>
+        <v>45691.78472222222</v>
       </c>
       <c r="E28" s="1">
-        <v>98730.93</v>
+        <v>98730.92999999999</v>
       </c>
       <c r="F28" s="1">
-        <v>99908.622508374698</v>
+        <v>99908.6225083747</v>
       </c>
       <c r="G28" s="1">
-        <v>95197.852474875894</v>
+        <v>95197.85247487589</v>
       </c>
       <c r="H28" s="1">
         <v>99943.63</v>
       </c>
-      <c r="I28" s="1">
-        <v>9.5379388290535314E-2</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="I28">
+        <v>0.08976341939800007</v>
+      </c>
+      <c r="J28" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="1">
-        <v>-112.32759104312549</v>
+        <v>-105.7137065511213</v>
       </c>
       <c r="L28" s="1">
-        <v>11120.431513269419</v>
+        <v>10465.65694856101</v>
       </c>
       <c r="M28" s="1">
-        <v>112.32759104312549</v>
+        <v>105.7137065511213</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O28" s="1">
-        <v>1177.6925083747051</v>
+        <v>1177.692508374705</v>
       </c>
       <c r="P28" s="1">
-        <v>3533.0775251240989</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3533.077525124099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1898,49 +1884,49 @@
         <v>15</v>
       </c>
       <c r="C29" s="4">
-        <v>45693.576388888891</v>
+        <v>45693.57638888889</v>
       </c>
       <c r="D29" s="4">
-        <v>45693.611111111109</v>
+        <v>45693.61111111111</v>
       </c>
       <c r="E29" s="1">
-        <v>98581.99</v>
+        <v>98581.99000000001</v>
       </c>
       <c r="F29" s="1">
-        <v>98923.605897969013</v>
+        <v>98923.60589796901</v>
       </c>
       <c r="G29" s="1">
-        <v>97557.142306092981</v>
+        <v>97557.14230609298</v>
       </c>
       <c r="H29" s="1">
         <v>99149</v>
       </c>
-      <c r="I29" s="1">
-        <v>0.32552441439005519</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="I29">
+        <v>0.3063574327419174</v>
+      </c>
+      <c r="J29" t="s">
         <v>17</v>
       </c>
       <c r="K29" s="1">
-        <v>-111.20431513269421</v>
+        <v>-104.6565694856101</v>
       </c>
       <c r="L29" s="1">
-        <v>11009.22719813673</v>
+        <v>10361.0003790754</v>
       </c>
       <c r="M29" s="1">
-        <v>111.20431513269421</v>
+        <v>104.6565694856101</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O29" s="1">
-        <v>341.61589796900807</v>
+        <v>341.6158979690081</v>
       </c>
       <c r="P29" s="1">
         <v>1024.847693907024</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1948,49 +1934,49 @@
         <v>15</v>
       </c>
       <c r="C30" s="4">
-        <v>45694.864583333343</v>
+        <v>45694.86458333334</v>
       </c>
       <c r="D30" s="4">
-        <v>45695.541666666657</v>
+        <v>45695.54166666666</v>
       </c>
       <c r="E30" s="1">
-        <v>96870.9</v>
+        <v>96870.89999999999</v>
       </c>
       <c r="F30" s="1">
-        <v>97360.841236914697</v>
+        <v>97360.8412369147</v>
       </c>
       <c r="G30" s="1">
-        <v>95401.076289255885</v>
+        <v>95401.07628925589</v>
       </c>
       <c r="H30" s="1">
         <v>98007</v>
       </c>
-      <c r="I30" s="1">
-        <v>0.22470505376246569</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="I30">
+        <v>0.2114743483182089</v>
+      </c>
+      <c r="J30" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="1">
-        <v>-110.0922719813673</v>
+        <v>-103.610003790754</v>
       </c>
       <c r="L30" s="1">
-        <v>10899.134926155361</v>
+        <v>10257.39037528465</v>
       </c>
       <c r="M30" s="1">
-        <v>110.0922719813673</v>
+        <v>103.610003790754</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O30" s="1">
-        <v>489.94123691470298</v>
+        <v>489.941236914703</v>
       </c>
       <c r="P30" s="1">
-        <v>1469.8237107441089</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1469.823710744109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1998,37 +1984,37 @@
         <v>15</v>
       </c>
       <c r="C31" s="4">
-        <v>45696.569444444453</v>
+        <v>45696.56944444445</v>
       </c>
       <c r="D31" s="4">
-        <v>45696.645833333343</v>
+        <v>45696.64583333334</v>
       </c>
       <c r="E31" s="1">
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
-        <v>96632.080105326022</v>
+        <v>96632.08010532602</v>
       </c>
       <c r="G31" s="1">
-        <v>95777.079684021941</v>
+        <v>95777.07968402194</v>
       </c>
       <c r="H31" s="1">
         <v>95688</v>
       </c>
-      <c r="I31" s="1">
-        <v>0.5099007979215523</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="I31">
+        <v>0.4798776758327048</v>
+      </c>
+      <c r="J31" t="s">
         <v>18</v>
       </c>
       <c r="K31" s="1">
-        <v>372.39584974604821</v>
+        <v>307.7217112585394</v>
       </c>
       <c r="L31" s="1">
-        <v>11271.53077590141</v>
+        <v>10565.11208654318</v>
       </c>
       <c r="M31" s="1">
-        <v>108.99134926155359</v>
+        <v>102.5739037528465</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>19</v>
@@ -2037,10 +2023,10 @@
         <v>213.7501053260203</v>
       </c>
       <c r="P31" s="1">
-        <v>641.25031597806083</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>641.2503159780608</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2048,49 +2034,49 @@
         <v>15</v>
       </c>
       <c r="C32" s="4">
-        <v>45696.711805555547</v>
+        <v>45696.71180555555</v>
       </c>
       <c r="D32" s="4">
-        <v>45696.777777777781</v>
+        <v>45696.77777777778</v>
       </c>
       <c r="E32" s="1">
-        <v>96282.74</v>
+        <v>96282.74000000001</v>
       </c>
       <c r="F32" s="1">
-        <v>96504.355459768733</v>
+        <v>96504.35545976873</v>
       </c>
       <c r="G32" s="1">
-        <v>95617.893620693823</v>
+        <v>95617.89362069382</v>
       </c>
       <c r="H32" s="1">
         <v>96526.59</v>
       </c>
-      <c r="I32" s="1">
-        <v>0.50860760290207696</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="I32">
+        <v>0.4767317269999434</v>
+      </c>
+      <c r="J32" t="s">
         <v>17</v>
       </c>
       <c r="K32" s="1">
-        <v>-112.7153077590141</v>
+        <v>-105.6511208654318</v>
       </c>
       <c r="L32" s="1">
-        <v>11158.815468142389</v>
+        <v>10459.46096567775</v>
       </c>
       <c r="M32" s="1">
-        <v>112.7153077590141</v>
+        <v>105.6511208654318</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O32" s="1">
-        <v>221.61545976872731</v>
+        <v>221.6154597687273</v>
       </c>
       <c r="P32" s="1">
-        <v>664.84637930618192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>664.8463793061819</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2098,49 +2084,49 @@
         <v>15</v>
       </c>
       <c r="C33" s="4">
-        <v>45696.805555555547</v>
+        <v>45696.80555555555</v>
       </c>
       <c r="D33" s="4">
-        <v>45697.572916666657</v>
+        <v>45697.57291666666</v>
       </c>
       <c r="E33" s="1">
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
-        <v>96814.100350878842</v>
+        <v>96814.10035087884</v>
       </c>
       <c r="G33" s="1">
-        <v>96048.258947363458</v>
+        <v>96048.25894736346</v>
       </c>
       <c r="H33" s="1">
         <v>95915.44</v>
       </c>
-      <c r="I33" s="1">
-        <v>0.58282643988278204</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="I33">
+        <v>0.5462990597095785</v>
+      </c>
+      <c r="J33" t="s">
         <v>18</v>
       </c>
       <c r="K33" s="1">
-        <v>412.17485828510178</v>
+        <v>313.7838289703326</v>
       </c>
       <c r="L33" s="1">
-        <v>11570.990326427491</v>
+        <v>10773.24479464808</v>
       </c>
       <c r="M33" s="1">
-        <v>111.5881546814239</v>
+        <v>104.5946096567775</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O33" s="1">
-        <v>191.46035087884229</v>
+        <v>191.4603508788423</v>
       </c>
       <c r="P33" s="1">
-        <v>574.38105263654143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>574.3810526365414</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2148,49 +2134,49 @@
         <v>15</v>
       </c>
       <c r="C34" s="4">
-        <v>45697.652777777781</v>
+        <v>45697.65277777778</v>
       </c>
       <c r="D34" s="4">
-        <v>45697.899305555547</v>
+        <v>45697.89930555555</v>
       </c>
       <c r="E34" s="1">
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
-        <v>96880.507053391193</v>
+        <v>96880.50705339119</v>
       </c>
       <c r="G34" s="1">
-        <v>95806.678839826433</v>
+        <v>95806.67883982643</v>
       </c>
       <c r="H34" s="1">
-        <v>95376.65</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0.43101830182001161</v>
-      </c>
-      <c r="J34" s="1" t="s">
+        <v>95376.64999999999</v>
+      </c>
+      <c r="I34">
+        <v>0.4013023557607753</v>
+      </c>
+      <c r="J34" t="s">
         <v>18</v>
       </c>
       <c r="K34" s="1">
-        <v>532.48001006844606</v>
+        <v>323.1973438394425</v>
       </c>
       <c r="L34" s="1">
-        <v>12103.470336495941</v>
+        <v>11096.44213848753</v>
       </c>
       <c r="M34" s="1">
-        <v>115.7099032642749</v>
+        <v>107.7324479464808</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O34" s="1">
-        <v>268.45705339119007</v>
+        <v>268.4570533911901</v>
       </c>
       <c r="P34" s="1">
-        <v>805.37116017357039</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <v>805.3711601735704</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2198,16 +2184,16 @@
         <v>15</v>
       </c>
       <c r="C35" s="4">
-        <v>45699.888888888891</v>
+        <v>45699.88888888889</v>
       </c>
       <c r="D35" s="4">
-        <v>45699.899305555547</v>
+        <v>45699.89930555555</v>
       </c>
       <c r="E35" s="1">
         <v>95686.37</v>
       </c>
       <c r="F35" s="1">
-        <v>96056.143740286512</v>
+        <v>96056.14374028651</v>
       </c>
       <c r="G35" s="1">
         <v>94577.04877914043</v>
@@ -2215,32 +2201,32 @@
       <c r="H35" s="1">
         <v>96155.59</v>
       </c>
-      <c r="I35" s="1">
-        <v>0.32732098085487749</v>
-      </c>
-      <c r="J35" s="1" t="s">
+      <c r="I35">
+        <v>0.3000873488174017</v>
+      </c>
+      <c r="J35" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="1">
-        <v>-121.0347033649594</v>
+        <v>-110.9644213848753</v>
       </c>
       <c r="L35" s="1">
-        <v>11982.435633130979</v>
+        <v>10985.47771710265</v>
       </c>
       <c r="M35" s="1">
-        <v>121.0347033649594</v>
+        <v>110.9644213848753</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O35" s="1">
-        <v>369.77374028651678</v>
+        <v>369.7737402865168</v>
       </c>
       <c r="P35" s="1">
-        <v>1109.3212208595651</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1109.321220859565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2257,40 +2243,40 @@
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
-        <v>96720.531834451787</v>
+        <v>96720.53183445179</v>
       </c>
       <c r="G36" s="1">
-        <v>95109.084496644617</v>
+        <v>95109.08449664462</v>
       </c>
       <c r="H36" s="1">
-        <v>94844.800000000003</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0.29743288165871012</v>
-      </c>
-      <c r="J36" s="1" t="s">
+        <v>94844.8</v>
+      </c>
+      <c r="I36">
+        <v>0.2726859875433869</v>
+      </c>
+      <c r="J36" t="s">
         <v>18</v>
       </c>
       <c r="K36" s="1">
-        <v>438.07996840866292</v>
+        <v>329.5643315130796</v>
       </c>
       <c r="L36" s="1">
-        <v>12420.515601539641</v>
+        <v>11315.04204861573</v>
       </c>
       <c r="M36" s="1">
-        <v>119.8243563313098</v>
+        <v>109.8547771710265</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O36" s="1">
-        <v>402.86183445178898</v>
+        <v>402.861834451789</v>
       </c>
       <c r="P36" s="1">
-        <v>1208.5855033553819</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1208.585503355382</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2298,54 +2284,54 @@
         <v>15</v>
       </c>
       <c r="C37" s="4">
-        <v>45701.798611111109</v>
+        <v>45701.79861111111</v>
       </c>
       <c r="D37" s="4">
-        <v>45701.895833333343</v>
+        <v>45701.89583333334</v>
       </c>
       <c r="E37" s="1">
         <v>96270.05</v>
       </c>
       <c r="F37" s="1">
-        <v>96701.702112878746</v>
+        <v>96701.70211287875</v>
       </c>
       <c r="G37" s="1">
         <v>94975.09366136376</v>
       </c>
       <c r="H37" s="1">
-        <v>96774.71</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0.28774365353399178</v>
-      </c>
-      <c r="J37" s="1" t="s">
+        <v>96774.71000000001</v>
+      </c>
+      <c r="I37">
+        <v>0.2621333641379463</v>
+      </c>
+      <c r="J37" t="s">
         <v>17</v>
       </c>
       <c r="K37" s="1">
-        <v>-124.2051560153964</v>
+        <v>-113.1504204861573</v>
       </c>
       <c r="L37" s="1">
-        <v>12296.31044552425</v>
+        <v>11201.89162812958</v>
       </c>
       <c r="M37" s="1">
-        <v>124.2051560153964</v>
+        <v>113.1504204861573</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O37" s="1">
-        <v>431.65211287874263</v>
+        <v>431.6521128787426</v>
       </c>
       <c r="P37" s="1">
         <v>1294.956338636242</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2353,23 +2339,23 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="1">
-        <v>12296.31044552425</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>11201.89162812958</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="5">
-        <v>0.22963104455242481</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.1201891628129574</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -2377,12 +2363,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>25</v>
       </c>
       <c r="B46" s="5">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert back to >3 reward for higher ROR
</commit_message>
<xml_diff>
--- a/trading_results.xlsx
+++ b/trading_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="22">
   <si>
     <t>Position</t>
   </si>
@@ -28,37 +28,28 @@
     <t>Entry Price</t>
   </si>
   <si>
-    <t>Stop Loss</t>
-  </si>
-  <si>
-    <t>Take Profit</t>
-  </si>
-  <si>
     <t>Exit Price</t>
   </si>
   <si>
     <t>Position Size</t>
   </si>
   <si>
-    <t>Outcome</t>
-  </si>
-  <si>
     <t>PnL ($)</t>
   </si>
   <si>
-    <t>Balance After Trade</t>
+    <t>R-Multiple</t>
+  </si>
+  <si>
+    <t>Excess Beyond 3R</t>
+  </si>
+  <si>
+    <t>Price Movement %</t>
   </si>
   <si>
     <t>Risk Amount ($)</t>
   </si>
   <si>
-    <t>Risk-Reward Ratio</t>
-  </si>
-  <si>
-    <t>Price Risk (Points)</t>
-  </si>
-  <si>
-    <t>Potential Reward (Points)</t>
+    <t>Exit Type</t>
   </si>
   <si>
     <t>SHORT</t>
@@ -71,9 +62,6 @@
   </si>
   <si>
     <t>TAKE_PROFIT</t>
-  </si>
-  <si>
-    <t>1:3</t>
   </si>
   <si>
     <t>Summary Statistics</t>
@@ -479,7 +467,7 @@
     <col min="12" max="16" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:13">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,22 +504,13 @@
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4">
         <v>45666.63541666666</v>
@@ -546,42 +525,33 @@
         <v>93801.34997159497</v>
       </c>
       <c r="G2" s="1">
-        <v>91348.75008521508</v>
+        <v>0.1630922362107786</v>
       </c>
       <c r="H2" s="1">
-        <v>93915.89999999999</v>
+        <v>-100</v>
       </c>
       <c r="I2">
-        <v>0.1630922362107786</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>-100</v>
+        <v>-1</v>
       </c>
       <c r="L2" s="1">
-        <v>9900</v>
-      </c>
-      <c r="M2" s="1">
         <v>100</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1">
-        <v>613.1499715949758</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1839.449914784913</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4">
         <v>45666.64930555555</v>
@@ -596,42 +566,33 @@
         <v>94376.30887387348</v>
       </c>
       <c r="G3" s="1">
-        <v>91830.55337837953</v>
+        <v>0.1555530374778455</v>
       </c>
       <c r="H3" s="1">
-        <v>94588.23</v>
+        <v>-99</v>
       </c>
       <c r="I3">
-        <v>0.1555530374778455</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3" s="1">
-        <v>-99</v>
+        <v>-1</v>
       </c>
       <c r="L3" s="1">
-        <v>9801</v>
-      </c>
-      <c r="M3" s="1">
         <v>99</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="1">
-        <v>636.4388738734851</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1909.31662162047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="M3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4">
         <v>45666.66319444445</v>
@@ -643,45 +604,36 @@
         <v>94244.02</v>
       </c>
       <c r="F4" s="1">
-        <v>94919.84370097617</v>
+        <v>92106.85000000001</v>
       </c>
       <c r="G4" s="1">
-        <v>92216.54889707149</v>
+        <v>0.1450230287254407</v>
       </c>
       <c r="H4" s="1">
-        <v>92106.85000000001</v>
+        <v>309.9388663011497</v>
       </c>
       <c r="I4">
-        <v>0.1450230287254407</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
+        <v>3.162318807276296</v>
+      </c>
+      <c r="J4">
+        <v>0.1623188072762956</v>
       </c>
       <c r="K4" s="1">
-        <v>294.03</v>
+        <v>2.267698258202481</v>
       </c>
       <c r="L4" s="1">
-        <v>10095.03</v>
-      </c>
-      <c r="M4" s="1">
         <v>98.01000000000001</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="1">
-        <v>675.8237009761651</v>
-      </c>
-      <c r="P4" s="1">
-        <v>2027.47110292851</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4">
         <v>45667.75</v>
@@ -693,45 +645,36 @@
         <v>95486.73</v>
       </c>
       <c r="F5" s="1">
-        <v>96318.69892474354</v>
+        <v>90583.24000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>92990.82322576936</v>
+        <v>0.1215302466906183</v>
       </c>
       <c r="H5" s="1">
-        <v>90583.24000000001</v>
+        <v>595.9223493449787</v>
       </c>
       <c r="I5">
-        <v>0.1213390272132075</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
+        <v>5.893837923707899</v>
+      </c>
+      <c r="J5">
+        <v>2.893837923707899</v>
       </c>
       <c r="K5" s="1">
-        <v>302.8509</v>
+        <v>5.135258061512831</v>
       </c>
       <c r="L5" s="1">
-        <v>10397.8809</v>
-      </c>
-      <c r="M5" s="1">
-        <v>100.9503</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="1">
-        <v>831.9689247435454</v>
-      </c>
-      <c r="P5" s="1">
-        <v>2495.906774230636</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>101.1093886630115</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>45670.63541666666</v>
@@ -746,42 +689,33 @@
         <v>93739.19579047592</v>
       </c>
       <c r="G6" s="1">
-        <v>89502.45262857222</v>
+        <v>0.1010857708998836</v>
       </c>
       <c r="H6" s="1">
-        <v>93783.12</v>
+        <v>-107.0686121564613</v>
       </c>
       <c r="I6">
-        <v>0.09816862153454611</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6" s="1">
-        <v>-103.978809</v>
+        <v>-1</v>
       </c>
       <c r="L6" s="1">
-        <v>10293.902091</v>
-      </c>
-      <c r="M6" s="1">
-        <v>103.978809</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1059.185790475924</v>
-      </c>
-      <c r="P6" s="1">
-        <v>3177.557371427771</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>107.0686121564613</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4">
         <v>45673.625</v>
@@ -793,45 +727,36 @@
         <v>97571.23</v>
       </c>
       <c r="F7" s="1">
-        <v>96887.64624180444</v>
+        <v>99815.27</v>
       </c>
       <c r="G7" s="1">
-        <v>99621.98127458667</v>
+        <v>0.1550620897060185</v>
       </c>
       <c r="H7" s="1">
-        <v>99815.27</v>
+        <v>347.9655317838951</v>
       </c>
       <c r="I7">
-        <v>0.150587283088361</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
+        <v>3.282757925559201</v>
+      </c>
+      <c r="J7">
+        <v>0.2827579255592014</v>
       </c>
       <c r="K7" s="1">
-        <v>308.81706273</v>
+        <v>2.299899263338187</v>
       </c>
       <c r="L7" s="1">
-        <v>10602.71915373</v>
-      </c>
-      <c r="M7" s="1">
-        <v>102.93902091</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="1">
-        <v>683.5837581955566</v>
-      </c>
-      <c r="P7" s="1">
-        <v>2050.75127458667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>105.9979260348967</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
         <v>45674.87152777778</v>
@@ -846,42 +771,33 @@
         <v>104197.1529992671</v>
       </c>
       <c r="G8" s="1">
-        <v>106179.3410021986</v>
+        <v>0.2209226999473812</v>
       </c>
       <c r="H8" s="1">
-        <v>103424.59</v>
+        <v>-109.4775813527356</v>
       </c>
       <c r="I8">
-        <v>0.2139599097169233</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>-106.0271915373</v>
+        <v>-1</v>
       </c>
       <c r="L8" s="1">
-        <v>10496.6919621927</v>
-      </c>
-      <c r="M8" s="1">
-        <v>106.0271915373</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="1">
-        <v>495.547000732884</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1486.641002198638</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>109.4775813527356</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4">
         <v>45675.70138888889</v>
@@ -893,45 +809,36 @@
         <v>103240.85</v>
       </c>
       <c r="F9" s="1">
-        <v>102688.8552242209</v>
+        <v>105157.8</v>
       </c>
       <c r="G9" s="1">
-        <v>104896.8343273375</v>
+        <v>0.1963475204746705</v>
       </c>
       <c r="H9" s="1">
-        <v>105157.8</v>
+        <v>376.388379373919</v>
       </c>
       <c r="I9">
-        <v>0.1901592627824493</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
+        <v>3.472768374110391</v>
+      </c>
+      <c r="J9">
+        <v>0.472768374110391</v>
       </c>
       <c r="K9" s="1">
-        <v>314.900758865781</v>
+        <v>1.856774716597158</v>
       </c>
       <c r="L9" s="1">
-        <v>10811.59272105848</v>
-      </c>
-      <c r="M9" s="1">
-        <v>104.966919621927</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="1">
-        <v>551.9947757791524</v>
-      </c>
-      <c r="P9" s="1">
-        <v>1655.984327337472</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>108.3828055392083</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" s="4">
         <v>45677.65972222222</v>
@@ -946,42 +853,33 @@
         <v>104427.1512541753</v>
       </c>
       <c r="G10" s="1">
-        <v>108861.3462374741</v>
+        <v>0.1011653206549046</v>
       </c>
       <c r="H10" s="1">
-        <v>103708</v>
+        <v>-112.1466893329475</v>
       </c>
       <c r="I10">
-        <v>0.09752924949651455</v>
-      </c>
-      <c r="J10" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10" s="1">
-        <v>-108.1159272105848</v>
+        <v>-1</v>
       </c>
       <c r="L10" s="1">
-        <v>10703.4767938479</v>
-      </c>
-      <c r="M10" s="1">
-        <v>108.1159272105848</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="1">
-        <v>1108.548745824693</v>
-      </c>
-      <c r="P10" s="1">
-        <v>3325.64623747408</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>112.1466893329475</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4">
         <v>45678.62847222222</v>
@@ -993,45 +891,36 @@
         <v>103281.22</v>
       </c>
       <c r="F11" s="1">
-        <v>102325.420213087</v>
+        <v>106300</v>
       </c>
       <c r="G11" s="1">
-        <v>106148.619360739</v>
+        <v>0.1161594969572064</v>
       </c>
       <c r="H11" s="1">
-        <v>106300</v>
+        <v>350.6599662244753</v>
       </c>
       <c r="I11">
-        <v>0.1119845070108001</v>
-      </c>
-      <c r="J11" t="s">
-        <v>18</v>
+        <v>3.158381118445268</v>
+      </c>
+      <c r="J11">
+        <v>0.1583811184452677</v>
       </c>
       <c r="K11" s="1">
-        <v>321.1043038154369</v>
+        <v>2.922874071394586</v>
       </c>
       <c r="L11" s="1">
-        <v>11024.58109766333</v>
-      </c>
-      <c r="M11" s="1">
-        <v>107.034767938479</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="1">
-        <v>955.7997869129904</v>
-      </c>
-      <c r="P11" s="1">
-        <v>2867.399360738986</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>111.025222439618</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4">
         <v>45678.86111111111</v>
@@ -1046,42 +935,33 @@
         <v>105391.0783661026</v>
       </c>
       <c r="G12" s="1">
-        <v>108114.7649016923</v>
+        <v>0.1682011796956895</v>
       </c>
       <c r="H12" s="1">
-        <v>105039.74</v>
+        <v>-114.5318221018627</v>
       </c>
       <c r="I12">
-        <v>0.1619067532714659</v>
-      </c>
-      <c r="J12" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>-110.2458109766333</v>
+        <v>-1</v>
       </c>
       <c r="L12" s="1">
-        <v>10914.3352866867</v>
-      </c>
-      <c r="M12" s="1">
-        <v>110.2458109766333</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" s="1">
-        <v>680.921633897422</v>
-      </c>
-      <c r="P12" s="1">
-        <v>2042.764901692251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>114.5318221018627</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4">
         <v>45679.54861111111</v>
@@ -1096,42 +976,33 @@
         <v>104638.4792248785</v>
       </c>
       <c r="G13" s="1">
-        <v>105873.2423253646</v>
+        <v>0.3673141960144353</v>
       </c>
       <c r="H13" s="1">
-        <v>104283.67</v>
+        <v>-113.3865038808441</v>
       </c>
       <c r="I13">
-        <v>0.3535685600708073</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>-109.143352866867</v>
+        <v>-1</v>
       </c>
       <c r="L13" s="1">
-        <v>10805.19193381983</v>
-      </c>
-      <c r="M13" s="1">
-        <v>109.143352866867</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="1">
-        <v>308.6907751215476</v>
-      </c>
-      <c r="P13" s="1">
-        <v>926.0723253646429</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>113.3865038808441</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4">
         <v>45679.57986111111</v>
@@ -1146,42 +1017,33 @@
         <v>103607.8322012325</v>
       </c>
       <c r="G14" s="1">
-        <v>105472.2633963026</v>
+        <v>0.2408297804474614</v>
       </c>
       <c r="H14" s="1">
-        <v>103339.12</v>
+        <v>-112.2526388420357</v>
       </c>
       <c r="I14">
-        <v>0.2318174457151425</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
       </c>
       <c r="K14" s="1">
-        <v>-108.0519193381983</v>
+        <v>-1</v>
       </c>
       <c r="L14" s="1">
-        <v>10697.14001448163</v>
-      </c>
-      <c r="M14" s="1">
-        <v>108.0519193381983</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="1">
-        <v>466.107798767538</v>
-      </c>
-      <c r="P14" s="1">
-        <v>1398.323396302614</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>112.2526388420357</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4">
         <v>45679.88194444445</v>
@@ -1196,42 +1058,33 @@
         <v>103383.4969139</v>
       </c>
       <c r="G15" s="1">
-        <v>105416.5492583</v>
+        <v>0.2186468297478371</v>
       </c>
       <c r="H15" s="1">
-        <v>101592.48</v>
+        <v>-111.1301124536153</v>
       </c>
       <c r="I15">
-        <v>0.2104646256442307</v>
-      </c>
-      <c r="J15" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>-106.9714001448163</v>
+        <v>-1</v>
       </c>
       <c r="L15" s="1">
-        <v>10590.16861433682</v>
-      </c>
-      <c r="M15" s="1">
-        <v>106.9714001448163</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="1">
-        <v>508.2630860999925</v>
-      </c>
-      <c r="P15" s="1">
-        <v>1524.789258299978</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>111.1301124536153</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4">
         <v>45680.82986111111</v>
@@ -1243,45 +1096,36 @@
         <v>103770.04</v>
       </c>
       <c r="F16" s="1">
-        <v>102905.7172240915</v>
+        <v>106421.03</v>
       </c>
       <c r="G16" s="1">
-        <v>106363.0083277254</v>
+        <v>0.1272890341382467</v>
       </c>
       <c r="H16" s="1">
-        <v>106421.03</v>
+        <v>337.4419566101514</v>
       </c>
       <c r="I16">
-        <v>0.1225256224817813</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
+        <v>3.06712963477512</v>
+      </c>
+      <c r="J16">
+        <v>0.06712963477511957</v>
       </c>
       <c r="K16" s="1">
-        <v>317.7050584301045</v>
+        <v>2.554677631424259</v>
       </c>
       <c r="L16" s="1">
-        <v>10907.87367276692</v>
-      </c>
-      <c r="M16" s="1">
-        <v>105.9016861433682</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="1">
-        <v>864.3227759084839</v>
-      </c>
-      <c r="P16" s="1">
-        <v>2592.968327725452</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>110.0188113290792</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4">
         <v>45681.82986111111</v>
@@ -1296,42 +1140,33 @@
         <v>105294.4043978837</v>
       </c>
       <c r="G17" s="1">
-        <v>107160.546806349</v>
+        <v>0.2430537570569146</v>
       </c>
       <c r="H17" s="1">
-        <v>105291.54</v>
+        <v>-113.3932308951807</v>
       </c>
       <c r="I17">
-        <v>0.233805815103632</v>
-      </c>
-      <c r="J17" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
       </c>
       <c r="K17" s="1">
-        <v>-109.0787367276692</v>
+        <v>-1</v>
       </c>
       <c r="L17" s="1">
-        <v>10798.79493603925</v>
-      </c>
-      <c r="M17" s="1">
-        <v>109.0787367276692</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="1">
-        <v>466.535602116317</v>
-      </c>
-      <c r="P17" s="1">
-        <v>1399.606806348951</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>113.3932308951807</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="4">
         <v>45681.85763888889</v>
@@ -1346,42 +1181,33 @@
         <v>104590.815085935</v>
       </c>
       <c r="G18" s="1">
-        <v>106437.6347421952</v>
+        <v>0.2431407922385961</v>
       </c>
       <c r="H18" s="1">
-        <v>104541.68</v>
+        <v>-112.2592985862289</v>
       </c>
       <c r="I18">
-        <v>0.2338895386874273</v>
-      </c>
-      <c r="J18" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
       </c>
       <c r="K18" s="1">
-        <v>-107.9879493603925</v>
+        <v>-1</v>
       </c>
       <c r="L18" s="1">
-        <v>10690.80698667886</v>
-      </c>
-      <c r="M18" s="1">
-        <v>107.9879493603925</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="1">
-        <v>461.7049140650488</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1385.114742195161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>112.2592985862289</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="4">
         <v>45683.88541666666</v>
@@ -1396,42 +1222,33 @@
         <v>104635.5126717815</v>
       </c>
       <c r="G19" s="1">
-        <v>105275.6219846556</v>
+        <v>0.6944857908806404</v>
       </c>
       <c r="H19" s="1">
-        <v>104552.48</v>
+        <v>-111.1367056003666</v>
       </c>
       <c r="I19">
-        <v>0.6680613308796381</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>-106.9080698667886</v>
+        <v>-1</v>
       </c>
       <c r="L19" s="1">
-        <v>10583.89891681207</v>
-      </c>
-      <c r="M19" s="1">
-        <v>106.9080698667886</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" s="1">
-        <v>160.0273282185371</v>
-      </c>
-      <c r="P19" s="1">
-        <v>480.0819846555969</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>111.1367056003666</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4">
         <v>45684.54166666666</v>
@@ -1446,42 +1263,33 @@
         <v>101286.0915115136</v>
       </c>
       <c r="G20" s="1">
-        <v>98669.76546545928</v>
+        <v>0.1682134972593229</v>
       </c>
       <c r="H20" s="1">
-        <v>101360.94</v>
+        <v>-110.0253385443629</v>
       </c>
       <c r="I20">
-        <v>0.1618131491336668</v>
-      </c>
-      <c r="J20" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>-105.8389891681207</v>
+        <v>-1</v>
       </c>
       <c r="L20" s="1">
-        <v>10478.05992764395</v>
-      </c>
-      <c r="M20" s="1">
-        <v>105.8389891681207</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20" s="1">
-        <v>654.0815115135774</v>
-      </c>
-      <c r="P20" s="1">
-        <v>1962.244534540718</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>110.0253385443629</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C21" s="4">
         <v>45684.85069444445</v>
@@ -1496,42 +1304,33 @@
         <v>100958.2739530618</v>
       </c>
       <c r="G21" s="1">
-        <v>98531.89814081455</v>
+        <v>0.1795683663002464</v>
       </c>
       <c r="H21" s="1">
-        <v>101356.8</v>
+        <v>-108.9250851589193</v>
       </c>
       <c r="I21">
-        <v>0.1727359772506024</v>
-      </c>
-      <c r="J21" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
       </c>
       <c r="K21" s="1">
-        <v>-104.7805992764395</v>
+        <v>-1</v>
       </c>
       <c r="L21" s="1">
-        <v>10373.27932836751</v>
-      </c>
-      <c r="M21" s="1">
-        <v>104.7805992764395</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O21" s="1">
-        <v>606.5939530618198</v>
-      </c>
-      <c r="P21" s="1">
-        <v>1819.781859185445</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>108.9250851589193</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22" s="4">
         <v>45684.87152777778</v>
@@ -1546,42 +1345,33 @@
         <v>102047.4840323447</v>
       </c>
       <c r="G22" s="1">
-        <v>99403.54790296599</v>
+        <v>0.1631443862944925</v>
       </c>
       <c r="H22" s="1">
-        <v>102221.99</v>
+        <v>-107.8358343073301</v>
       </c>
       <c r="I22">
-        <v>0.1569369125540142</v>
-      </c>
-      <c r="J22" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
       </c>
       <c r="K22" s="1">
-        <v>-103.7327932836751</v>
+        <v>-1</v>
       </c>
       <c r="L22" s="1">
-        <v>10269.54653508384</v>
-      </c>
-      <c r="M22" s="1">
-        <v>103.7327932836751</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22" s="1">
-        <v>660.9840323446697</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1982.952097034009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>107.8358343073301</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4">
         <v>45684.88194444445</v>
@@ -1596,42 +1386,33 @@
         <v>103009.0155608824</v>
       </c>
       <c r="G23" s="1">
-        <v>100153.4333173529</v>
+        <v>0.1495421484794003</v>
       </c>
       <c r="H23" s="1">
-        <v>103315.79</v>
+        <v>-106.7574759642568</v>
       </c>
       <c r="I23">
-        <v>0.143852225700783</v>
-      </c>
-      <c r="J23" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
       </c>
       <c r="K23" s="1">
-        <v>-102.6954653508384</v>
+        <v>-1</v>
       </c>
       <c r="L23" s="1">
-        <v>10166.851069733</v>
-      </c>
-      <c r="M23" s="1">
-        <v>102.6954653508384</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" s="1">
-        <v>713.8955608823744</v>
-      </c>
-      <c r="P23" s="1">
-        <v>2141.686682647123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>106.7574759642568</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4">
         <v>45687.73611111111</v>
@@ -1646,42 +1427,33 @@
         <v>104555.7455826141</v>
       </c>
       <c r="G24" s="1">
-        <v>106405.3232521578</v>
+        <v>0.2285708850079048</v>
       </c>
       <c r="H24" s="1">
-        <v>104551.09</v>
+        <v>-105.6899012046142</v>
       </c>
       <c r="I24">
-        <v>0.2198740012305906</v>
-      </c>
-      <c r="J24" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
       </c>
       <c r="K24" s="1">
-        <v>-101.66851069733</v>
+        <v>-1</v>
       </c>
       <c r="L24" s="1">
-        <v>10065.18255903567</v>
-      </c>
-      <c r="M24" s="1">
-        <v>101.66851069733</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24" s="1">
-        <v>462.39441738592</v>
-      </c>
-      <c r="P24" s="1">
-        <v>1387.183252157774</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>105.6899012046142</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4">
         <v>45690.59027777778</v>
@@ -1693,45 +1465,36 @@
         <v>99272.12</v>
       </c>
       <c r="F25" s="1">
-        <v>99715.13450807023</v>
+        <v>97727</v>
       </c>
       <c r="G25" s="1">
-        <v>97943.07647578928</v>
+        <v>0.2361841436036666</v>
       </c>
       <c r="H25" s="1">
-        <v>97727</v>
+        <v>364.9328439648962</v>
       </c>
       <c r="I25">
-        <v>0.2271975832773392</v>
-      </c>
-      <c r="J25" t="s">
-        <v>18</v>
+        <v>3.487741308361472</v>
+      </c>
+      <c r="J25">
+        <v>0.4877413083614721</v>
       </c>
       <c r="K25" s="1">
-        <v>301.9554767710701</v>
+        <v>1.556449081574963</v>
       </c>
       <c r="L25" s="1">
-        <v>10367.13803580674</v>
-      </c>
-      <c r="M25" s="1">
-        <v>100.6518255903567</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" s="1">
-        <v>443.014508070235</v>
-      </c>
-      <c r="P25" s="1">
-        <v>1329.04352421072</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>104.6330021925681</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4">
         <v>45690.82291666666</v>
@@ -1743,45 +1506,36 @@
         <v>98512.55</v>
       </c>
       <c r="F26" s="1">
-        <v>99337.82221928821</v>
+        <v>94564.71000000001</v>
       </c>
       <c r="G26" s="1">
-        <v>96036.73334213537</v>
+        <v>0.1312080160963252</v>
       </c>
       <c r="H26" s="1">
-        <v>94564.71000000001</v>
+        <v>517.9882542657161</v>
       </c>
       <c r="I26">
-        <v>0.125620829024735</v>
-      </c>
-      <c r="J26" t="s">
-        <v>18</v>
+        <v>4.783682169024168</v>
+      </c>
+      <c r="J26">
+        <v>1.783682169024168</v>
       </c>
       <c r="K26" s="1">
-        <v>311.0141410742022</v>
+        <v>4.00744879713295</v>
       </c>
       <c r="L26" s="1">
-        <v>10678.15217688094</v>
-      </c>
-      <c r="M26" s="1">
-        <v>103.6713803580674</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" s="1">
-        <v>825.2722192882065</v>
-      </c>
-      <c r="P26" s="1">
-        <v>2475.816657864634</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>108.2823306322171</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27" s="4">
         <v>45691.61111111111</v>
@@ -1796,42 +1550,33 @@
         <v>97150.404590042</v>
       </c>
       <c r="G27" s="1">
-        <v>93152.14622987396</v>
+        <v>0.1135116372720907</v>
       </c>
       <c r="H27" s="1">
-        <v>97200</v>
+        <v>-113.4622131748742</v>
       </c>
       <c r="I27">
-        <v>0.106828035759372</v>
-      </c>
-      <c r="J27" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27" s="1">
-        <v>-106.7815217688094</v>
+        <v>-1</v>
       </c>
       <c r="L27" s="1">
-        <v>10571.37065511213</v>
-      </c>
-      <c r="M27" s="1">
-        <v>106.7815217688094</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O27" s="1">
-        <v>999.5645900420059</v>
-      </c>
-      <c r="P27" s="1">
-        <v>2998.693770126032</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>113.4622131748742</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C28" s="4">
         <v>45691.66666666666</v>
@@ -1846,42 +1591,33 @@
         <v>99908.6225083747</v>
       </c>
       <c r="G28" s="1">
-        <v>95197.85247487589</v>
+        <v>0.09537938829053531</v>
       </c>
       <c r="H28" s="1">
-        <v>99943.63</v>
+        <v>-112.3275910431255</v>
       </c>
       <c r="I28">
-        <v>0.08976341939800007</v>
-      </c>
-      <c r="J28" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
       </c>
       <c r="K28" s="1">
-        <v>-105.7137065511213</v>
+        <v>-1</v>
       </c>
       <c r="L28" s="1">
-        <v>10465.65694856101</v>
-      </c>
-      <c r="M28" s="1">
-        <v>105.7137065511213</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O28" s="1">
-        <v>1177.692508374705</v>
-      </c>
-      <c r="P28" s="1">
-        <v>3533.077525124099</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>112.3275910431255</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4">
         <v>45693.57638888889</v>
@@ -1896,42 +1632,33 @@
         <v>98923.60589796901</v>
       </c>
       <c r="G29" s="1">
-        <v>97557.14230609298</v>
+        <v>0.3255244143900552</v>
       </c>
       <c r="H29" s="1">
-        <v>99149</v>
+        <v>-111.2043151326942</v>
       </c>
       <c r="I29">
-        <v>0.3063574327419174</v>
-      </c>
-      <c r="J29" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
       </c>
       <c r="K29" s="1">
-        <v>-104.6565694856101</v>
+        <v>-1</v>
       </c>
       <c r="L29" s="1">
-        <v>10361.0003790754</v>
-      </c>
-      <c r="M29" s="1">
-        <v>104.6565694856101</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O29" s="1">
-        <v>341.6158979690081</v>
-      </c>
-      <c r="P29" s="1">
-        <v>1024.847693907024</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+        <v>111.2043151326942</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C30" s="4">
         <v>45694.86458333334</v>
@@ -1946,42 +1673,33 @@
         <v>97360.8412369147</v>
       </c>
       <c r="G30" s="1">
-        <v>95401.07628925589</v>
+        <v>0.2247050537624657</v>
       </c>
       <c r="H30" s="1">
-        <v>98007</v>
+        <v>-110.0922719813673</v>
       </c>
       <c r="I30">
-        <v>0.2114743483182089</v>
-      </c>
-      <c r="J30" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>-103.610003790754</v>
+        <v>-1</v>
       </c>
       <c r="L30" s="1">
-        <v>10257.39037528465</v>
-      </c>
-      <c r="M30" s="1">
-        <v>103.610003790754</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O30" s="1">
-        <v>489.941236914703</v>
-      </c>
-      <c r="P30" s="1">
-        <v>1469.823710744109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>110.0922719813673</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C31" s="4">
         <v>45696.56944444445</v>
@@ -1993,45 +1711,36 @@
         <v>96418.33</v>
       </c>
       <c r="F31" s="1">
-        <v>96632.08010532602</v>
+        <v>95688</v>
       </c>
       <c r="G31" s="1">
-        <v>95777.07968402194</v>
+        <v>0.5099007979215523</v>
       </c>
       <c r="H31" s="1">
-        <v>95688</v>
+        <v>372.3958497460482</v>
       </c>
       <c r="I31">
-        <v>0.4798776758327048</v>
-      </c>
-      <c r="J31" t="s">
-        <v>18</v>
+        <v>3.416746854398377</v>
+      </c>
+      <c r="J31">
+        <v>0.4167468543983772</v>
       </c>
       <c r="K31" s="1">
-        <v>307.7217112585394</v>
+        <v>0.7574597070909668</v>
       </c>
       <c r="L31" s="1">
-        <v>10565.11208654318</v>
-      </c>
-      <c r="M31" s="1">
-        <v>102.5739037528465</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O31" s="1">
-        <v>213.7501053260203</v>
-      </c>
-      <c r="P31" s="1">
-        <v>641.2503159780608</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+        <v>108.9913492615536</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C32" s="4">
         <v>45696.71180555555</v>
@@ -2046,42 +1755,33 @@
         <v>96504.35545976873</v>
       </c>
       <c r="G32" s="1">
-        <v>95617.89362069382</v>
+        <v>0.508607602902077</v>
       </c>
       <c r="H32" s="1">
-        <v>96526.59</v>
+        <v>-112.7153077590141</v>
       </c>
       <c r="I32">
-        <v>0.4767317269999434</v>
-      </c>
-      <c r="J32" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
       </c>
       <c r="K32" s="1">
-        <v>-105.6511208654318</v>
+        <v>-1</v>
       </c>
       <c r="L32" s="1">
-        <v>10459.46096567775</v>
-      </c>
-      <c r="M32" s="1">
-        <v>105.6511208654318</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O32" s="1">
-        <v>221.6154597687273</v>
-      </c>
-      <c r="P32" s="1">
-        <v>664.8463793061819</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>112.7153077590141</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C33" s="4">
         <v>45696.80555555555</v>
@@ -2093,45 +1793,36 @@
         <v>96622.64</v>
       </c>
       <c r="F33" s="1">
-        <v>96814.10035087884</v>
+        <v>95915.44</v>
       </c>
       <c r="G33" s="1">
-        <v>96048.25894736346</v>
+        <v>0.582826439882782</v>
       </c>
       <c r="H33" s="1">
-        <v>95915.44</v>
+        <v>412.1748582851018</v>
       </c>
       <c r="I33">
-        <v>0.5462990597095785</v>
-      </c>
-      <c r="J33" t="s">
-        <v>18</v>
+        <v>3.69371515697012</v>
+      </c>
+      <c r="J33">
+        <v>0.6937151569701197</v>
       </c>
       <c r="K33" s="1">
-        <v>313.7838289703326</v>
+        <v>0.7319195583974906</v>
       </c>
       <c r="L33" s="1">
-        <v>10773.24479464808</v>
-      </c>
-      <c r="M33" s="1">
-        <v>104.5946096567775</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O33" s="1">
-        <v>191.4603508788423</v>
-      </c>
-      <c r="P33" s="1">
-        <v>574.3810526365414</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+        <v>111.5881546814239</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C34" s="4">
         <v>45697.65277777778</v>
@@ -2143,45 +1834,36 @@
         <v>96612.05</v>
       </c>
       <c r="F34" s="1">
-        <v>96880.50705339119</v>
+        <v>95376.64999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>95806.67883982643</v>
+        <v>0.4310183018200116</v>
       </c>
       <c r="H34" s="1">
-        <v>95376.64999999999</v>
+        <v>532.4800100684461</v>
       </c>
       <c r="I34">
-        <v>0.4013023557607753</v>
-      </c>
-      <c r="J34" t="s">
-        <v>18</v>
+        <v>4.601853385464263</v>
+      </c>
+      <c r="J34">
+        <v>1.601853385464263</v>
       </c>
       <c r="K34" s="1">
-        <v>323.1973438394425</v>
+        <v>1.278722478200192</v>
       </c>
       <c r="L34" s="1">
-        <v>11096.44213848753</v>
-      </c>
-      <c r="M34" s="1">
-        <v>107.7324479464808</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O34" s="1">
-        <v>268.4570533911901</v>
-      </c>
-      <c r="P34" s="1">
-        <v>805.3711601735704</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>115.7099032642749</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C35" s="4">
         <v>45699.88888888889</v>
@@ -2196,42 +1878,33 @@
         <v>96056.14374028651</v>
       </c>
       <c r="G35" s="1">
-        <v>94577.04877914043</v>
+        <v>0.3273209808548775</v>
       </c>
       <c r="H35" s="1">
-        <v>96155.59</v>
+        <v>-121.0347033649594</v>
       </c>
       <c r="I35">
-        <v>0.3000873488174017</v>
-      </c>
-      <c r="J35" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
       </c>
       <c r="K35" s="1">
-        <v>-110.9644213848753</v>
+        <v>-1</v>
       </c>
       <c r="L35" s="1">
-        <v>10985.47771710265</v>
-      </c>
-      <c r="M35" s="1">
-        <v>110.9644213848753</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O35" s="1">
-        <v>369.7737402865168</v>
-      </c>
-      <c r="P35" s="1">
-        <v>1109.321220859565</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+        <v>121.0347033649594</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C36" s="4">
         <v>45699.90625</v>
@@ -2243,45 +1916,36 @@
         <v>96317.67</v>
       </c>
       <c r="F36" s="1">
-        <v>96720.53183445179</v>
+        <v>94844.8</v>
       </c>
       <c r="G36" s="1">
-        <v>95109.08449664462</v>
+        <v>0.2974328816587101</v>
       </c>
       <c r="H36" s="1">
-        <v>94844.8</v>
+        <v>438.0799684086629</v>
       </c>
       <c r="I36">
-        <v>0.2726859875433869</v>
-      </c>
-      <c r="J36" t="s">
-        <v>18</v>
+        <v>3.656017706428469</v>
+      </c>
+      <c r="J36">
+        <v>0.6560177064284689</v>
       </c>
       <c r="K36" s="1">
-        <v>329.5643315130796</v>
+        <v>1.529179433015765</v>
       </c>
       <c r="L36" s="1">
-        <v>11315.04204861573</v>
-      </c>
-      <c r="M36" s="1">
-        <v>109.8547771710265</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36" s="1">
-        <v>402.861834451789</v>
-      </c>
-      <c r="P36" s="1">
-        <v>1208.585503355382</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+        <v>119.8243563313098</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C37" s="4">
         <v>45701.79861111111</v>
@@ -2296,76 +1960,67 @@
         <v>96701.70211287875</v>
       </c>
       <c r="G37" s="1">
-        <v>94975.09366136376</v>
+        <v>0.2877436535339918</v>
       </c>
       <c r="H37" s="1">
-        <v>96774.71000000001</v>
+        <v>-124.2051560153964</v>
       </c>
       <c r="I37">
-        <v>0.2621333641379463</v>
-      </c>
-      <c r="J37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L37" s="1">
+        <v>124.2051560153964</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
         <v>17</v>
-      </c>
-      <c r="K37" s="1">
-        <v>-113.1504204861573</v>
-      </c>
-      <c r="L37" s="1">
-        <v>11201.89162812958</v>
-      </c>
-      <c r="M37" s="1">
-        <v>113.1504204861573</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O37" s="1">
-        <v>431.6521128787426</v>
-      </c>
-      <c r="P37" s="1">
-        <v>1294.956338636242</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="A41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" t="s">
-        <v>21</v>
       </c>
       <c r="B42" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="1">
-        <v>11201.89162812958</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+        <v>12296.31044552425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B44" s="5">
-        <v>0.1201891628129574</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>0.2296310445524248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B45">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B46" s="5">
         <v>0.3333333333333333</v>

</xml_diff>